<commit_message>
Added ticket OmegaT#1766 Customize segment properties fields
</commit_message>
<xml_diff>
--- a/docs/tools/tickets/OmegaT_issues_nopw.xlsx
+++ b/docs/tools/tickets/OmegaT_issues_nopw.xlsx
@@ -13,8 +13,8 @@
     <sheet name="ETS" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A:$F</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A$1:$F$134</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A$1:$F$135</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A:$F</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="true" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="303">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -118,6 +118,18 @@
     <t xml:space="preserve">WIP</t>
   </si>
   <si>
+    <t xml:space="preserve">#1766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customize segment properties fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RFE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open!</t>
+  </si>
+  <si>
     <t xml:space="preserve">#274</t>
   </si>
   <si>
@@ -127,9 +139,6 @@
     <t xml:space="preserve">Translated and final segments in XLIFF 2.0</t>
   </si>
   <si>
-    <t xml:space="preserve">Open!</t>
-  </si>
-  <si>
     <t xml:space="preserve">#273</t>
   </si>
   <si>
@@ -146,9 +155,6 @@
   </si>
   <si>
     <t xml:space="preserve">Let user decide the maximum number of TM matches displayed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RFE</t>
   </si>
   <si>
     <t xml:space="preserve">#1752</t>
@@ -1704,14 +1710,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ136"/>
+  <dimension ref="A1:AMJ137"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1762,21 +1768,21 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="n">
-        <v>45563</v>
+        <v>45604</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>9</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>33</v>
@@ -1788,16 +1794,16 @@
     </row>
     <row r="4" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="n">
-        <v>45488</v>
+        <v>45563</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>9</v>
@@ -1810,18 +1816,18 @@
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" s="8" customFormat="true" ht="11.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="n">
+    <row r="5" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="n">
         <v>45488</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>9</v>
@@ -1834,21 +1840,21 @@
       <c r="AMI5" s="0"/>
       <c r="AMJ5" s="0"/>
     </row>
-    <row r="6" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="8" customFormat="true" ht="11.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>33</v>
@@ -1860,7 +1866,7 @@
     </row>
     <row r="7" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="n">
-        <v>45469</v>
+        <v>45483</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>41</v>
@@ -1872,10 +1878,10 @@
         <v>42</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="AMG7" s="0"/>
       <c r="AMH7" s="0"/>
@@ -1884,22 +1890,22 @@
     </row>
     <row r="8" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="n">
-        <v>45784</v>
+        <v>45469</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="13" t="s">
+      <c r="E8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="AMG8" s="0"/>
       <c r="AMH8" s="0"/>
@@ -1908,7 +1914,7 @@
     </row>
     <row r="9" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="n">
-        <v>45411</v>
+        <v>45784</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>46</v>
@@ -1920,7 +1926,7 @@
         <v>47</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>33</v>
@@ -1930,9 +1936,9 @@
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="n">
-        <v>45394</v>
+        <v>45411</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>48</v>
@@ -1944,10 +1950,10 @@
         <v>49</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>43</v>
+        <v>32</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="AMG10" s="0"/>
       <c r="AMH10" s="0"/>
@@ -1955,23 +1961,23 @@
       <c r="AMJ10" s="0"/>
     </row>
     <row r="11" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="n">
-        <v>45390</v>
+      <c r="A11" s="12" t="n">
+        <v>45394</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>50</v>
       </c>
       <c r="C11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>51</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>52</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="14" t="s">
-        <v>53</v>
+      <c r="F11" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="AMG11" s="0"/>
       <c r="AMH11" s="0"/>
@@ -1980,22 +1986,22 @@
     </row>
     <row r="12" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="n">
-        <v>45365</v>
+        <v>45390</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>56</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>43</v>
+      <c r="F12" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="AMG12" s="0"/>
       <c r="AMH12" s="0"/>
@@ -2004,58 +2010,58 @@
     </row>
     <row r="13" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="n">
-        <v>45363</v>
+        <v>45365</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="13" t="s">
         <v>58</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AMG13" s="0"/>
       <c r="AMH13" s="0"/>
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
+    <row r="14" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9" t="n">
+        <v>45363</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>29</v>
+      <c r="C14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="AMG14" s="0"/>
       <c r="AMH14" s="0"/>
       <c r="AMI14" s="0"/>
       <c r="AMJ14" s="0"/>
     </row>
-    <row r="15" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="n">
-        <v>45238</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="13" t="s">
+    <row r="15" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>33</v>
+      <c r="F15" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="AMG15" s="0"/>
       <c r="AMH15" s="0"/>
@@ -2064,7 +2070,7 @@
     </row>
     <row r="16" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="n">
-        <v>45230</v>
+        <v>45238</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>62</v>
@@ -2072,11 +2078,11 @@
       <c r="C16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="13" t="s">
         <v>63</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>33</v>
@@ -2088,7 +2094,7 @@
     </row>
     <row r="17" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="n">
-        <v>45223</v>
+        <v>45230</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>64</v>
@@ -2100,10 +2106,10 @@
         <v>65</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>43</v>
+        <v>32</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="AMG17" s="0"/>
       <c r="AMH17" s="0"/>
@@ -2112,7 +2118,7 @@
     </row>
     <row r="18" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="n">
-        <v>45236</v>
+        <v>45223</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>66</v>
@@ -2124,10 +2130,10 @@
         <v>67</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>68</v>
+        <v>32</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="AMG18" s="0"/>
       <c r="AMH18" s="0"/>
@@ -2136,22 +2142,22 @@
     </row>
     <row r="19" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="n">
-        <v>45233</v>
+        <v>45236</v>
       </c>
       <c r="B19" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>69</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>70</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="14" t="s">
-        <v>33</v>
+      <c r="F19" s="15" t="s">
+        <v>70</v>
       </c>
       <c r="AMG19" s="0"/>
       <c r="AMH19" s="0"/>
@@ -2160,7 +2166,7 @@
     </row>
     <row r="20" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="n">
-        <v>45213</v>
+        <v>45233</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>71</v>
@@ -2172,10 +2178,10 @@
         <v>72</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>43</v>
+        <v>9</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="AMG20" s="0"/>
       <c r="AMH20" s="0"/>
@@ -2184,22 +2190,22 @@
     </row>
     <row r="21" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="n">
-        <v>45199</v>
+        <v>45213</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>73</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>74</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AMG21" s="0"/>
       <c r="AMH21" s="0"/>
@@ -2208,22 +2214,22 @@
     </row>
     <row r="22" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="n">
-        <v>45170</v>
+        <v>45199</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>75</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>76</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AMG22" s="0"/>
       <c r="AMH22" s="0"/>
@@ -2232,7 +2238,7 @@
     </row>
     <row r="23" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="n">
-        <v>45169</v>
+        <v>45170</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>77</v>
@@ -2244,10 +2250,10 @@
         <v>78</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AMG23" s="0"/>
       <c r="AMH23" s="0"/>
@@ -2255,23 +2261,23 @@
       <c r="AMJ23" s="0"/>
     </row>
     <row r="24" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="16" t="n">
+      <c r="A24" s="9" t="n">
         <v>45169</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C24" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="18" t="s">
+      <c r="C24" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>80</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="AMG24" s="0"/>
       <c r="AMH24" s="0"/>
@@ -2280,7 +2286,7 @@
     </row>
     <row r="25" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="n">
-        <v>45145</v>
+        <v>45169</v>
       </c>
       <c r="B25" s="17" t="s">
         <v>81</v>
@@ -2289,7 +2295,7 @@
         <v>7</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>9</v>
@@ -2303,23 +2309,23 @@
       <c r="AMJ25" s="0"/>
     </row>
     <row r="26" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="n">
+      <c r="A26" s="16" t="n">
         <v>45145</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="11" t="s">
+      <c r="C26" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="18" t="s">
         <v>84</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>53</v>
       </c>
       <c r="AMG26" s="0"/>
       <c r="AMH26" s="0"/>
@@ -2343,37 +2349,40 @@
         <v>9</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AMG27" s="0"/>
       <c r="AMH27" s="0"/>
       <c r="AMI27" s="0"/>
       <c r="AMJ27" s="0"/>
     </row>
-    <row r="28" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="n">
-        <v>45112</v>
+        <v>45145</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>87</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>53</v>
+        <v>88</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="AMG28" s="0"/>
       <c r="AMH28" s="0"/>
       <c r="AMI28" s="0"/>
       <c r="AMJ28" s="0"/>
     </row>
-    <row r="29" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="n">
-        <v>45124</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>88</v>
+        <v>45112</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>7</v>
@@ -2381,11 +2390,8 @@
       <c r="D29" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E29" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>33</v>
+      <c r="F29" s="20" t="s">
+        <v>55</v>
       </c>
       <c r="AMG29" s="0"/>
       <c r="AMH29" s="0"/>
@@ -2394,19 +2400,19 @@
     </row>
     <row r="30" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="n">
-        <v>45119</v>
+        <v>45124</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C30" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D30" s="11" t="s">
-        <v>92</v>
-      </c>
       <c r="E30" s="11" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F30" s="14" t="s">
         <v>33</v>
@@ -2421,16 +2427,16 @@
         <v>45119</v>
       </c>
       <c r="B31" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>93</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>91</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>94</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F31" s="14" t="s">
         <v>33</v>
@@ -2442,19 +2448,19 @@
     </row>
     <row r="32" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="n">
-        <v>45118</v>
+        <v>45119</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>95</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="D32" s="11" t="s">
         <v>96</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F32" s="14" t="s">
         <v>33</v>
@@ -2490,7 +2496,7 @@
     </row>
     <row r="34" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="n">
-        <v>45110</v>
+        <v>45118</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>99</v>
@@ -2502,10 +2508,10 @@
         <v>100</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>43</v>
+        <v>9</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="AMG34" s="0"/>
       <c r="AMH34" s="0"/>
@@ -2514,7 +2520,7 @@
     </row>
     <row r="35" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="n">
-        <v>45104</v>
+        <v>45110</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>101</v>
@@ -2526,49 +2532,49 @@
         <v>102</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="21" t="s">
-        <v>103</v>
+        <v>32</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="AMG35" s="0"/>
       <c r="AMH35" s="0"/>
       <c r="AMI35" s="0"/>
       <c r="AMJ35" s="0"/>
     </row>
-    <row r="36" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="n">
-        <v>45094</v>
+        <v>45104</v>
       </c>
       <c r="B36" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="11" t="s">
         <v>104</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>106</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="20" t="s">
-        <v>53</v>
+      <c r="F36" s="21" t="s">
+        <v>105</v>
       </c>
       <c r="AMG36" s="0"/>
       <c r="AMH36" s="0"/>
       <c r="AMI36" s="0"/>
       <c r="AMJ36" s="0"/>
     </row>
-    <row r="37" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="n">
-        <v>45069</v>
+        <v>45094</v>
       </c>
       <c r="B37" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>107</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>13</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>108</v>
@@ -2576,41 +2582,41 @@
       <c r="E37" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="22" t="s">
-        <v>109</v>
+      <c r="F37" s="20" t="s">
+        <v>55</v>
       </c>
       <c r="AMG37" s="0"/>
       <c r="AMH37" s="0"/>
       <c r="AMI37" s="0"/>
       <c r="AMJ37" s="0"/>
     </row>
-    <row r="38" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="n">
         <v>45069</v>
       </c>
       <c r="B38" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="E38" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F38" s="20" t="s">
-        <v>53</v>
+      <c r="F38" s="22" t="s">
+        <v>111</v>
       </c>
       <c r="AMG38" s="0"/>
       <c r="AMH38" s="0"/>
       <c r="AMI38" s="0"/>
       <c r="AMJ38" s="0"/>
     </row>
-    <row r="39" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="n">
-        <v>45064</v>
+        <v>45069</v>
       </c>
       <c r="B39" s="10" t="s">
         <v>112</v>
@@ -2624,17 +2630,17 @@
       <c r="E39" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F39" s="11" t="s">
-        <v>43</v>
+      <c r="F39" s="20" t="s">
+        <v>55</v>
       </c>
       <c r="AMG39" s="0"/>
       <c r="AMH39" s="0"/>
       <c r="AMI39" s="0"/>
       <c r="AMJ39" s="0"/>
     </row>
-    <row r="40" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="n">
-        <v>45049</v>
+        <v>45064</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>114</v>
@@ -2648,8 +2654,8 @@
       <c r="E40" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F40" s="23" t="s">
-        <v>53</v>
+      <c r="F40" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="AMG40" s="0"/>
       <c r="AMH40" s="0"/>
@@ -2663,17 +2669,17 @@
       <c r="B41" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C41" s="24" t="s">
-        <v>105</v>
+      <c r="C41" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>117</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>53</v>
+        <v>9</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>55</v>
       </c>
       <c r="AMG41" s="0"/>
       <c r="AMH41" s="0"/>
@@ -2682,31 +2688,31 @@
     </row>
     <row r="42" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="n">
-        <v>45044</v>
+        <v>45049</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="11" t="s">
-        <v>7</v>
+      <c r="C42" s="24" t="s">
+        <v>107</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>119</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AMG42" s="0"/>
       <c r="AMH42" s="0"/>
       <c r="AMI42" s="0"/>
       <c r="AMJ42" s="0"/>
     </row>
-    <row r="43" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="n">
-        <v>45040</v>
+        <v>45044</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>120</v>
@@ -2720,17 +2726,17 @@
       <c r="E43" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="11" t="s">
-        <v>43</v>
+      <c r="F43" s="20" t="s">
+        <v>55</v>
       </c>
       <c r="AMG43" s="0"/>
       <c r="AMH43" s="0"/>
       <c r="AMI43" s="0"/>
       <c r="AMJ43" s="0"/>
     </row>
-    <row r="44" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="n">
-        <v>45028</v>
+        <v>45040</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>122</v>
@@ -2742,10 +2748,10 @@
         <v>123</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F44" s="20" t="s">
-        <v>53</v>
+        <v>9</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="AMG44" s="0"/>
       <c r="AMH44" s="0"/>
@@ -2754,16 +2760,22 @@
     </row>
     <row r="45" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="n">
-        <v>44996</v>
+        <v>45028</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>124</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AMG45" s="0"/>
       <c r="AMH45" s="0"/>
@@ -2772,31 +2784,25 @@
     </row>
     <row r="46" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="n">
-        <v>45007</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>125</v>
+        <v>44996</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="E46" s="11" t="s">
-        <v>9</v>
-      </c>
       <c r="F46" s="20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AMG46" s="0"/>
       <c r="AMH46" s="0"/>
       <c r="AMI46" s="0"/>
       <c r="AMJ46" s="0"/>
     </row>
-    <row r="47" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="n">
-        <v>44993</v>
+        <v>45007</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>127</v>
@@ -2810,8 +2816,8 @@
       <c r="E47" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F47" s="21" t="s">
-        <v>103</v>
+      <c r="F47" s="20" t="s">
+        <v>55</v>
       </c>
       <c r="AMG47" s="0"/>
       <c r="AMH47" s="0"/>
@@ -2835,7 +2841,7 @@
         <v>9</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AMG48" s="0"/>
       <c r="AMH48" s="0"/>
@@ -2844,22 +2850,22 @@
     </row>
     <row r="49" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="n">
-        <v>44991</v>
+        <v>44993</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>97</v>
+        <v>131</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E49" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F49" s="11" t="s">
-        <v>132</v>
+      <c r="F49" s="21" t="s">
+        <v>105</v>
       </c>
       <c r="AMG49" s="0"/>
       <c r="AMH49" s="0"/>
@@ -2868,22 +2874,22 @@
     </row>
     <row r="50" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="n">
-        <v>44981</v>
+        <v>44991</v>
       </c>
       <c r="B50" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="C50" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" s="11" t="s">
+      <c r="E50" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="11" t="s">
         <v>134</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="AMG50" s="0"/>
       <c r="AMH50" s="0"/>
@@ -2892,22 +2898,22 @@
     </row>
     <row r="51" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="n">
-        <v>44973</v>
+        <v>44981</v>
       </c>
       <c r="B51" s="10" t="s">
         <v>135</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D51" s="11" t="s">
         <v>136</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="AMG51" s="0"/>
       <c r="AMH51" s="0"/>
@@ -2915,47 +2921,47 @@
       <c r="AMJ51" s="0"/>
     </row>
     <row r="52" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="16" t="n">
-        <v>44972</v>
-      </c>
-      <c r="B52" s="17" t="s">
+      <c r="A52" s="9" t="n">
+        <v>44973</v>
+      </c>
+      <c r="B52" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="C52" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="E52" s="18" t="s">
+      <c r="C52" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E52" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F52" s="18" t="s">
-        <v>80</v>
+      <c r="F52" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="AMG52" s="0"/>
       <c r="AMH52" s="0"/>
       <c r="AMI52" s="0"/>
       <c r="AMJ52" s="0"/>
     </row>
-    <row r="53" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="26" t="n">
-        <v>44970</v>
-      </c>
-      <c r="B53" s="27" t="s">
+    <row r="53" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="16" t="n">
+        <v>44972</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="C53" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D53" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="E53" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F53" s="24" t="s">
-        <v>43</v>
+      <c r="E53" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="18" t="s">
+        <v>82</v>
       </c>
       <c r="AMG53" s="0"/>
       <c r="AMH53" s="0"/>
@@ -2964,22 +2970,22 @@
     </row>
     <row r="54" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="26" t="n">
-        <v>44967</v>
+        <v>44970</v>
       </c>
       <c r="B54" s="27" t="s">
         <v>140</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>7</v>
+        <v>107</v>
       </c>
       <c r="D54" s="24" t="s">
         <v>141</v>
       </c>
       <c r="E54" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F54" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F54" s="24" t="s">
+        <v>45</v>
       </c>
       <c r="AMG54" s="0"/>
       <c r="AMH54" s="0"/>
@@ -2988,7 +2994,7 @@
     </row>
     <row r="55" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="26" t="n">
-        <v>44964</v>
+        <v>44967</v>
       </c>
       <c r="B55" s="27" t="s">
         <v>142</v>
@@ -3000,10 +3006,10 @@
         <v>143</v>
       </c>
       <c r="E55" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F55" s="21" t="s">
-        <v>103</v>
+        <v>32</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="AMG55" s="0"/>
       <c r="AMH55" s="0"/>
@@ -3012,7 +3018,7 @@
     </row>
     <row r="56" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="26" t="n">
-        <v>44952</v>
+        <v>44964</v>
       </c>
       <c r="B56" s="27" t="s">
         <v>144</v>
@@ -3024,10 +3030,10 @@
         <v>145</v>
       </c>
       <c r="E56" s="24" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F56" s="21" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AMG56" s="0"/>
       <c r="AMH56" s="0"/>
@@ -3048,10 +3054,10 @@
         <v>147</v>
       </c>
       <c r="E57" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F57" s="20" t="s">
-        <v>53</v>
+        <v>32</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>105</v>
       </c>
       <c r="AMG57" s="0"/>
       <c r="AMH57" s="0"/>
@@ -3059,23 +3065,23 @@
       <c r="AMJ57" s="0"/>
     </row>
     <row r="58" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="28" t="n">
-        <v>44949</v>
-      </c>
-      <c r="B58" s="29" t="s">
+      <c r="A58" s="26" t="n">
+        <v>44952</v>
+      </c>
+      <c r="B58" s="27" t="s">
         <v>148</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D58" s="24" t="s">
         <v>149</v>
       </c>
       <c r="E58" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F58" s="20" t="s">
+        <v>55</v>
       </c>
       <c r="AMG58" s="0"/>
       <c r="AMH58" s="0"/>
@@ -3083,23 +3089,23 @@
       <c r="AMJ58" s="0"/>
     </row>
     <row r="59" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="26" t="n">
-        <v>44948</v>
-      </c>
-      <c r="B59" s="27" t="s">
+      <c r="A59" s="28" t="n">
+        <v>44949</v>
+      </c>
+      <c r="B59" s="29" t="s">
         <v>150</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D59" s="24" t="s">
         <v>151</v>
       </c>
       <c r="E59" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F59" s="20" t="s">
-        <v>53</v>
+        <v>9</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="AMG59" s="0"/>
       <c r="AMH59" s="0"/>
@@ -3108,58 +3114,70 @@
     </row>
     <row r="60" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="26" t="n">
-        <v>44946</v>
+        <v>44948</v>
       </c>
       <c r="B60" s="27" t="s">
         <v>152</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="D60" s="24" t="s">
         <v>153</v>
       </c>
       <c r="E60" s="24" t="s">
-        <v>154</v>
+        <v>32</v>
       </c>
       <c r="F60" s="20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AMG60" s="0"/>
       <c r="AMH60" s="0"/>
       <c r="AMI60" s="0"/>
       <c r="AMJ60" s="0"/>
     </row>
-    <row r="61" s="24" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="26" t="n">
-        <v>44929</v>
-      </c>
-      <c r="B61" s="30" t="s">
+        <v>44946</v>
+      </c>
+      <c r="B61" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="C61" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D61" s="24" t="s">
+      <c r="E61" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="E61" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="F61" s="14" t="s">
-        <v>33</v>
+      <c r="F61" s="20" t="s">
+        <v>55</v>
       </c>
       <c r="AMG61" s="0"/>
       <c r="AMH61" s="0"/>
       <c r="AMI61" s="0"/>
       <c r="AMJ61" s="0"/>
     </row>
-    <row r="62" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="8" t="s">
+    <row r="62" s="24" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="26" t="n">
+        <v>44929</v>
+      </c>
+      <c r="B62" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="F62" s="8" t="s">
-        <v>29</v>
+      <c r="C62" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="E62" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="AMG62" s="0"/>
       <c r="AMH62" s="0"/>
@@ -3167,71 +3185,59 @@
       <c r="AMJ62" s="0"/>
     </row>
     <row r="63" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="26" t="n">
-        <v>44879</v>
-      </c>
-      <c r="B63" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D63" s="5" t="s">
+      <c r="A63" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="E63" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>43</v>
+      <c r="F63" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="AMG63" s="0"/>
       <c r="AMH63" s="0"/>
       <c r="AMI63" s="0"/>
       <c r="AMJ63" s="0"/>
     </row>
-    <row r="64" s="24" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="26" t="n">
-        <v>44858</v>
-      </c>
-      <c r="B64" s="27" t="s">
+        <v>44879</v>
+      </c>
+      <c r="B64" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="C64" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D64" s="24" t="s">
+      <c r="C64" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="E64" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F64" s="24" t="s">
-        <v>43</v>
+      <c r="E64" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="AMG64" s="0"/>
       <c r="AMH64" s="0"/>
       <c r="AMI64" s="0"/>
       <c r="AMJ64" s="0"/>
     </row>
-    <row r="65" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" s="24" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="26" t="n">
-        <v>44855</v>
-      </c>
-      <c r="B65" s="31" t="s">
+        <v>44858</v>
+      </c>
+      <c r="B65" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="C65" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D65" s="5" t="s">
+      <c r="C65" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="E65" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F65" s="21" t="s">
-        <v>103</v>
+      <c r="E65" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F65" s="24" t="s">
+        <v>45</v>
       </c>
       <c r="AMG65" s="0"/>
       <c r="AMH65" s="0"/>
@@ -3240,7 +3246,7 @@
     </row>
     <row r="66" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="26" t="n">
-        <v>44844</v>
+        <v>44855</v>
       </c>
       <c r="B66" s="31" t="s">
         <v>164</v>
@@ -3252,105 +3258,109 @@
         <v>165</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>166</v>
+        <v>156</v>
+      </c>
+      <c r="F66" s="21" t="s">
+        <v>105</v>
       </c>
       <c r="AMG66" s="0"/>
       <c r="AMH66" s="0"/>
       <c r="AMI66" s="0"/>
       <c r="AMJ66" s="0"/>
     </row>
-    <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="26" t="n">
-        <v>44757</v>
-      </c>
-      <c r="B67" s="32" t="s">
+        <v>44844</v>
+      </c>
+      <c r="B67" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D67" s="5" t="s">
+      <c r="E67" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F67" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="E67" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F67" s="20" t="s">
-        <v>53</v>
-      </c>
+      <c r="AMG67" s="0"/>
+      <c r="AMH67" s="0"/>
+      <c r="AMI67" s="0"/>
+      <c r="AMJ67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="26" t="n">
-        <v>373466</v>
-      </c>
-      <c r="B68" s="31" t="s">
+        <v>44757</v>
+      </c>
+      <c r="B68" s="32" t="s">
         <v>169</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>170</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>43</v>
+        <v>156</v>
+      </c>
+      <c r="F68" s="20" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="26" t="n">
-        <v>44743</v>
+        <v>373466</v>
+      </c>
+      <c r="B69" s="31" t="s">
+        <v>171</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="F69" s="20" t="s">
-        <v>53</v>
+        <v>172</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="26" t="n">
-        <v>44740</v>
-      </c>
-      <c r="B70" s="33" t="s">
-        <v>172</v>
+        <v>44743</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="E70" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F70" s="14" t="s">
-        <v>33</v>
+      <c r="F70" s="20" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="26" t="n">
-        <v>44739</v>
-      </c>
-      <c r="B71" s="34" t="s">
+        <v>44740</v>
+      </c>
+      <c r="B71" s="33" t="s">
         <v>174</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>175</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>23</v>
+        <v>156</v>
       </c>
       <c r="F71" s="14" t="s">
         <v>33</v>
@@ -3358,7 +3368,7 @@
     </row>
     <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="26" t="n">
-        <v>44693</v>
+        <v>44739</v>
       </c>
       <c r="B72" s="34" t="s">
         <v>176</v>
@@ -3370,7 +3380,7 @@
         <v>177</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="F72" s="14" t="s">
         <v>33</v>
@@ -3378,69 +3388,69 @@
     </row>
     <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="26" t="n">
-        <v>44695</v>
-      </c>
-      <c r="B73" s="35" t="s">
+        <v>44693</v>
+      </c>
+      <c r="B73" s="34" t="s">
         <v>178</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>179</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F73" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F73" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="26" t="n">
+        <v>44695</v>
+      </c>
+      <c r="B74" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="C74" s="5" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="28" t="n">
-        <v>44659</v>
-      </c>
-      <c r="B74" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>181</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F74" s="14" t="s">
-        <v>33</v>
+        <v>156</v>
+      </c>
+      <c r="F74" s="20" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="26" t="n">
-        <v>44712</v>
-      </c>
-      <c r="B75" s="34" t="s">
+      <c r="A75" s="28" t="n">
+        <v>44659</v>
+      </c>
+      <c r="B75" s="36" t="s">
         <v>182</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>109</v>
+        <v>156</v>
+      </c>
+      <c r="F75" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="26" t="n">
-        <v>44705</v>
-      </c>
-      <c r="B76" s="31" t="s">
+        <v>44712</v>
+      </c>
+      <c r="B76" s="34" t="s">
         <v>184</v>
       </c>
       <c r="C76" s="5" t="s">
@@ -3450,10 +3460,10 @@
         <v>185</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F76" s="20" t="s">
-        <v>53</v>
+        <v>32</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3470,15 +3480,15 @@
         <v>187</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F77" s="20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="26" t="n">
-        <v>44693</v>
+        <v>44705</v>
       </c>
       <c r="B78" s="31" t="s">
         <v>188</v>
@@ -3490,15 +3500,15 @@
         <v>189</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>43</v>
+        <v>156</v>
+      </c>
+      <c r="F78" s="20" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="26" t="n">
-        <v>44622</v>
+        <v>44693</v>
       </c>
       <c r="B79" s="31" t="s">
         <v>190</v>
@@ -3510,57 +3520,57 @@
         <v>191</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F79" s="20" t="s">
-        <v>53</v>
+        <v>32</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="26" t="n">
-        <v>44614</v>
+        <v>44622</v>
       </c>
       <c r="B80" s="31" t="s">
         <v>192</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>193</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F80" s="14" t="s">
-        <v>33</v>
+        <v>156</v>
+      </c>
+      <c r="F80" s="20" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="26" t="n">
-        <v>44613</v>
+        <v>44614</v>
       </c>
       <c r="B81" s="31" t="s">
         <v>194</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>195</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>43</v>
+        <v>156</v>
+      </c>
+      <c r="F81" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="26" t="n">
-        <v>44608</v>
-      </c>
-      <c r="B82" s="34" t="s">
+        <v>44613</v>
+      </c>
+      <c r="B82" s="31" t="s">
         <v>196</v>
       </c>
       <c r="C82" s="5" t="s">
@@ -3570,60 +3580,60 @@
         <v>197</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F82" s="20" t="s">
-        <v>53</v>
+        <v>156</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="26" t="n">
-        <v>44580</v>
-      </c>
-      <c r="B83" s="31" t="s">
+        <v>44608</v>
+      </c>
+      <c r="B83" s="34" t="s">
         <v>198</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>199</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F83" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="26" t="n">
+        <v>44580</v>
+      </c>
+      <c r="B84" s="31" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="26" t="n">
-        <v>44463</v>
-      </c>
-      <c r="B85" s="31" t="s">
+      <c r="C84" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D84" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C85" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D85" s="5" t="s">
+      <c r="E84" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="26" t="n">
-        <v>44460</v>
+        <v>44463</v>
       </c>
       <c r="B86" s="31" t="s">
         <v>203</v>
@@ -3635,10 +3645,10 @@
         <v>204</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>40</v>
+        <v>156</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>205</v>
+        <v>45</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3646,24 +3656,24 @@
         <v>44460</v>
       </c>
       <c r="B87" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C87" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D87" s="5" t="s">
+      <c r="E87" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F87" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F87" s="20" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="26" t="n">
-        <v>44372</v>
+        <v>44460</v>
       </c>
       <c r="B88" s="31" t="s">
         <v>208</v>
@@ -3677,73 +3687,73 @@
       <c r="E88" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F88" s="5" t="s">
-        <v>43</v>
+      <c r="F88" s="20" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="26" t="n">
-        <v>44326</v>
+        <v>44372</v>
       </c>
       <c r="B89" s="31" t="s">
         <v>210</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>211</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>154</v>
+        <v>23</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>166</v>
+        <v>45</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="28" t="n">
-        <v>44325</v>
-      </c>
-      <c r="B90" s="37" t="s">
+      <c r="A90" s="26" t="n">
+        <v>44326</v>
+      </c>
+      <c r="B90" s="31" t="s">
         <v>212</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>213</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F90" s="14" t="s">
-        <v>33</v>
+        <v>156</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="26" t="n">
+      <c r="A91" s="28" t="n">
         <v>44325</v>
       </c>
-      <c r="B91" s="31" t="s">
+      <c r="B91" s="37" t="s">
         <v>214</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>215</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>43</v>
+        <v>156</v>
+      </c>
+      <c r="F91" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="26" t="n">
-        <v>44321</v>
+        <v>44325</v>
       </c>
       <c r="B92" s="31" t="s">
         <v>216</v>
@@ -3755,15 +3765,15 @@
         <v>217</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F92" s="21" t="s">
-        <v>103</v>
+        <v>23</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="26" t="n">
-        <v>44316</v>
+        <v>44321</v>
       </c>
       <c r="B93" s="31" t="s">
         <v>218</v>
@@ -3775,37 +3785,37 @@
         <v>219</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F93" s="5" t="s">
-        <v>220</v>
+        <v>32</v>
+      </c>
+      <c r="F93" s="21" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="26" t="n">
-        <v>44279</v>
-      </c>
-      <c r="B94" s="5" t="s">
+        <v>44316</v>
+      </c>
+      <c r="B94" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="C94" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D94" s="5" t="s">
+      <c r="E94" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F94" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F94" s="14" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="26" t="n">
-        <v>44257</v>
-      </c>
-      <c r="B95" s="31" t="s">
+        <v>44279</v>
+      </c>
+      <c r="B95" s="5" t="s">
         <v>223</v>
       </c>
       <c r="C95" s="5" t="s">
@@ -3815,15 +3825,15 @@
         <v>224</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F95" s="5" t="s">
-        <v>43</v>
+        <v>23</v>
+      </c>
+      <c r="F95" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="26" t="n">
-        <v>44243</v>
+        <v>44257</v>
       </c>
       <c r="B96" s="31" t="s">
         <v>225</v>
@@ -3835,57 +3845,57 @@
         <v>226</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="38" t="n">
+      <c r="A97" s="26" t="n">
+        <v>44243</v>
+      </c>
+      <c r="B97" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="38" t="n">
         <v>44231</v>
       </c>
-      <c r="B97" s="39" t="s">
-        <v>227</v>
-      </c>
-      <c r="C97" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D97" s="40" t="s">
-        <v>173</v>
-      </c>
-      <c r="E97" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="F97" s="40" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="26" t="n">
-        <v>44218</v>
-      </c>
-      <c r="B98" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D98" s="5" t="s">
+      <c r="B98" s="39" t="s">
         <v>229</v>
       </c>
-      <c r="E98" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F98" s="5" t="s">
-        <v>43</v>
+      <c r="C98" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D98" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="E98" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="F98" s="40" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="26" t="n">
-        <v>44216</v>
-      </c>
-      <c r="B99" s="34" t="s">
+        <v>44218</v>
+      </c>
+      <c r="B99" s="31" t="s">
         <v>230</v>
       </c>
       <c r="C99" s="5" t="s">
@@ -3895,17 +3905,17 @@
         <v>231</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F99" s="14" t="s">
-        <v>33</v>
+        <v>156</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="26" t="n">
-        <v>44175</v>
-      </c>
-      <c r="B100" s="31" t="s">
+        <v>44216</v>
+      </c>
+      <c r="B100" s="34" t="s">
         <v>232</v>
       </c>
       <c r="C100" s="5" t="s">
@@ -3915,10 +3925,10 @@
         <v>233</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F100" s="5" t="s">
-        <v>43</v>
+        <v>23</v>
+      </c>
+      <c r="F100" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3935,40 +3945,40 @@
         <v>235</v>
       </c>
       <c r="E101" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="26" t="n">
+        <v>44175</v>
+      </c>
+      <c r="B102" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E102" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F101" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="26" t="n">
-        <v>44162</v>
-      </c>
-      <c r="B103" s="31" t="s">
-        <v>236</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="E103" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F103" s="5" t="s">
-        <v>43</v>
+      <c r="F102" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="26" t="n">
-        <v>44148</v>
+        <v>44162</v>
       </c>
       <c r="B104" s="31" t="s">
         <v>238</v>
@@ -3977,158 +3987,158 @@
         <v>7</v>
       </c>
       <c r="D104" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="26" t="n">
+        <v>44148</v>
+      </c>
+      <c r="B105" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D105" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E104" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F104" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="38" t="n">
+      <c r="E105" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="38" t="n">
         <v>44146</v>
       </c>
-      <c r="B105" s="39" t="s">
-        <v>239</v>
-      </c>
-      <c r="C105" s="40" t="s">
+      <c r="B106" s="39" t="s">
+        <v>241</v>
+      </c>
+      <c r="C106" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D105" s="40" t="s">
-        <v>240</v>
-      </c>
-      <c r="E105" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="F105" s="40" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="26" t="n">
-        <v>44132</v>
-      </c>
-      <c r="B106" s="31" t="s">
-        <v>227</v>
-      </c>
-      <c r="C106" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D106" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="E106" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F106" s="5" t="s">
-        <v>43</v>
+      <c r="D106" s="40" t="s">
+        <v>242</v>
+      </c>
+      <c r="E106" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="F106" s="40" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="26" t="n">
-        <v>44103</v>
+        <v>44132</v>
       </c>
       <c r="B107" s="31" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>243</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="38" t="n">
+      <c r="A108" s="26" t="n">
+        <v>44103</v>
+      </c>
+      <c r="B108" s="31" t="s">
+        <v>244</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="38" t="n">
         <v>44095</v>
       </c>
-      <c r="B108" s="39" t="s">
-        <v>244</v>
-      </c>
-      <c r="C108" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D108" s="40" t="s">
-        <v>245</v>
-      </c>
-      <c r="E108" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="F108" s="40" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="26" t="n">
-        <v>44095</v>
-      </c>
-      <c r="B109" s="31" t="s">
+      <c r="B109" s="39" t="s">
         <v>246</v>
       </c>
-      <c r="C109" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D109" s="5" t="s">
+      <c r="C109" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D109" s="40" t="s">
         <v>247</v>
       </c>
-      <c r="E109" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F109" s="20" t="s">
-        <v>53</v>
+      <c r="E109" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F109" s="40" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="26" t="n">
-        <v>44057</v>
+        <v>44095</v>
       </c>
       <c r="B110" s="31" t="s">
         <v>248</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>249</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F110" s="5" t="s">
-        <v>205</v>
+        <v>32</v>
+      </c>
+      <c r="F110" s="20" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="26" t="n">
-        <v>44028</v>
+        <v>44057</v>
       </c>
       <c r="B111" s="31" t="s">
         <v>250</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>251</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F111" s="20" t="s">
-        <v>53</v>
+        <v>32</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="26" t="n">
-        <v>44064</v>
+        <v>44028</v>
       </c>
       <c r="B112" s="31" t="s">
         <v>252</v>
@@ -4140,15 +4150,15 @@
         <v>253</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F112" s="5" t="s">
-        <v>43</v>
+        <v>156</v>
+      </c>
+      <c r="F112" s="20" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="26" t="n">
-        <v>44028</v>
+        <v>44064</v>
       </c>
       <c r="B113" s="31" t="s">
         <v>254</v>
@@ -4160,15 +4170,15 @@
         <v>255</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F113" s="20" t="s">
-        <v>53</v>
+        <v>156</v>
+      </c>
+      <c r="F113" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="26" t="n">
-        <v>44016</v>
+        <v>44028</v>
       </c>
       <c r="B114" s="31" t="s">
         <v>256</v>
@@ -4180,15 +4190,15 @@
         <v>257</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F114" s="5" t="s">
-        <v>43</v>
+        <v>156</v>
+      </c>
+      <c r="F114" s="20" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="26" t="n">
-        <v>44010</v>
+        <v>44016</v>
       </c>
       <c r="B115" s="31" t="s">
         <v>258</v>
@@ -4200,35 +4210,35 @@
         <v>259</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="26" t="n">
-        <v>43995</v>
+        <v>44010</v>
       </c>
       <c r="B116" s="31" t="s">
         <v>260</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>261</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="26" t="n">
-        <v>43948</v>
+        <v>43995</v>
       </c>
       <c r="B117" s="31" t="s">
         <v>262</v>
@@ -4240,15 +4250,15 @@
         <v>263</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F117" s="20" t="s">
-        <v>53</v>
+        <v>32</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="26" t="n">
-        <v>43947</v>
+        <v>43948</v>
       </c>
       <c r="B118" s="31" t="s">
         <v>264</v>
@@ -4260,15 +4270,15 @@
         <v>265</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F118" s="14" t="s">
-        <v>33</v>
+        <v>156</v>
+      </c>
+      <c r="F118" s="20" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="26" t="n">
-        <v>43936</v>
+        <v>43947</v>
       </c>
       <c r="B119" s="31" t="s">
         <v>266</v>
@@ -4280,35 +4290,35 @@
         <v>267</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F119" s="5" t="s">
-        <v>43</v>
+        <v>156</v>
+      </c>
+      <c r="F119" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="26" t="n">
-        <v>43929</v>
+        <v>43936</v>
       </c>
       <c r="B120" s="31" t="s">
         <v>268</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>269</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>154</v>
+        <v>32</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="26" t="n">
-        <v>43891</v>
+        <v>43929</v>
       </c>
       <c r="B121" s="31" t="s">
         <v>270</v>
@@ -4320,15 +4330,15 @@
         <v>271</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F121" s="20" t="s">
-        <v>53</v>
+        <v>156</v>
+      </c>
+      <c r="F121" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="26" t="n">
-        <v>43885</v>
+        <v>43891</v>
       </c>
       <c r="B122" s="31" t="s">
         <v>272</v>
@@ -4340,15 +4350,15 @@
         <v>273</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F122" s="5" t="s">
-        <v>43</v>
+        <v>156</v>
+      </c>
+      <c r="F122" s="20" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="26" t="n">
-        <v>43857</v>
+        <v>43885</v>
       </c>
       <c r="B123" s="31" t="s">
         <v>274</v>
@@ -4360,10 +4370,10 @@
         <v>275</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4380,15 +4390,15 @@
         <v>277</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F124" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="26" t="n">
-        <v>43852</v>
+        <v>43857</v>
       </c>
       <c r="B125" s="31" t="s">
         <v>278</v>
@@ -4400,15 +4410,15 @@
         <v>279</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F125" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="26" t="n">
-        <v>43584</v>
+        <v>43852</v>
       </c>
       <c r="B126" s="31" t="s">
         <v>280</v>
@@ -4420,10 +4430,10 @@
         <v>281</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>23</v>
+        <v>156</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4443,14 +4453,14 @@
         <v>23</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="26" t="n">
-        <v>43540</v>
-      </c>
-      <c r="B128" s="5" t="s">
+        <v>43584</v>
+      </c>
+      <c r="B128" s="31" t="s">
         <v>284</v>
       </c>
       <c r="C128" s="5" t="s">
@@ -4463,32 +4473,32 @@
         <v>23</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="26" t="n">
-        <v>43203</v>
-      </c>
-      <c r="B130" s="41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="26" t="n">
+        <v>43540</v>
+      </c>
+      <c r="B129" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="C130" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D130" s="5" t="s">
+      <c r="C129" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D129" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="E130" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F130" s="14" t="s">
-        <v>33</v>
+      <c r="E129" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F129" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4499,61 +4509,61 @@
         <v>288</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D131" s="5" t="s">
         <v>289</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F131" s="5" t="s">
-        <v>290</v>
+        <v>156</v>
+      </c>
+      <c r="F131" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="26" t="n">
-        <v>42842</v>
+        <v>43203</v>
       </c>
       <c r="B132" s="41" t="s">
+        <v>290</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D132" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="C132" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D132" s="5" t="s">
+      <c r="E132" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F132" s="5" t="s">
         <v>292</v>
-      </c>
-      <c r="E132" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F132" s="14" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="26" t="n">
-        <v>42457</v>
-      </c>
-      <c r="B133" s="5" t="s">
+        <v>42842</v>
+      </c>
+      <c r="B133" s="41" t="s">
         <v>293</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="D133" s="5" t="s">
         <v>294</v>
       </c>
       <c r="E133" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F133" s="5" t="s">
-        <v>43</v>
+        <v>32</v>
+      </c>
+      <c r="F133" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="26" t="n">
-        <v>39028</v>
+        <v>42457</v>
       </c>
       <c r="B134" s="5" t="s">
         <v>295</v>
@@ -4565,21 +4575,41 @@
         <v>296</v>
       </c>
       <c r="E134" s="5" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="F134" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="136" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AMG136" s="0"/>
-      <c r="AMH136" s="0"/>
-      <c r="AMI136" s="0"/>
-      <c r="AMJ136" s="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="26" t="n">
+        <v>39028</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C135" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="E135" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F135" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="137" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMG137" s="0"/>
+      <c r="AMH137" s="0"/>
+      <c r="AMI137" s="0"/>
+      <c r="AMJ137" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A:F"/>
-  <conditionalFormatting sqref="F85:F1048576 F1:F83">
+  <autoFilter ref="A1:F135"/>
+  <conditionalFormatting sqref="F86:F1048576 F1:F84">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="resolved" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("resolved",F1)))</formula>
     </cfRule>
@@ -4588,130 +4618,131 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="#274"/>
-    <hyperlink ref="B4" r:id="rId2" display="#273"/>
-    <hyperlink ref="B5" r:id="rId3" display="#272"/>
-    <hyperlink ref="B6" r:id="rId4" display="#1754"/>
-    <hyperlink ref="B7" r:id="rId5" display="#1752"/>
-    <hyperlink ref="B8" r:id="rId6" display="#1745"/>
-    <hyperlink ref="B9" r:id="rId7" display="#1743"/>
-    <hyperlink ref="B10" r:id="rId8" display="#1258"/>
-    <hyperlink ref="B11" r:id="rId9" display="#271"/>
-    <hyperlink ref="B12" r:id="rId10" display="#2"/>
-    <hyperlink ref="B13" r:id="rId11" display="#1349"/>
-    <hyperlink ref="B15" r:id="rId12" display="#1725"/>
-    <hyperlink ref="B16" r:id="rId13" display="#1724"/>
-    <hyperlink ref="B17" r:id="rId14" display="#1722"/>
-    <hyperlink ref="B18" r:id="rId15" display="#1226"/>
-    <hyperlink ref="B19" r:id="rId16" display="#1225"/>
-    <hyperlink ref="B20" r:id="rId17" display="#1720"/>
-    <hyperlink ref="B21" r:id="rId18" display="#1323"/>
-    <hyperlink ref="B22" r:id="rId19" display="#30"/>
-    <hyperlink ref="B23" r:id="rId20" display="#1712"/>
-    <hyperlink ref="B24" r:id="rId21" display="#1215"/>
-    <hyperlink ref="B25" r:id="rId22" display="#1214"/>
-    <hyperlink ref="B26" r:id="rId23" display="#1213"/>
-    <hyperlink ref="B27" r:id="rId24" display="#1212"/>
-    <hyperlink ref="B29" r:id="rId25" display="#1202"/>
-    <hyperlink ref="B30" r:id="rId26" display="#27"/>
-    <hyperlink ref="B31" r:id="rId27" display="#26"/>
-    <hyperlink ref="B32" r:id="rId28" display="#1201"/>
-    <hyperlink ref="B33" r:id="rId29" display="#1200"/>
-    <hyperlink ref="B34" r:id="rId30" display="#1708"/>
-    <hyperlink ref="B35" r:id="rId31" display="#1185"/>
-    <hyperlink ref="B36" r:id="rId32" display="#11"/>
-    <hyperlink ref="B37" r:id="rId33" display="#1309"/>
-    <hyperlink ref="B38" r:id="rId34" display="#1176"/>
-    <hyperlink ref="B39" r:id="rId35" display="#1171"/>
-    <hyperlink ref="B40" r:id="rId36" display="#1164"/>
-    <hyperlink ref="B41" r:id="rId37" display="#9"/>
-    <hyperlink ref="B42" r:id="rId38" display="#1163"/>
-    <hyperlink ref="B43" r:id="rId39" display="#1161"/>
-    <hyperlink ref="B44" r:id="rId40" display="#1690"/>
-    <hyperlink ref="B46" r:id="rId41" display="#1155"/>
-    <hyperlink ref="B47" r:id="rId42" display="#1150"/>
-    <hyperlink ref="B48" r:id="rId43" display="#1151"/>
-    <hyperlink ref="B49" r:id="rId44" display="#1200"/>
-    <hyperlink ref="B50" r:id="rId45" display="#1681"/>
-    <hyperlink ref="B51" r:id="rId46" display="#51"/>
-    <hyperlink ref="B52" r:id="rId47" display="#1142"/>
-    <hyperlink ref="B53" r:id="rId48" display="#8"/>
-    <hyperlink ref="B54" r:id="rId49" display="#1674"/>
-    <hyperlink ref="B55" r:id="rId50" display="#1672"/>
-    <hyperlink ref="B56" r:id="rId51" display="#1669"/>
-    <hyperlink ref="B57" r:id="rId52" display="#1670"/>
-    <hyperlink ref="B58" r:id="rId53" display="#1184"/>
-    <hyperlink ref="B59" r:id="rId54" display="#49"/>
-    <hyperlink ref="B60" r:id="rId55" display="#1140"/>
-    <hyperlink ref="B61" r:id="rId56" display="#1132"/>
-    <hyperlink ref="B63" r:id="rId57" display="#1125"/>
-    <hyperlink ref="B64" r:id="rId58" display="#1641"/>
-    <hyperlink ref="B65" r:id="rId59" display="#1124"/>
-    <hyperlink ref="B66" r:id="rId60" display="#1122"/>
-    <hyperlink ref="B67" r:id="rId61" display="#43"/>
-    <hyperlink ref="B68" r:id="rId62" display="#1622"/>
-    <hyperlink ref="B70" r:id="rId63" display="#38"/>
-    <hyperlink ref="B71" r:id="rId64" display="#1621"/>
-    <hyperlink ref="B72" r:id="rId65" display="#1616"/>
-    <hyperlink ref="B73" r:id="rId66" display="#37"/>
-    <hyperlink ref="B74" r:id="rId67" display="#36"/>
-    <hyperlink ref="B75" r:id="rId68" display="#1101"/>
-    <hyperlink ref="B76" r:id="rId69" display="#1099"/>
-    <hyperlink ref="B77" r:id="rId70" display="#1098"/>
-    <hyperlink ref="B78" r:id="rId71" display="#1617"/>
-    <hyperlink ref="B79" r:id="rId72" display="#1092"/>
-    <hyperlink ref="B80" r:id="rId73" display="#1128"/>
-    <hyperlink ref="B81" r:id="rId74" display="#1090"/>
-    <hyperlink ref="B82" r:id="rId75" display="#1608"/>
-    <hyperlink ref="B83" r:id="rId76" display="#35"/>
-    <hyperlink ref="B85" r:id="rId77" display="#1070"/>
-    <hyperlink ref="B86" r:id="rId78" display="#1592"/>
-    <hyperlink ref="B87" r:id="rId79" display="#1591"/>
-    <hyperlink ref="B88" r:id="rId80" display="#1578"/>
-    <hyperlink ref="B89" r:id="rId81" display="#41"/>
-    <hyperlink ref="B90" r:id="rId82" display="#42"/>
-    <hyperlink ref="B91" r:id="rId83" display="#1566"/>
-    <hyperlink ref="B92" r:id="rId84" display="#1565"/>
-    <hyperlink ref="B93" r:id="rId85" display="#1046"/>
-    <hyperlink ref="B94" r:id="rId86" display="#1559"/>
-    <hyperlink ref="B95" r:id="rId87" display="#1038"/>
-    <hyperlink ref="B96" r:id="rId88" display="#1037"/>
-    <hyperlink ref="B97" r:id="rId89" display="#1020"/>
-    <hyperlink ref="B98" r:id="rId90" display="#1032"/>
-    <hyperlink ref="B99" r:id="rId91" display="#1546"/>
-    <hyperlink ref="B100" r:id="rId92" display="#1027"/>
-    <hyperlink ref="B101" r:id="rId93" display="#1529"/>
-    <hyperlink ref="B103" r:id="rId94" display="#1527"/>
-    <hyperlink ref="B104" r:id="rId95" display="#558"/>
-    <hyperlink ref="B105" r:id="rId96" display="#1005"/>
-    <hyperlink ref="B106" r:id="rId97" display="#1020"/>
-    <hyperlink ref="B107" r:id="rId98" display="#993"/>
-    <hyperlink ref="B108" r:id="rId99" display="#1520"/>
-    <hyperlink ref="B109" r:id="rId100" display="#1519"/>
-    <hyperlink ref="B110" r:id="rId101" display="#969"/>
-    <hyperlink ref="B111" r:id="rId102" display="#1003"/>
-    <hyperlink ref="B112" r:id="rId103" display="#1015"/>
-    <hyperlink ref="B113" r:id="rId104" display="#1002"/>
-    <hyperlink ref="B114" r:id="rId105" display="#1471"/>
-    <hyperlink ref="B115" r:id="rId106" display="#1497"/>
-    <hyperlink ref="B116" r:id="rId107" display="#947"/>
-    <hyperlink ref="B117" r:id="rId108" display="#933"/>
-    <hyperlink ref="B118" r:id="rId109" display="#932"/>
-    <hyperlink ref="B119" r:id="rId110" display="#931"/>
-    <hyperlink ref="B120" r:id="rId111" display="#987"/>
-    <hyperlink ref="B121" r:id="rId112" display="#988"/>
-    <hyperlink ref="B122" r:id="rId113" display="#982"/>
-    <hyperlink ref="B123" r:id="rId114" display="#979"/>
-    <hyperlink ref="B124" r:id="rId115" display="#977"/>
-    <hyperlink ref="B125" r:id="rId116" display="#975"/>
-    <hyperlink ref="B126" r:id="rId117" display="#1445"/>
-    <hyperlink ref="B127" r:id="rId118" display="#1444"/>
-    <hyperlink ref="B128" r:id="rId119" display="#1427"/>
-    <hyperlink ref="B130" r:id="rId120" display="#23"/>
-    <hyperlink ref="B131" r:id="rId121" display="#22"/>
-    <hyperlink ref="B132" r:id="rId122" display="#18"/>
-    <hyperlink ref="B133" r:id="rId123" display="#1207"/>
-    <hyperlink ref="B134" r:id="rId124" display="#245"/>
+    <hyperlink ref="B3" r:id="rId1" display="#1766"/>
+    <hyperlink ref="B4" r:id="rId2" display="#274"/>
+    <hyperlink ref="B5" r:id="rId3" display="#273"/>
+    <hyperlink ref="B6" r:id="rId4" display="#272"/>
+    <hyperlink ref="B7" r:id="rId5" display="#1754"/>
+    <hyperlink ref="B8" r:id="rId6" display="#1752"/>
+    <hyperlink ref="B9" r:id="rId7" display="#1745"/>
+    <hyperlink ref="B10" r:id="rId8" display="#1743"/>
+    <hyperlink ref="B11" r:id="rId9" display="#1258"/>
+    <hyperlink ref="B12" r:id="rId10" display="#271"/>
+    <hyperlink ref="B13" r:id="rId11" display="#2"/>
+    <hyperlink ref="B14" r:id="rId12" display="#1349"/>
+    <hyperlink ref="B16" r:id="rId13" display="#1725"/>
+    <hyperlink ref="B17" r:id="rId14" display="#1724"/>
+    <hyperlink ref="B18" r:id="rId15" display="#1722"/>
+    <hyperlink ref="B19" r:id="rId16" display="#1226"/>
+    <hyperlink ref="B20" r:id="rId17" display="#1225"/>
+    <hyperlink ref="B21" r:id="rId18" display="#1720"/>
+    <hyperlink ref="B22" r:id="rId19" display="#1323"/>
+    <hyperlink ref="B23" r:id="rId20" display="#30"/>
+    <hyperlink ref="B24" r:id="rId21" display="#1712"/>
+    <hyperlink ref="B25" r:id="rId22" display="#1215"/>
+    <hyperlink ref="B26" r:id="rId23" display="#1214"/>
+    <hyperlink ref="B27" r:id="rId24" display="#1213"/>
+    <hyperlink ref="B28" r:id="rId25" display="#1212"/>
+    <hyperlink ref="B30" r:id="rId26" display="#1202"/>
+    <hyperlink ref="B31" r:id="rId27" display="#27"/>
+    <hyperlink ref="B32" r:id="rId28" display="#26"/>
+    <hyperlink ref="B33" r:id="rId29" display="#1201"/>
+    <hyperlink ref="B34" r:id="rId30" display="#1200"/>
+    <hyperlink ref="B35" r:id="rId31" display="#1708"/>
+    <hyperlink ref="B36" r:id="rId32" display="#1185"/>
+    <hyperlink ref="B37" r:id="rId33" display="#11"/>
+    <hyperlink ref="B38" r:id="rId34" display="#1309"/>
+    <hyperlink ref="B39" r:id="rId35" display="#1176"/>
+    <hyperlink ref="B40" r:id="rId36" display="#1171"/>
+    <hyperlink ref="B41" r:id="rId37" display="#1164"/>
+    <hyperlink ref="B42" r:id="rId38" display="#9"/>
+    <hyperlink ref="B43" r:id="rId39" display="#1163"/>
+    <hyperlink ref="B44" r:id="rId40" display="#1161"/>
+    <hyperlink ref="B45" r:id="rId41" display="#1690"/>
+    <hyperlink ref="B47" r:id="rId42" display="#1155"/>
+    <hyperlink ref="B48" r:id="rId43" display="#1150"/>
+    <hyperlink ref="B49" r:id="rId44" display="#1151"/>
+    <hyperlink ref="B50" r:id="rId45" display="#1200"/>
+    <hyperlink ref="B51" r:id="rId46" display="#1681"/>
+    <hyperlink ref="B52" r:id="rId47" display="#51"/>
+    <hyperlink ref="B53" r:id="rId48" display="#1142"/>
+    <hyperlink ref="B54" r:id="rId49" display="#8"/>
+    <hyperlink ref="B55" r:id="rId50" display="#1674"/>
+    <hyperlink ref="B56" r:id="rId51" display="#1672"/>
+    <hyperlink ref="B57" r:id="rId52" display="#1669"/>
+    <hyperlink ref="B58" r:id="rId53" display="#1670"/>
+    <hyperlink ref="B59" r:id="rId54" display="#1184"/>
+    <hyperlink ref="B60" r:id="rId55" display="#49"/>
+    <hyperlink ref="B61" r:id="rId56" display="#1140"/>
+    <hyperlink ref="B62" r:id="rId57" display="#1132"/>
+    <hyperlink ref="B64" r:id="rId58" display="#1125"/>
+    <hyperlink ref="B65" r:id="rId59" display="#1641"/>
+    <hyperlink ref="B66" r:id="rId60" display="#1124"/>
+    <hyperlink ref="B67" r:id="rId61" display="#1122"/>
+    <hyperlink ref="B68" r:id="rId62" display="#43"/>
+    <hyperlink ref="B69" r:id="rId63" display="#1622"/>
+    <hyperlink ref="B71" r:id="rId64" display="#38"/>
+    <hyperlink ref="B72" r:id="rId65" display="#1621"/>
+    <hyperlink ref="B73" r:id="rId66" display="#1616"/>
+    <hyperlink ref="B74" r:id="rId67" display="#37"/>
+    <hyperlink ref="B75" r:id="rId68" display="#36"/>
+    <hyperlink ref="B76" r:id="rId69" display="#1101"/>
+    <hyperlink ref="B77" r:id="rId70" display="#1099"/>
+    <hyperlink ref="B78" r:id="rId71" display="#1098"/>
+    <hyperlink ref="B79" r:id="rId72" display="#1617"/>
+    <hyperlink ref="B80" r:id="rId73" display="#1092"/>
+    <hyperlink ref="B81" r:id="rId74" display="#1128"/>
+    <hyperlink ref="B82" r:id="rId75" display="#1090"/>
+    <hyperlink ref="B83" r:id="rId76" display="#1608"/>
+    <hyperlink ref="B84" r:id="rId77" display="#35"/>
+    <hyperlink ref="B86" r:id="rId78" display="#1070"/>
+    <hyperlink ref="B87" r:id="rId79" display="#1592"/>
+    <hyperlink ref="B88" r:id="rId80" display="#1591"/>
+    <hyperlink ref="B89" r:id="rId81" display="#1578"/>
+    <hyperlink ref="B90" r:id="rId82" display="#41"/>
+    <hyperlink ref="B91" r:id="rId83" display="#42"/>
+    <hyperlink ref="B92" r:id="rId84" display="#1566"/>
+    <hyperlink ref="B93" r:id="rId85" display="#1565"/>
+    <hyperlink ref="B94" r:id="rId86" display="#1046"/>
+    <hyperlink ref="B95" r:id="rId87" display="#1559"/>
+    <hyperlink ref="B96" r:id="rId88" display="#1038"/>
+    <hyperlink ref="B97" r:id="rId89" display="#1037"/>
+    <hyperlink ref="B98" r:id="rId90" display="#1020"/>
+    <hyperlink ref="B99" r:id="rId91" display="#1032"/>
+    <hyperlink ref="B100" r:id="rId92" display="#1546"/>
+    <hyperlink ref="B101" r:id="rId93" display="#1027"/>
+    <hyperlink ref="B102" r:id="rId94" display="#1529"/>
+    <hyperlink ref="B104" r:id="rId95" display="#1527"/>
+    <hyperlink ref="B105" r:id="rId96" display="#558"/>
+    <hyperlink ref="B106" r:id="rId97" display="#1005"/>
+    <hyperlink ref="B107" r:id="rId98" display="#1020"/>
+    <hyperlink ref="B108" r:id="rId99" display="#993"/>
+    <hyperlink ref="B109" r:id="rId100" display="#1520"/>
+    <hyperlink ref="B110" r:id="rId101" display="#1519"/>
+    <hyperlink ref="B111" r:id="rId102" display="#969"/>
+    <hyperlink ref="B112" r:id="rId103" display="#1003"/>
+    <hyperlink ref="B113" r:id="rId104" display="#1015"/>
+    <hyperlink ref="B114" r:id="rId105" display="#1002"/>
+    <hyperlink ref="B115" r:id="rId106" display="#1471"/>
+    <hyperlink ref="B116" r:id="rId107" display="#1497"/>
+    <hyperlink ref="B117" r:id="rId108" display="#947"/>
+    <hyperlink ref="B118" r:id="rId109" display="#933"/>
+    <hyperlink ref="B119" r:id="rId110" display="#932"/>
+    <hyperlink ref="B120" r:id="rId111" display="#931"/>
+    <hyperlink ref="B121" r:id="rId112" display="#987"/>
+    <hyperlink ref="B122" r:id="rId113" display="#988"/>
+    <hyperlink ref="B123" r:id="rId114" display="#982"/>
+    <hyperlink ref="B124" r:id="rId115" display="#979"/>
+    <hyperlink ref="B125" r:id="rId116" display="#977"/>
+    <hyperlink ref="B126" r:id="rId117" display="#975"/>
+    <hyperlink ref="B127" r:id="rId118" display="#1445"/>
+    <hyperlink ref="B128" r:id="rId119" display="#1444"/>
+    <hyperlink ref="B129" r:id="rId120" display="#1427"/>
+    <hyperlink ref="B131" r:id="rId121" display="#23"/>
+    <hyperlink ref="B132" r:id="rId122" display="#22"/>
+    <hyperlink ref="B133" r:id="rId123" display="#18"/>
+    <hyperlink ref="B134" r:id="rId124" display="#1207"/>
+    <hyperlink ref="B135" r:id="rId125" display="#245"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
@@ -4720,7 +4751,7 @@
     <oddHeader>&amp;C&amp;"Sans,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Sans,Regular"Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId125"/>
+  <drawing r:id="rId126"/>
 </worksheet>
 </file>
 
@@ -4753,10 +4784,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -4765,10 +4796,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added omegat ticket #1768
</commit_message>
<xml_diff>
--- a/docs/tools/tickets/OmegaT_issues_nopw.xlsx
+++ b/docs/tools/tickets/OmegaT_issues_nopw.xlsx
@@ -13,8 +13,8 @@
     <sheet name="ETS" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A$1:$F$135</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A:$F</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A:$F</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A$1:$F$136</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="true" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="305">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -118,16 +118,22 @@
     <t xml:space="preserve">WIP</t>
   </si>
   <si>
+    <t xml:space="preserve">#1768</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make the segment marker customizable in Preferences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RFE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open!</t>
+  </si>
+  <si>
     <t xml:space="preserve">#1766</t>
   </si>
   <si>
     <t xml:space="preserve">Customize segment properties fields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RFE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open!</t>
   </si>
   <si>
     <t xml:space="preserve">#274</t>
@@ -1710,14 +1716,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ137"/>
+  <dimension ref="A1:AMJ138"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1770,7 +1776,7 @@
     </row>
     <row r="3" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="n">
-        <v>45604</v>
+        <v>45609</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>30</v>
@@ -1792,21 +1798,21 @@
       <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="n">
-        <v>45563</v>
+        <v>45604</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>36</v>
-      </c>
       <c r="E4" s="11" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>33</v>
@@ -1818,13 +1824,13 @@
     </row>
     <row r="5" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="n">
-        <v>45488</v>
+        <v>45563</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>35</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>38</v>
@@ -1840,17 +1846,17 @@
       <c r="AMI5" s="0"/>
       <c r="AMJ5" s="0"/>
     </row>
-    <row r="6" s="8" customFormat="true" ht="11.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="n">
+    <row r="6" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="n">
         <v>45488</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>39</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>40</v>
       </c>
       <c r="E6" s="11" t="s">
@@ -1864,21 +1870,21 @@
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="8" customFormat="true" ht="11.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>33</v>
@@ -1890,7 +1896,7 @@
     </row>
     <row r="8" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="n">
-        <v>45469</v>
+        <v>45483</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>43</v>
@@ -1905,7 +1911,7 @@
         <v>32</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="AMG8" s="0"/>
       <c r="AMH8" s="0"/>
@@ -1914,22 +1920,22 @@
     </row>
     <row r="9" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="n">
-        <v>45784</v>
+        <v>45469</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>46</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>47</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>32</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="AMG9" s="0"/>
       <c r="AMH9" s="0"/>
@@ -1938,7 +1944,7 @@
     </row>
     <row r="10" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="n">
-        <v>45411</v>
+        <v>45784</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>48</v>
@@ -1960,9 +1966,9 @@
       <c r="AMI10" s="0"/>
       <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="n">
-        <v>45394</v>
+        <v>45411</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>50</v>
@@ -1974,10 +1980,10 @@
         <v>51</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>45</v>
+        <v>32</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="AMG11" s="0"/>
       <c r="AMH11" s="0"/>
@@ -1985,23 +1991,23 @@
       <c r="AMJ11" s="0"/>
     </row>
     <row r="12" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="n">
-        <v>45390</v>
+      <c r="A12" s="12" t="n">
+        <v>45394</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>53</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>54</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="14" t="s">
-        <v>55</v>
+      <c r="F12" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="AMG12" s="0"/>
       <c r="AMH12" s="0"/>
@@ -2010,22 +2016,22 @@
     </row>
     <row r="13" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="n">
-        <v>45365</v>
+        <v>45390</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>56</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>58</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="11" t="s">
-        <v>45</v>
+      <c r="F13" s="14" t="s">
+        <v>57</v>
       </c>
       <c r="AMG13" s="0"/>
       <c r="AMH13" s="0"/>
@@ -2034,58 +2040,58 @@
     </row>
     <row r="14" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="n">
-        <v>45363</v>
+        <v>45365</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="13" t="s">
         <v>60</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AMG14" s="0"/>
       <c r="AMH14" s="0"/>
       <c r="AMI14" s="0"/>
       <c r="AMJ14" s="0"/>
     </row>
-    <row r="15" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+    <row r="15" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="n">
+        <v>45363</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>29</v>
+      <c r="C15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="AMG15" s="0"/>
       <c r="AMH15" s="0"/>
       <c r="AMI15" s="0"/>
       <c r="AMJ15" s="0"/>
     </row>
-    <row r="16" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="n">
-        <v>45238</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="13" t="s">
+    <row r="16" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>33</v>
+      <c r="F16" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="AMG16" s="0"/>
       <c r="AMH16" s="0"/>
@@ -2094,7 +2100,7 @@
     </row>
     <row r="17" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="n">
-        <v>45230</v>
+        <v>45238</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>64</v>
@@ -2102,7 +2108,7 @@
       <c r="C17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="13" t="s">
         <v>65</v>
       </c>
       <c r="E17" s="11" t="s">
@@ -2118,7 +2124,7 @@
     </row>
     <row r="18" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="n">
-        <v>45223</v>
+        <v>45230</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>66</v>
@@ -2132,8 +2138,8 @@
       <c r="E18" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="11" t="s">
-        <v>45</v>
+      <c r="F18" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="AMG18" s="0"/>
       <c r="AMH18" s="0"/>
@@ -2142,7 +2148,7 @@
     </row>
     <row r="19" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="n">
-        <v>45236</v>
+        <v>45223</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>68</v>
@@ -2154,10 +2160,10 @@
         <v>69</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>70</v>
+        <v>32</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="AMG19" s="0"/>
       <c r="AMH19" s="0"/>
@@ -2166,22 +2172,22 @@
     </row>
     <row r="20" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="n">
-        <v>45233</v>
+        <v>45236</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>71</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>72</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="14" t="s">
-        <v>33</v>
+      <c r="F20" s="15" t="s">
+        <v>72</v>
       </c>
       <c r="AMG20" s="0"/>
       <c r="AMH20" s="0"/>
@@ -2190,7 +2196,7 @@
     </row>
     <row r="21" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="n">
-        <v>45213</v>
+        <v>45233</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>73</v>
@@ -2202,10 +2208,10 @@
         <v>74</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>45</v>
+        <v>9</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="AMG21" s="0"/>
       <c r="AMH21" s="0"/>
@@ -2214,22 +2220,22 @@
     </row>
     <row r="22" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="n">
-        <v>45199</v>
+        <v>45213</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>75</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>76</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AMG22" s="0"/>
       <c r="AMH22" s="0"/>
@@ -2238,22 +2244,22 @@
     </row>
     <row r="23" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="n">
-        <v>45170</v>
+        <v>45199</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>77</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>78</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AMG23" s="0"/>
       <c r="AMH23" s="0"/>
@@ -2262,7 +2268,7 @@
     </row>
     <row r="24" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="n">
-        <v>45169</v>
+        <v>45170</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>79</v>
@@ -2277,7 +2283,7 @@
         <v>32</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AMG24" s="0"/>
       <c r="AMH24" s="0"/>
@@ -2285,23 +2291,23 @@
       <c r="AMJ24" s="0"/>
     </row>
     <row r="25" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16" t="n">
+      <c r="A25" s="9" t="n">
         <v>45169</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="18" t="s">
+      <c r="C25" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>82</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="AMG25" s="0"/>
       <c r="AMH25" s="0"/>
@@ -2310,7 +2316,7 @@
     </row>
     <row r="26" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="n">
-        <v>45145</v>
+        <v>45169</v>
       </c>
       <c r="B26" s="17" t="s">
         <v>83</v>
@@ -2319,7 +2325,7 @@
         <v>7</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="E26" s="18" t="s">
         <v>9</v>
@@ -2333,23 +2339,23 @@
       <c r="AMJ26" s="0"/>
     </row>
     <row r="27" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="n">
+      <c r="A27" s="16" t="n">
         <v>45145</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="11" t="s">
+      <c r="C27" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="18" t="s">
         <v>86</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="19" t="s">
-        <v>55</v>
       </c>
       <c r="AMG27" s="0"/>
       <c r="AMH27" s="0"/>
@@ -2373,37 +2379,40 @@
         <v>9</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AMG28" s="0"/>
       <c r="AMH28" s="0"/>
       <c r="AMI28" s="0"/>
       <c r="AMJ28" s="0"/>
     </row>
-    <row r="29" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="n">
-        <v>45112</v>
+        <v>45145</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>55</v>
+        <v>90</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>57</v>
       </c>
       <c r="AMG29" s="0"/>
       <c r="AMH29" s="0"/>
       <c r="AMI29" s="0"/>
       <c r="AMJ29" s="0"/>
     </row>
-    <row r="30" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="n">
-        <v>45124</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>90</v>
+        <v>45112</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>7</v>
@@ -2411,11 +2420,8 @@
       <c r="D30" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E30" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>33</v>
+      <c r="F30" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="AMG30" s="0"/>
       <c r="AMH30" s="0"/>
@@ -2424,19 +2430,19 @@
     </row>
     <row r="31" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="n">
-        <v>45119</v>
+        <v>45124</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>92</v>
       </c>
       <c r="C31" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D31" s="11" t="s">
-        <v>94</v>
-      </c>
       <c r="E31" s="11" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F31" s="14" t="s">
         <v>33</v>
@@ -2451,10 +2457,10 @@
         <v>45119</v>
       </c>
       <c r="B32" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="D32" s="11" t="s">
         <v>96</v>
@@ -2472,19 +2478,19 @@
     </row>
     <row r="33" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="n">
-        <v>45118</v>
+        <v>45119</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>97</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>98</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F33" s="14" t="s">
         <v>33</v>
@@ -2520,7 +2526,7 @@
     </row>
     <row r="35" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="n">
-        <v>45110</v>
+        <v>45118</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>101</v>
@@ -2532,10 +2538,10 @@
         <v>102</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>45</v>
+        <v>9</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="AMG35" s="0"/>
       <c r="AMH35" s="0"/>
@@ -2544,7 +2550,7 @@
     </row>
     <row r="36" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="n">
-        <v>45104</v>
+        <v>45110</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>103</v>
@@ -2556,49 +2562,49 @@
         <v>104</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="21" t="s">
-        <v>105</v>
+        <v>32</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="AMG36" s="0"/>
       <c r="AMH36" s="0"/>
       <c r="AMI36" s="0"/>
       <c r="AMJ36" s="0"/>
     </row>
-    <row r="37" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="n">
-        <v>45094</v>
+        <v>45104</v>
       </c>
       <c r="B37" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="11" t="s">
         <v>106</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>108</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="20" t="s">
-        <v>55</v>
+      <c r="F37" s="21" t="s">
+        <v>107</v>
       </c>
       <c r="AMG37" s="0"/>
       <c r="AMH37" s="0"/>
       <c r="AMI37" s="0"/>
       <c r="AMJ37" s="0"/>
     </row>
-    <row r="38" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="n">
-        <v>45069</v>
+        <v>45094</v>
       </c>
       <c r="B38" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="11" t="s">
         <v>109</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>13</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>110</v>
@@ -2606,41 +2612,41 @@
       <c r="E38" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F38" s="22" t="s">
-        <v>111</v>
+      <c r="F38" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="AMG38" s="0"/>
       <c r="AMH38" s="0"/>
       <c r="AMI38" s="0"/>
       <c r="AMJ38" s="0"/>
     </row>
-    <row r="39" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="n">
         <v>45069</v>
       </c>
       <c r="B39" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="11" t="s">
         <v>112</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>113</v>
       </c>
       <c r="E39" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F39" s="20" t="s">
-        <v>55</v>
+      <c r="F39" s="22" t="s">
+        <v>113</v>
       </c>
       <c r="AMG39" s="0"/>
       <c r="AMH39" s="0"/>
       <c r="AMI39" s="0"/>
       <c r="AMJ39" s="0"/>
     </row>
-    <row r="40" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="n">
-        <v>45064</v>
+        <v>45069</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>114</v>
@@ -2654,17 +2660,17 @@
       <c r="E40" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F40" s="11" t="s">
-        <v>45</v>
+      <c r="F40" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="AMG40" s="0"/>
       <c r="AMH40" s="0"/>
       <c r="AMI40" s="0"/>
       <c r="AMJ40" s="0"/>
     </row>
-    <row r="41" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="n">
-        <v>45049</v>
+        <v>45064</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>116</v>
@@ -2678,8 +2684,8 @@
       <c r="E41" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F41" s="23" t="s">
-        <v>55</v>
+      <c r="F41" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="AMG41" s="0"/>
       <c r="AMH41" s="0"/>
@@ -2693,17 +2699,17 @@
       <c r="B42" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="24" t="s">
-        <v>107</v>
+      <c r="C42" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>119</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>55</v>
+        <v>9</v>
+      </c>
+      <c r="F42" s="23" t="s">
+        <v>57</v>
       </c>
       <c r="AMG42" s="0"/>
       <c r="AMH42" s="0"/>
@@ -2712,31 +2718,31 @@
     </row>
     <row r="43" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="n">
-        <v>45044</v>
+        <v>45049</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="C43" s="11" t="s">
-        <v>7</v>
+      <c r="C43" s="24" t="s">
+        <v>109</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>121</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AMG43" s="0"/>
       <c r="AMH43" s="0"/>
       <c r="AMI43" s="0"/>
       <c r="AMJ43" s="0"/>
     </row>
-    <row r="44" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="n">
-        <v>45040</v>
+        <v>45044</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>122</v>
@@ -2750,17 +2756,17 @@
       <c r="E44" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F44" s="11" t="s">
-        <v>45</v>
+      <c r="F44" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="AMG44" s="0"/>
       <c r="AMH44" s="0"/>
       <c r="AMI44" s="0"/>
       <c r="AMJ44" s="0"/>
     </row>
-    <row r="45" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="n">
-        <v>45028</v>
+        <v>45040</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>124</v>
@@ -2772,10 +2778,10 @@
         <v>125</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F45" s="20" t="s">
-        <v>55</v>
+        <v>9</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="AMG45" s="0"/>
       <c r="AMH45" s="0"/>
@@ -2784,16 +2790,22 @@
     </row>
     <row r="46" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="n">
-        <v>44996</v>
+        <v>45028</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>126</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AMG46" s="0"/>
       <c r="AMH46" s="0"/>
@@ -2802,31 +2814,25 @@
     </row>
     <row r="47" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="n">
-        <v>45007</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>127</v>
+        <v>44996</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="D47" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="E47" s="11" t="s">
-        <v>9</v>
-      </c>
       <c r="F47" s="20" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AMG47" s="0"/>
       <c r="AMH47" s="0"/>
       <c r="AMI47" s="0"/>
       <c r="AMJ47" s="0"/>
     </row>
-    <row r="48" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="n">
-        <v>44993</v>
+        <v>45007</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>129</v>
@@ -2840,8 +2846,8 @@
       <c r="E48" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F48" s="21" t="s">
-        <v>105</v>
+      <c r="F48" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="AMG48" s="0"/>
       <c r="AMH48" s="0"/>
@@ -2865,7 +2871,7 @@
         <v>9</v>
       </c>
       <c r="F49" s="21" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AMG49" s="0"/>
       <c r="AMH49" s="0"/>
@@ -2874,22 +2880,22 @@
     </row>
     <row r="50" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="n">
-        <v>44991</v>
+        <v>44993</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E50" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F50" s="11" t="s">
-        <v>134</v>
+      <c r="F50" s="21" t="s">
+        <v>107</v>
       </c>
       <c r="AMG50" s="0"/>
       <c r="AMH50" s="0"/>
@@ -2898,22 +2904,22 @@
     </row>
     <row r="51" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="n">
-        <v>44981</v>
+        <v>44991</v>
       </c>
       <c r="B51" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="C51" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" s="11" t="s">
+      <c r="E51" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="11" t="s">
         <v>136</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F51" s="11" t="s">
-        <v>45</v>
       </c>
       <c r="AMG51" s="0"/>
       <c r="AMH51" s="0"/>
@@ -2922,22 +2928,22 @@
     </row>
     <row r="52" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="n">
-        <v>44973</v>
+        <v>44981</v>
       </c>
       <c r="B52" s="10" t="s">
         <v>137</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="D52" s="11" t="s">
         <v>138</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="AMG52" s="0"/>
       <c r="AMH52" s="0"/>
@@ -2945,47 +2951,47 @@
       <c r="AMJ52" s="0"/>
     </row>
     <row r="53" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="16" t="n">
-        <v>44972</v>
-      </c>
-      <c r="B53" s="17" t="s">
+      <c r="A53" s="9" t="n">
+        <v>44973</v>
+      </c>
+      <c r="B53" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C53" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="E53" s="18" t="s">
+      <c r="C53" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="E53" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F53" s="18" t="s">
-        <v>82</v>
+      <c r="F53" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="AMG53" s="0"/>
       <c r="AMH53" s="0"/>
       <c r="AMI53" s="0"/>
       <c r="AMJ53" s="0"/>
     </row>
-    <row r="54" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="26" t="n">
-        <v>44970</v>
-      </c>
-      <c r="B54" s="27" t="s">
+    <row r="54" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="16" t="n">
+        <v>44972</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="C54" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="D54" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="E54" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F54" s="24" t="s">
-        <v>45</v>
+      <c r="E54" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>84</v>
       </c>
       <c r="AMG54" s="0"/>
       <c r="AMH54" s="0"/>
@@ -2994,13 +3000,13 @@
     </row>
     <row r="55" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="26" t="n">
-        <v>44967</v>
+        <v>44970</v>
       </c>
       <c r="B55" s="27" t="s">
         <v>142</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>7</v>
+        <v>109</v>
       </c>
       <c r="D55" s="24" t="s">
         <v>143</v>
@@ -3008,8 +3014,8 @@
       <c r="E55" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F55" s="14" t="s">
-        <v>33</v>
+      <c r="F55" s="24" t="s">
+        <v>47</v>
       </c>
       <c r="AMG55" s="0"/>
       <c r="AMH55" s="0"/>
@@ -3018,7 +3024,7 @@
     </row>
     <row r="56" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="26" t="n">
-        <v>44964</v>
+        <v>44967</v>
       </c>
       <c r="B56" s="27" t="s">
         <v>144</v>
@@ -3032,8 +3038,8 @@
       <c r="E56" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F56" s="21" t="s">
-        <v>105</v>
+      <c r="F56" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="AMG56" s="0"/>
       <c r="AMH56" s="0"/>
@@ -3042,7 +3048,7 @@
     </row>
     <row r="57" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="26" t="n">
-        <v>44952</v>
+        <v>44964</v>
       </c>
       <c r="B57" s="27" t="s">
         <v>146</v>
@@ -3057,7 +3063,7 @@
         <v>32</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AMG57" s="0"/>
       <c r="AMH57" s="0"/>
@@ -3080,8 +3086,8 @@
       <c r="E58" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F58" s="20" t="s">
-        <v>55</v>
+      <c r="F58" s="21" t="s">
+        <v>107</v>
       </c>
       <c r="AMG58" s="0"/>
       <c r="AMH58" s="0"/>
@@ -3089,23 +3095,23 @@
       <c r="AMJ58" s="0"/>
     </row>
     <row r="59" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="28" t="n">
-        <v>44949</v>
-      </c>
-      <c r="B59" s="29" t="s">
+      <c r="A59" s="26" t="n">
+        <v>44952</v>
+      </c>
+      <c r="B59" s="27" t="s">
         <v>150</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D59" s="24" t="s">
         <v>151</v>
       </c>
       <c r="E59" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="AMG59" s="0"/>
       <c r="AMH59" s="0"/>
@@ -3113,23 +3119,23 @@
       <c r="AMJ59" s="0"/>
     </row>
     <row r="60" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="26" t="n">
-        <v>44948</v>
-      </c>
-      <c r="B60" s="27" t="s">
+      <c r="A60" s="28" t="n">
+        <v>44949</v>
+      </c>
+      <c r="B60" s="29" t="s">
         <v>152</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="D60" s="24" t="s">
         <v>153</v>
       </c>
       <c r="E60" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F60" s="20" t="s">
-        <v>55</v>
+        <v>9</v>
+      </c>
+      <c r="F60" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="AMG60" s="0"/>
       <c r="AMH60" s="0"/>
@@ -3138,58 +3144,70 @@
     </row>
     <row r="61" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="26" t="n">
-        <v>44946</v>
+        <v>44948</v>
       </c>
       <c r="B61" s="27" t="s">
         <v>154</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="D61" s="24" t="s">
         <v>155</v>
       </c>
       <c r="E61" s="24" t="s">
-        <v>156</v>
+        <v>32</v>
       </c>
       <c r="F61" s="20" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AMG61" s="0"/>
       <c r="AMH61" s="0"/>
       <c r="AMI61" s="0"/>
       <c r="AMJ61" s="0"/>
     </row>
-    <row r="62" s="24" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="26" t="n">
-        <v>44929</v>
-      </c>
-      <c r="B62" s="30" t="s">
+        <v>44946</v>
+      </c>
+      <c r="B62" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="C62" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="C62" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D62" s="24" t="s">
+      <c r="E62" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="E62" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="F62" s="14" t="s">
-        <v>33</v>
+      <c r="F62" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="AMG62" s="0"/>
       <c r="AMH62" s="0"/>
       <c r="AMI62" s="0"/>
       <c r="AMJ62" s="0"/>
     </row>
-    <row r="63" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="8" t="s">
+    <row r="63" s="24" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="26" t="n">
+        <v>44929</v>
+      </c>
+      <c r="B63" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="F63" s="8" t="s">
-        <v>29</v>
+      <c r="C63" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="E63" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="AMG63" s="0"/>
       <c r="AMH63" s="0"/>
@@ -3197,71 +3215,59 @@
       <c r="AMJ63" s="0"/>
     </row>
     <row r="64" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="26" t="n">
-        <v>44879</v>
-      </c>
-      <c r="B64" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D64" s="5" t="s">
+      <c r="A64" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="E64" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>45</v>
+      <c r="F64" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="AMG64" s="0"/>
       <c r="AMH64" s="0"/>
       <c r="AMI64" s="0"/>
       <c r="AMJ64" s="0"/>
     </row>
-    <row r="65" s="24" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="26" t="n">
-        <v>44858</v>
-      </c>
-      <c r="B65" s="27" t="s">
+        <v>44879</v>
+      </c>
+      <c r="B65" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="C65" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D65" s="24" t="s">
+      <c r="C65" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="E65" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F65" s="24" t="s">
-        <v>45</v>
+      <c r="E65" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="AMG65" s="0"/>
       <c r="AMH65" s="0"/>
       <c r="AMI65" s="0"/>
       <c r="AMJ65" s="0"/>
     </row>
-    <row r="66" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" s="24" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="26" t="n">
-        <v>44855</v>
-      </c>
-      <c r="B66" s="31" t="s">
+        <v>44858</v>
+      </c>
+      <c r="B66" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="C66" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D66" s="5" t="s">
+      <c r="C66" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="E66" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F66" s="21" t="s">
-        <v>105</v>
+      <c r="E66" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F66" s="24" t="s">
+        <v>47</v>
       </c>
       <c r="AMG66" s="0"/>
       <c r="AMH66" s="0"/>
@@ -3270,7 +3276,7 @@
     </row>
     <row r="67" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="26" t="n">
-        <v>44844</v>
+        <v>44855</v>
       </c>
       <c r="B67" s="31" t="s">
         <v>166</v>
@@ -3282,105 +3288,109 @@
         <v>167</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>168</v>
+        <v>158</v>
+      </c>
+      <c r="F67" s="21" t="s">
+        <v>107</v>
       </c>
       <c r="AMG67" s="0"/>
       <c r="AMH67" s="0"/>
       <c r="AMI67" s="0"/>
       <c r="AMJ67" s="0"/>
     </row>
-    <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="26" t="n">
-        <v>44757</v>
-      </c>
-      <c r="B68" s="32" t="s">
+        <v>44844</v>
+      </c>
+      <c r="B68" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="C68" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D68" s="5" t="s">
+      <c r="E68" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F68" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="E68" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F68" s="20" t="s">
-        <v>55</v>
-      </c>
+      <c r="AMG68" s="0"/>
+      <c r="AMH68" s="0"/>
+      <c r="AMI68" s="0"/>
+      <c r="AMJ68" s="0"/>
     </row>
     <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="26" t="n">
-        <v>373466</v>
-      </c>
-      <c r="B69" s="31" t="s">
+        <v>44757</v>
+      </c>
+      <c r="B69" s="32" t="s">
         <v>171</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>172</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>45</v>
+        <v>158</v>
+      </c>
+      <c r="F69" s="20" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="26" t="n">
-        <v>44743</v>
+        <v>373466</v>
+      </c>
+      <c r="B70" s="31" t="s">
+        <v>173</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F70" s="20" t="s">
-        <v>55</v>
+        <v>174</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="26" t="n">
-        <v>44740</v>
-      </c>
-      <c r="B71" s="33" t="s">
-        <v>174</v>
+        <v>44743</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="E71" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F71" s="14" t="s">
-        <v>33</v>
+      <c r="F71" s="20" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="26" t="n">
-        <v>44739</v>
-      </c>
-      <c r="B72" s="34" t="s">
+        <v>44740</v>
+      </c>
+      <c r="B72" s="33" t="s">
         <v>176</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>177</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>23</v>
+        <v>158</v>
       </c>
       <c r="F72" s="14" t="s">
         <v>33</v>
@@ -3388,7 +3398,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="26" t="n">
-        <v>44693</v>
+        <v>44739</v>
       </c>
       <c r="B73" s="34" t="s">
         <v>178</v>
@@ -3400,7 +3410,7 @@
         <v>179</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F73" s="14" t="s">
         <v>33</v>
@@ -3408,69 +3418,69 @@
     </row>
     <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="26" t="n">
-        <v>44695</v>
-      </c>
-      <c r="B74" s="35" t="s">
+        <v>44693</v>
+      </c>
+      <c r="B74" s="34" t="s">
         <v>180</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>181</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F74" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F74" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="26" t="n">
+        <v>44695</v>
+      </c>
+      <c r="B75" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="C75" s="5" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="28" t="n">
-        <v>44659</v>
-      </c>
-      <c r="B75" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F75" s="14" t="s">
-        <v>33</v>
+        <v>158</v>
+      </c>
+      <c r="F75" s="20" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="26" t="n">
-        <v>44712</v>
-      </c>
-      <c r="B76" s="34" t="s">
+      <c r="A76" s="28" t="n">
+        <v>44659</v>
+      </c>
+      <c r="B76" s="36" t="s">
         <v>184</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>185</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>111</v>
+        <v>158</v>
+      </c>
+      <c r="F76" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="26" t="n">
-        <v>44705</v>
-      </c>
-      <c r="B77" s="31" t="s">
+        <v>44712</v>
+      </c>
+      <c r="B77" s="34" t="s">
         <v>186</v>
       </c>
       <c r="C77" s="5" t="s">
@@ -3480,10 +3490,10 @@
         <v>187</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F77" s="20" t="s">
-        <v>55</v>
+        <v>32</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3500,15 +3510,15 @@
         <v>189</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F78" s="20" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="26" t="n">
-        <v>44693</v>
+        <v>44705</v>
       </c>
       <c r="B79" s="31" t="s">
         <v>190</v>
@@ -3520,15 +3530,15 @@
         <v>191</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>45</v>
+        <v>158</v>
+      </c>
+      <c r="F79" s="20" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="26" t="n">
-        <v>44622</v>
+        <v>44693</v>
       </c>
       <c r="B80" s="31" t="s">
         <v>192</v>
@@ -3540,57 +3550,57 @@
         <v>193</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F80" s="20" t="s">
-        <v>55</v>
+        <v>32</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="26" t="n">
-        <v>44614</v>
+        <v>44622</v>
       </c>
       <c r="B81" s="31" t="s">
         <v>194</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>195</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F81" s="14" t="s">
-        <v>33</v>
+        <v>158</v>
+      </c>
+      <c r="F81" s="20" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="26" t="n">
-        <v>44613</v>
+        <v>44614</v>
       </c>
       <c r="B82" s="31" t="s">
         <v>196</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>197</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>45</v>
+        <v>158</v>
+      </c>
+      <c r="F82" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="26" t="n">
-        <v>44608</v>
-      </c>
-      <c r="B83" s="34" t="s">
+        <v>44613</v>
+      </c>
+      <c r="B83" s="31" t="s">
         <v>198</v>
       </c>
       <c r="C83" s="5" t="s">
@@ -3600,60 +3610,60 @@
         <v>199</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F83" s="20" t="s">
-        <v>55</v>
+        <v>158</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="26" t="n">
-        <v>44580</v>
-      </c>
-      <c r="B84" s="31" t="s">
+        <v>44608</v>
+      </c>
+      <c r="B84" s="34" t="s">
         <v>200</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>201</v>
       </c>
       <c r="E84" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F84" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="26" t="n">
+        <v>44580</v>
+      </c>
+      <c r="B85" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E85" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F84" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="26" t="n">
-        <v>44463</v>
-      </c>
-      <c r="B86" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D86" s="5" t="s">
+      <c r="F85" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="5" t="s">
         <v>204</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="26" t="n">
-        <v>44460</v>
+        <v>44463</v>
       </c>
       <c r="B87" s="31" t="s">
         <v>205</v>
@@ -3665,10 +3675,10 @@
         <v>206</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>32</v>
+        <v>158</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>207</v>
+        <v>47</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3676,24 +3686,24 @@
         <v>44460</v>
       </c>
       <c r="B88" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D88" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C88" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D88" s="5" t="s">
+      <c r="E88" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F88" s="5" t="s">
         <v>209</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F88" s="20" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="26" t="n">
-        <v>44372</v>
+        <v>44460</v>
       </c>
       <c r="B89" s="31" t="s">
         <v>210</v>
@@ -3707,73 +3717,73 @@
       <c r="E89" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F89" s="5" t="s">
-        <v>45</v>
+      <c r="F89" s="20" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="26" t="n">
-        <v>44326</v>
+        <v>44372</v>
       </c>
       <c r="B90" s="31" t="s">
         <v>212</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>213</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>156</v>
+        <v>23</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>168</v>
+        <v>47</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="28" t="n">
-        <v>44325</v>
-      </c>
-      <c r="B91" s="37" t="s">
+      <c r="A91" s="26" t="n">
+        <v>44326</v>
+      </c>
+      <c r="B91" s="31" t="s">
         <v>214</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>215</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F91" s="14" t="s">
-        <v>33</v>
+        <v>158</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="26" t="n">
+      <c r="A92" s="28" t="n">
         <v>44325</v>
       </c>
-      <c r="B92" s="31" t="s">
+      <c r="B92" s="37" t="s">
         <v>216</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>217</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F92" s="5" t="s">
-        <v>45</v>
+        <v>158</v>
+      </c>
+      <c r="F92" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="26" t="n">
-        <v>44321</v>
+        <v>44325</v>
       </c>
       <c r="B93" s="31" t="s">
         <v>218</v>
@@ -3785,15 +3795,15 @@
         <v>219</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F93" s="21" t="s">
-        <v>105</v>
+        <v>23</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="26" t="n">
-        <v>44316</v>
+        <v>44321</v>
       </c>
       <c r="B94" s="31" t="s">
         <v>220</v>
@@ -3805,37 +3815,37 @@
         <v>221</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F94" s="5" t="s">
-        <v>222</v>
+        <v>32</v>
+      </c>
+      <c r="F94" s="21" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="26" t="n">
-        <v>44279</v>
-      </c>
-      <c r="B95" s="5" t="s">
+        <v>44316</v>
+      </c>
+      <c r="B95" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D95" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="C95" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D95" s="5" t="s">
+      <c r="E95" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F95" s="5" t="s">
         <v>224</v>
-      </c>
-      <c r="E95" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F95" s="14" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="26" t="n">
-        <v>44257</v>
-      </c>
-      <c r="B96" s="31" t="s">
+        <v>44279</v>
+      </c>
+      <c r="B96" s="5" t="s">
         <v>225</v>
       </c>
       <c r="C96" s="5" t="s">
@@ -3845,15 +3855,15 @@
         <v>226</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
+      </c>
+      <c r="F96" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="26" t="n">
-        <v>44243</v>
+        <v>44257</v>
       </c>
       <c r="B97" s="31" t="s">
         <v>227</v>
@@ -3865,57 +3875,57 @@
         <v>228</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="38" t="n">
+      <c r="A98" s="26" t="n">
+        <v>44243</v>
+      </c>
+      <c r="B98" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="38" t="n">
         <v>44231</v>
       </c>
-      <c r="B98" s="39" t="s">
-        <v>229</v>
-      </c>
-      <c r="C98" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D98" s="40" t="s">
-        <v>175</v>
-      </c>
-      <c r="E98" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="F98" s="40" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="26" t="n">
-        <v>44218</v>
-      </c>
-      <c r="B99" s="31" t="s">
-        <v>230</v>
-      </c>
-      <c r="C99" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D99" s="5" t="s">
+      <c r="B99" s="39" t="s">
         <v>231</v>
       </c>
-      <c r="E99" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F99" s="5" t="s">
-        <v>45</v>
+      <c r="C99" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D99" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="E99" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="F99" s="40" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="26" t="n">
-        <v>44216</v>
-      </c>
-      <c r="B100" s="34" t="s">
+        <v>44218</v>
+      </c>
+      <c r="B100" s="31" t="s">
         <v>232</v>
       </c>
       <c r="C100" s="5" t="s">
@@ -3925,17 +3935,17 @@
         <v>233</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F100" s="14" t="s">
-        <v>33</v>
+        <v>158</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="26" t="n">
-        <v>44175</v>
-      </c>
-      <c r="B101" s="31" t="s">
+        <v>44216</v>
+      </c>
+      <c r="B101" s="34" t="s">
         <v>234</v>
       </c>
       <c r="C101" s="5" t="s">
@@ -3945,10 +3955,10 @@
         <v>235</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F101" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
+      </c>
+      <c r="F101" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3965,40 +3975,40 @@
         <v>237</v>
       </c>
       <c r="E102" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="26" t="n">
+        <v>44175</v>
+      </c>
+      <c r="B103" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="E103" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F102" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="26" t="n">
-        <v>44162</v>
-      </c>
-      <c r="B104" s="31" t="s">
-        <v>238</v>
-      </c>
-      <c r="C104" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D104" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="E104" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F104" s="5" t="s">
-        <v>45</v>
+      <c r="F103" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="5" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="26" t="n">
-        <v>44148</v>
+        <v>44162</v>
       </c>
       <c r="B105" s="31" t="s">
         <v>240</v>
@@ -4007,124 +4017,124 @@
         <v>7</v>
       </c>
       <c r="D105" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="26" t="n">
+        <v>44148</v>
+      </c>
+      <c r="B106" s="31" t="s">
+        <v>242</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D106" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E105" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F105" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="38" t="n">
+      <c r="E106" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="38" t="n">
         <v>44146</v>
       </c>
-      <c r="B106" s="39" t="s">
-        <v>241</v>
-      </c>
-      <c r="C106" s="40" t="s">
+      <c r="B107" s="39" t="s">
+        <v>243</v>
+      </c>
+      <c r="C107" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D106" s="40" t="s">
-        <v>242</v>
-      </c>
-      <c r="E106" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="F106" s="40" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="26" t="n">
-        <v>44132</v>
-      </c>
-      <c r="B107" s="31" t="s">
-        <v>229</v>
-      </c>
-      <c r="C107" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D107" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="E107" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F107" s="5" t="s">
-        <v>45</v>
+      <c r="D107" s="40" t="s">
+        <v>244</v>
+      </c>
+      <c r="E107" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="F107" s="40" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="26" t="n">
-        <v>44103</v>
+        <v>44132</v>
       </c>
       <c r="B108" s="31" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>245</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="38" t="n">
+      <c r="A109" s="26" t="n">
+        <v>44103</v>
+      </c>
+      <c r="B109" s="31" t="s">
+        <v>246</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="38" t="n">
         <v>44095</v>
       </c>
-      <c r="B109" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="C109" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D109" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="E109" s="40" t="s">
+      <c r="B110" s="39" t="s">
+        <v>248</v>
+      </c>
+      <c r="C110" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D110" s="40" t="s">
+        <v>249</v>
+      </c>
+      <c r="E110" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="F109" s="40" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="26" t="n">
-        <v>44095</v>
-      </c>
-      <c r="B110" s="31" t="s">
-        <v>248</v>
-      </c>
-      <c r="C110" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D110" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="E110" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F110" s="20" t="s">
-        <v>55</v>
+      <c r="F110" s="40" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="26" t="n">
-        <v>44057</v>
+        <v>44095</v>
       </c>
       <c r="B111" s="31" t="s">
         <v>250</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>251</v>
@@ -4132,33 +4142,33 @@
       <c r="E111" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F111" s="5" t="s">
-        <v>207</v>
+      <c r="F111" s="20" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="26" t="n">
-        <v>44028</v>
+        <v>44057</v>
       </c>
       <c r="B112" s="31" t="s">
         <v>252</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>253</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F112" s="20" t="s">
-        <v>55</v>
+        <v>32</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="26" t="n">
-        <v>44064</v>
+        <v>44028</v>
       </c>
       <c r="B113" s="31" t="s">
         <v>254</v>
@@ -4170,15 +4180,15 @@
         <v>255</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F113" s="5" t="s">
-        <v>45</v>
+        <v>158</v>
+      </c>
+      <c r="F113" s="20" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="26" t="n">
-        <v>44028</v>
+        <v>44064</v>
       </c>
       <c r="B114" s="31" t="s">
         <v>256</v>
@@ -4190,15 +4200,15 @@
         <v>257</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F114" s="20" t="s">
-        <v>55</v>
+        <v>158</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="26" t="n">
-        <v>44016</v>
+        <v>44028</v>
       </c>
       <c r="B115" s="31" t="s">
         <v>258</v>
@@ -4210,15 +4220,15 @@
         <v>259</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F115" s="5" t="s">
-        <v>45</v>
+        <v>158</v>
+      </c>
+      <c r="F115" s="20" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="26" t="n">
-        <v>44010</v>
+        <v>44016</v>
       </c>
       <c r="B116" s="31" t="s">
         <v>260</v>
@@ -4230,35 +4240,35 @@
         <v>261</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="26" t="n">
-        <v>43995</v>
+        <v>44010</v>
       </c>
       <c r="B117" s="31" t="s">
         <v>262</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>263</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="26" t="n">
-        <v>43948</v>
+        <v>43995</v>
       </c>
       <c r="B118" s="31" t="s">
         <v>264</v>
@@ -4270,15 +4280,15 @@
         <v>265</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F118" s="20" t="s">
-        <v>55</v>
+        <v>32</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="26" t="n">
-        <v>43947</v>
+        <v>43948</v>
       </c>
       <c r="B119" s="31" t="s">
         <v>266</v>
@@ -4290,15 +4300,15 @@
         <v>267</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F119" s="14" t="s">
-        <v>33</v>
+        <v>158</v>
+      </c>
+      <c r="F119" s="20" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="26" t="n">
-        <v>43936</v>
+        <v>43947</v>
       </c>
       <c r="B120" s="31" t="s">
         <v>268</v>
@@ -4310,35 +4320,35 @@
         <v>269</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F120" s="5" t="s">
-        <v>45</v>
+        <v>158</v>
+      </c>
+      <c r="F120" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="26" t="n">
-        <v>43929</v>
+        <v>43936</v>
       </c>
       <c r="B121" s="31" t="s">
         <v>270</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>271</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>156</v>
+        <v>32</v>
       </c>
       <c r="F121" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="26" t="n">
-        <v>43891</v>
+        <v>43929</v>
       </c>
       <c r="B122" s="31" t="s">
         <v>272</v>
@@ -4350,15 +4360,15 @@
         <v>273</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F122" s="20" t="s">
-        <v>55</v>
+        <v>158</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="26" t="n">
-        <v>43885</v>
+        <v>43891</v>
       </c>
       <c r="B123" s="31" t="s">
         <v>274</v>
@@ -4370,15 +4380,15 @@
         <v>275</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F123" s="5" t="s">
-        <v>45</v>
+        <v>158</v>
+      </c>
+      <c r="F123" s="20" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="26" t="n">
-        <v>43857</v>
+        <v>43885</v>
       </c>
       <c r="B124" s="31" t="s">
         <v>276</v>
@@ -4390,10 +4400,10 @@
         <v>277</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F124" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4410,15 +4420,15 @@
         <v>279</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F125" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="26" t="n">
-        <v>43852</v>
+        <v>43857</v>
       </c>
       <c r="B126" s="31" t="s">
         <v>280</v>
@@ -4430,15 +4440,15 @@
         <v>281</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="26" t="n">
-        <v>43584</v>
+        <v>43852</v>
       </c>
       <c r="B127" s="31" t="s">
         <v>282</v>
@@ -4450,10 +4460,10 @@
         <v>283</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>23</v>
+        <v>158</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4473,14 +4483,14 @@
         <v>23</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="26" t="n">
-        <v>43540</v>
-      </c>
-      <c r="B129" s="5" t="s">
+        <v>43584</v>
+      </c>
+      <c r="B129" s="31" t="s">
         <v>286</v>
       </c>
       <c r="C129" s="5" t="s">
@@ -4493,32 +4503,32 @@
         <v>23</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="26" t="n">
-        <v>43203</v>
-      </c>
-      <c r="B131" s="41" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="26" t="n">
+        <v>43540</v>
+      </c>
+      <c r="B130" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="C131" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D131" s="5" t="s">
+      <c r="C130" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D130" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="E131" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F131" s="14" t="s">
-        <v>33</v>
+      <c r="E130" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F130" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="5" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4529,61 +4539,61 @@
         <v>290</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D132" s="5" t="s">
         <v>291</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F132" s="5" t="s">
-        <v>292</v>
+        <v>158</v>
+      </c>
+      <c r="F132" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="26" t="n">
-        <v>42842</v>
+        <v>43203</v>
       </c>
       <c r="B133" s="41" t="s">
+        <v>292</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D133" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="C133" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D133" s="5" t="s">
+      <c r="E133" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F133" s="5" t="s">
         <v>294</v>
-      </c>
-      <c r="E133" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F133" s="14" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="26" t="n">
-        <v>42457</v>
-      </c>
-      <c r="B134" s="5" t="s">
+        <v>42842</v>
+      </c>
+      <c r="B134" s="41" t="s">
         <v>295</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="D134" s="5" t="s">
         <v>296</v>
       </c>
       <c r="E134" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F134" s="5" t="s">
-        <v>45</v>
+        <v>32</v>
+      </c>
+      <c r="F134" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="26" t="n">
-        <v>39028</v>
+        <v>42457</v>
       </c>
       <c r="B135" s="5" t="s">
         <v>297</v>
@@ -4595,21 +4605,41 @@
         <v>298</v>
       </c>
       <c r="E135" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F135" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="26" t="n">
+        <v>39028</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C136" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="E136" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F135" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="137" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AMG137" s="0"/>
-      <c r="AMH137" s="0"/>
-      <c r="AMI137" s="0"/>
-      <c r="AMJ137" s="0"/>
+      <c r="F136" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="138" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMG138" s="0"/>
+      <c r="AMH138" s="0"/>
+      <c r="AMI138" s="0"/>
+      <c r="AMJ138" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F135"/>
-  <conditionalFormatting sqref="F86:F1048576 F1:F84">
+  <autoFilter ref="A:F"/>
+  <conditionalFormatting sqref="F87:F1048576 F1:F85">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="resolved" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("resolved",F1)))</formula>
     </cfRule>
@@ -4618,131 +4648,132 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="#1766"/>
-    <hyperlink ref="B4" r:id="rId2" display="#274"/>
-    <hyperlink ref="B5" r:id="rId3" display="#273"/>
-    <hyperlink ref="B6" r:id="rId4" display="#272"/>
-    <hyperlink ref="B7" r:id="rId5" display="#1754"/>
-    <hyperlink ref="B8" r:id="rId6" display="#1752"/>
-    <hyperlink ref="B9" r:id="rId7" display="#1745"/>
-    <hyperlink ref="B10" r:id="rId8" display="#1743"/>
-    <hyperlink ref="B11" r:id="rId9" display="#1258"/>
-    <hyperlink ref="B12" r:id="rId10" display="#271"/>
-    <hyperlink ref="B13" r:id="rId11" display="#2"/>
-    <hyperlink ref="B14" r:id="rId12" display="#1349"/>
-    <hyperlink ref="B16" r:id="rId13" display="#1725"/>
-    <hyperlink ref="B17" r:id="rId14" display="#1724"/>
-    <hyperlink ref="B18" r:id="rId15" display="#1722"/>
-    <hyperlink ref="B19" r:id="rId16" display="#1226"/>
-    <hyperlink ref="B20" r:id="rId17" display="#1225"/>
-    <hyperlink ref="B21" r:id="rId18" display="#1720"/>
-    <hyperlink ref="B22" r:id="rId19" display="#1323"/>
-    <hyperlink ref="B23" r:id="rId20" display="#30"/>
-    <hyperlink ref="B24" r:id="rId21" display="#1712"/>
-    <hyperlink ref="B25" r:id="rId22" display="#1215"/>
-    <hyperlink ref="B26" r:id="rId23" display="#1214"/>
-    <hyperlink ref="B27" r:id="rId24" display="#1213"/>
-    <hyperlink ref="B28" r:id="rId25" display="#1212"/>
-    <hyperlink ref="B30" r:id="rId26" display="#1202"/>
-    <hyperlink ref="B31" r:id="rId27" display="#27"/>
-    <hyperlink ref="B32" r:id="rId28" display="#26"/>
-    <hyperlink ref="B33" r:id="rId29" display="#1201"/>
-    <hyperlink ref="B34" r:id="rId30" display="#1200"/>
-    <hyperlink ref="B35" r:id="rId31" display="#1708"/>
-    <hyperlink ref="B36" r:id="rId32" display="#1185"/>
-    <hyperlink ref="B37" r:id="rId33" display="#11"/>
-    <hyperlink ref="B38" r:id="rId34" display="#1309"/>
-    <hyperlink ref="B39" r:id="rId35" display="#1176"/>
-    <hyperlink ref="B40" r:id="rId36" display="#1171"/>
-    <hyperlink ref="B41" r:id="rId37" display="#1164"/>
-    <hyperlink ref="B42" r:id="rId38" display="#9"/>
-    <hyperlink ref="B43" r:id="rId39" display="#1163"/>
-    <hyperlink ref="B44" r:id="rId40" display="#1161"/>
-    <hyperlink ref="B45" r:id="rId41" display="#1690"/>
-    <hyperlink ref="B47" r:id="rId42" display="#1155"/>
-    <hyperlink ref="B48" r:id="rId43" display="#1150"/>
-    <hyperlink ref="B49" r:id="rId44" display="#1151"/>
-    <hyperlink ref="B50" r:id="rId45" display="#1200"/>
-    <hyperlink ref="B51" r:id="rId46" display="#1681"/>
-    <hyperlink ref="B52" r:id="rId47" display="#51"/>
-    <hyperlink ref="B53" r:id="rId48" display="#1142"/>
-    <hyperlink ref="B54" r:id="rId49" display="#8"/>
-    <hyperlink ref="B55" r:id="rId50" display="#1674"/>
-    <hyperlink ref="B56" r:id="rId51" display="#1672"/>
-    <hyperlink ref="B57" r:id="rId52" display="#1669"/>
-    <hyperlink ref="B58" r:id="rId53" display="#1670"/>
-    <hyperlink ref="B59" r:id="rId54" display="#1184"/>
-    <hyperlink ref="B60" r:id="rId55" display="#49"/>
-    <hyperlink ref="B61" r:id="rId56" display="#1140"/>
-    <hyperlink ref="B62" r:id="rId57" display="#1132"/>
-    <hyperlink ref="B64" r:id="rId58" display="#1125"/>
-    <hyperlink ref="B65" r:id="rId59" display="#1641"/>
-    <hyperlink ref="B66" r:id="rId60" display="#1124"/>
-    <hyperlink ref="B67" r:id="rId61" display="#1122"/>
-    <hyperlink ref="B68" r:id="rId62" display="#43"/>
-    <hyperlink ref="B69" r:id="rId63" display="#1622"/>
-    <hyperlink ref="B71" r:id="rId64" display="#38"/>
-    <hyperlink ref="B72" r:id="rId65" display="#1621"/>
-    <hyperlink ref="B73" r:id="rId66" display="#1616"/>
-    <hyperlink ref="B74" r:id="rId67" display="#37"/>
-    <hyperlink ref="B75" r:id="rId68" display="#36"/>
-    <hyperlink ref="B76" r:id="rId69" display="#1101"/>
-    <hyperlink ref="B77" r:id="rId70" display="#1099"/>
-    <hyperlink ref="B78" r:id="rId71" display="#1098"/>
-    <hyperlink ref="B79" r:id="rId72" display="#1617"/>
-    <hyperlink ref="B80" r:id="rId73" display="#1092"/>
-    <hyperlink ref="B81" r:id="rId74" display="#1128"/>
-    <hyperlink ref="B82" r:id="rId75" display="#1090"/>
-    <hyperlink ref="B83" r:id="rId76" display="#1608"/>
-    <hyperlink ref="B84" r:id="rId77" display="#35"/>
-    <hyperlink ref="B86" r:id="rId78" display="#1070"/>
-    <hyperlink ref="B87" r:id="rId79" display="#1592"/>
-    <hyperlink ref="B88" r:id="rId80" display="#1591"/>
-    <hyperlink ref="B89" r:id="rId81" display="#1578"/>
-    <hyperlink ref="B90" r:id="rId82" display="#41"/>
-    <hyperlink ref="B91" r:id="rId83" display="#42"/>
-    <hyperlink ref="B92" r:id="rId84" display="#1566"/>
-    <hyperlink ref="B93" r:id="rId85" display="#1565"/>
-    <hyperlink ref="B94" r:id="rId86" display="#1046"/>
-    <hyperlink ref="B95" r:id="rId87" display="#1559"/>
-    <hyperlink ref="B96" r:id="rId88" display="#1038"/>
-    <hyperlink ref="B97" r:id="rId89" display="#1037"/>
-    <hyperlink ref="B98" r:id="rId90" display="#1020"/>
-    <hyperlink ref="B99" r:id="rId91" display="#1032"/>
-    <hyperlink ref="B100" r:id="rId92" display="#1546"/>
-    <hyperlink ref="B101" r:id="rId93" display="#1027"/>
-    <hyperlink ref="B102" r:id="rId94" display="#1529"/>
-    <hyperlink ref="B104" r:id="rId95" display="#1527"/>
-    <hyperlink ref="B105" r:id="rId96" display="#558"/>
-    <hyperlink ref="B106" r:id="rId97" display="#1005"/>
-    <hyperlink ref="B107" r:id="rId98" display="#1020"/>
-    <hyperlink ref="B108" r:id="rId99" display="#993"/>
-    <hyperlink ref="B109" r:id="rId100" display="#1520"/>
-    <hyperlink ref="B110" r:id="rId101" display="#1519"/>
-    <hyperlink ref="B111" r:id="rId102" display="#969"/>
-    <hyperlink ref="B112" r:id="rId103" display="#1003"/>
-    <hyperlink ref="B113" r:id="rId104" display="#1015"/>
-    <hyperlink ref="B114" r:id="rId105" display="#1002"/>
-    <hyperlink ref="B115" r:id="rId106" display="#1471"/>
-    <hyperlink ref="B116" r:id="rId107" display="#1497"/>
-    <hyperlink ref="B117" r:id="rId108" display="#947"/>
-    <hyperlink ref="B118" r:id="rId109" display="#933"/>
-    <hyperlink ref="B119" r:id="rId110" display="#932"/>
-    <hyperlink ref="B120" r:id="rId111" display="#931"/>
-    <hyperlink ref="B121" r:id="rId112" display="#987"/>
-    <hyperlink ref="B122" r:id="rId113" display="#988"/>
-    <hyperlink ref="B123" r:id="rId114" display="#982"/>
-    <hyperlink ref="B124" r:id="rId115" display="#979"/>
-    <hyperlink ref="B125" r:id="rId116" display="#977"/>
-    <hyperlink ref="B126" r:id="rId117" display="#975"/>
-    <hyperlink ref="B127" r:id="rId118" display="#1445"/>
-    <hyperlink ref="B128" r:id="rId119" display="#1444"/>
-    <hyperlink ref="B129" r:id="rId120" display="#1427"/>
-    <hyperlink ref="B131" r:id="rId121" display="#23"/>
-    <hyperlink ref="B132" r:id="rId122" display="#22"/>
-    <hyperlink ref="B133" r:id="rId123" display="#18"/>
-    <hyperlink ref="B134" r:id="rId124" display="#1207"/>
-    <hyperlink ref="B135" r:id="rId125" display="#245"/>
+    <hyperlink ref="B3" r:id="rId1" display="#1768"/>
+    <hyperlink ref="B4" r:id="rId2" display="#1766"/>
+    <hyperlink ref="B5" r:id="rId3" display="#274"/>
+    <hyperlink ref="B6" r:id="rId4" display="#273"/>
+    <hyperlink ref="B7" r:id="rId5" display="#272"/>
+    <hyperlink ref="B8" r:id="rId6" display="#1754"/>
+    <hyperlink ref="B9" r:id="rId7" display="#1752"/>
+    <hyperlink ref="B10" r:id="rId8" display="#1745"/>
+    <hyperlink ref="B11" r:id="rId9" display="#1743"/>
+    <hyperlink ref="B12" r:id="rId10" display="#1258"/>
+    <hyperlink ref="B13" r:id="rId11" display="#271"/>
+    <hyperlink ref="B14" r:id="rId12" display="#2"/>
+    <hyperlink ref="B15" r:id="rId13" display="#1349"/>
+    <hyperlink ref="B17" r:id="rId14" display="#1725"/>
+    <hyperlink ref="B18" r:id="rId15" display="#1724"/>
+    <hyperlink ref="B19" r:id="rId16" display="#1722"/>
+    <hyperlink ref="B20" r:id="rId17" display="#1226"/>
+    <hyperlink ref="B21" r:id="rId18" display="#1225"/>
+    <hyperlink ref="B22" r:id="rId19" display="#1720"/>
+    <hyperlink ref="B23" r:id="rId20" display="#1323"/>
+    <hyperlink ref="B24" r:id="rId21" display="#30"/>
+    <hyperlink ref="B25" r:id="rId22" display="#1712"/>
+    <hyperlink ref="B26" r:id="rId23" display="#1215"/>
+    <hyperlink ref="B27" r:id="rId24" display="#1214"/>
+    <hyperlink ref="B28" r:id="rId25" display="#1213"/>
+    <hyperlink ref="B29" r:id="rId26" display="#1212"/>
+    <hyperlink ref="B31" r:id="rId27" display="#1202"/>
+    <hyperlink ref="B32" r:id="rId28" display="#27"/>
+    <hyperlink ref="B33" r:id="rId29" display="#26"/>
+    <hyperlink ref="B34" r:id="rId30" display="#1201"/>
+    <hyperlink ref="B35" r:id="rId31" display="#1200"/>
+    <hyperlink ref="B36" r:id="rId32" display="#1708"/>
+    <hyperlink ref="B37" r:id="rId33" display="#1185"/>
+    <hyperlink ref="B38" r:id="rId34" display="#11"/>
+    <hyperlink ref="B39" r:id="rId35" display="#1309"/>
+    <hyperlink ref="B40" r:id="rId36" display="#1176"/>
+    <hyperlink ref="B41" r:id="rId37" display="#1171"/>
+    <hyperlink ref="B42" r:id="rId38" display="#1164"/>
+    <hyperlink ref="B43" r:id="rId39" display="#9"/>
+    <hyperlink ref="B44" r:id="rId40" display="#1163"/>
+    <hyperlink ref="B45" r:id="rId41" display="#1161"/>
+    <hyperlink ref="B46" r:id="rId42" display="#1690"/>
+    <hyperlink ref="B48" r:id="rId43" display="#1155"/>
+    <hyperlink ref="B49" r:id="rId44" display="#1150"/>
+    <hyperlink ref="B50" r:id="rId45" display="#1151"/>
+    <hyperlink ref="B51" r:id="rId46" display="#1200"/>
+    <hyperlink ref="B52" r:id="rId47" display="#1681"/>
+    <hyperlink ref="B53" r:id="rId48" display="#51"/>
+    <hyperlink ref="B54" r:id="rId49" display="#1142"/>
+    <hyperlink ref="B55" r:id="rId50" display="#8"/>
+    <hyperlink ref="B56" r:id="rId51" display="#1674"/>
+    <hyperlink ref="B57" r:id="rId52" display="#1672"/>
+    <hyperlink ref="B58" r:id="rId53" display="#1669"/>
+    <hyperlink ref="B59" r:id="rId54" display="#1670"/>
+    <hyperlink ref="B60" r:id="rId55" display="#1184"/>
+    <hyperlink ref="B61" r:id="rId56" display="#49"/>
+    <hyperlink ref="B62" r:id="rId57" display="#1140"/>
+    <hyperlink ref="B63" r:id="rId58" display="#1132"/>
+    <hyperlink ref="B65" r:id="rId59" display="#1125"/>
+    <hyperlink ref="B66" r:id="rId60" display="#1641"/>
+    <hyperlink ref="B67" r:id="rId61" display="#1124"/>
+    <hyperlink ref="B68" r:id="rId62" display="#1122"/>
+    <hyperlink ref="B69" r:id="rId63" display="#43"/>
+    <hyperlink ref="B70" r:id="rId64" display="#1622"/>
+    <hyperlink ref="B72" r:id="rId65" display="#38"/>
+    <hyperlink ref="B73" r:id="rId66" display="#1621"/>
+    <hyperlink ref="B74" r:id="rId67" display="#1616"/>
+    <hyperlink ref="B75" r:id="rId68" display="#37"/>
+    <hyperlink ref="B76" r:id="rId69" display="#36"/>
+    <hyperlink ref="B77" r:id="rId70" display="#1101"/>
+    <hyperlink ref="B78" r:id="rId71" display="#1099"/>
+    <hyperlink ref="B79" r:id="rId72" display="#1098"/>
+    <hyperlink ref="B80" r:id="rId73" display="#1617"/>
+    <hyperlink ref="B81" r:id="rId74" display="#1092"/>
+    <hyperlink ref="B82" r:id="rId75" display="#1128"/>
+    <hyperlink ref="B83" r:id="rId76" display="#1090"/>
+    <hyperlink ref="B84" r:id="rId77" display="#1608"/>
+    <hyperlink ref="B85" r:id="rId78" display="#35"/>
+    <hyperlink ref="B87" r:id="rId79" display="#1070"/>
+    <hyperlink ref="B88" r:id="rId80" display="#1592"/>
+    <hyperlink ref="B89" r:id="rId81" display="#1591"/>
+    <hyperlink ref="B90" r:id="rId82" display="#1578"/>
+    <hyperlink ref="B91" r:id="rId83" display="#41"/>
+    <hyperlink ref="B92" r:id="rId84" display="#42"/>
+    <hyperlink ref="B93" r:id="rId85" display="#1566"/>
+    <hyperlink ref="B94" r:id="rId86" display="#1565"/>
+    <hyperlink ref="B95" r:id="rId87" display="#1046"/>
+    <hyperlink ref="B96" r:id="rId88" display="#1559"/>
+    <hyperlink ref="B97" r:id="rId89" display="#1038"/>
+    <hyperlink ref="B98" r:id="rId90" display="#1037"/>
+    <hyperlink ref="B99" r:id="rId91" display="#1020"/>
+    <hyperlink ref="B100" r:id="rId92" display="#1032"/>
+    <hyperlink ref="B101" r:id="rId93" display="#1546"/>
+    <hyperlink ref="B102" r:id="rId94" display="#1027"/>
+    <hyperlink ref="B103" r:id="rId95" display="#1529"/>
+    <hyperlink ref="B105" r:id="rId96" display="#1527"/>
+    <hyperlink ref="B106" r:id="rId97" display="#558"/>
+    <hyperlink ref="B107" r:id="rId98" display="#1005"/>
+    <hyperlink ref="B108" r:id="rId99" display="#1020"/>
+    <hyperlink ref="B109" r:id="rId100" display="#993"/>
+    <hyperlink ref="B110" r:id="rId101" display="#1520"/>
+    <hyperlink ref="B111" r:id="rId102" display="#1519"/>
+    <hyperlink ref="B112" r:id="rId103" display="#969"/>
+    <hyperlink ref="B113" r:id="rId104" display="#1003"/>
+    <hyperlink ref="B114" r:id="rId105" display="#1015"/>
+    <hyperlink ref="B115" r:id="rId106" display="#1002"/>
+    <hyperlink ref="B116" r:id="rId107" display="#1471"/>
+    <hyperlink ref="B117" r:id="rId108" display="#1497"/>
+    <hyperlink ref="B118" r:id="rId109" display="#947"/>
+    <hyperlink ref="B119" r:id="rId110" display="#933"/>
+    <hyperlink ref="B120" r:id="rId111" display="#932"/>
+    <hyperlink ref="B121" r:id="rId112" display="#931"/>
+    <hyperlink ref="B122" r:id="rId113" display="#987"/>
+    <hyperlink ref="B123" r:id="rId114" display="#988"/>
+    <hyperlink ref="B124" r:id="rId115" display="#982"/>
+    <hyperlink ref="B125" r:id="rId116" display="#979"/>
+    <hyperlink ref="B126" r:id="rId117" display="#977"/>
+    <hyperlink ref="B127" r:id="rId118" display="#975"/>
+    <hyperlink ref="B128" r:id="rId119" display="#1445"/>
+    <hyperlink ref="B129" r:id="rId120" display="#1444"/>
+    <hyperlink ref="B130" r:id="rId121" display="#1427"/>
+    <hyperlink ref="B132" r:id="rId122" display="#23"/>
+    <hyperlink ref="B133" r:id="rId123" display="#22"/>
+    <hyperlink ref="B134" r:id="rId124" display="#18"/>
+    <hyperlink ref="B135" r:id="rId125" display="#1207"/>
+    <hyperlink ref="B136" r:id="rId126" display="#245"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
@@ -4751,7 +4782,7 @@
     <oddHeader>&amp;C&amp;"Sans,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Sans,Regular"Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId126"/>
+  <drawing r:id="rId127"/>
 </worksheet>
 </file>
 
@@ -4784,10 +4815,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -4796,10 +4827,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added OmegaT bug ticket 1277
</commit_message>
<xml_diff>
--- a/docs/tools/tickets/OmegaT_issues_nopw.xlsx
+++ b/docs/tools/tickets/OmegaT_issues_nopw.xlsx
@@ -13,8 +13,8 @@
     <sheet name="ETS" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A:$F</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A$1:$F$136</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A$1:$F$137</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A:$F</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="true" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="307">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -118,6 +118,15 @@
     <t xml:space="preserve">WIP</t>
   </si>
   <si>
+    <t xml:space="preserve">#1277</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concurrency issue in COMPILE-triggered scripts in team projects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open!</t>
+  </si>
+  <si>
     <t xml:space="preserve">#1768</t>
   </si>
   <si>
@@ -125,9 +134,6 @@
   </si>
   <si>
     <t xml:space="preserve">RFE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open!</t>
   </si>
   <si>
     <t xml:space="preserve">#1766</t>
@@ -1716,14 +1722,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ138"/>
+  <dimension ref="A1:AMJ139"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1776,7 +1782,7 @@
     </row>
     <row r="3" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="n">
-        <v>45609</v>
+        <v>45629</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>30</v>
@@ -1788,10 +1794,10 @@
         <v>31</v>
       </c>
       <c r="E3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="AMG3" s="0"/>
       <c r="AMH3" s="0"/>
@@ -1800,46 +1806,46 @@
     </row>
     <row r="4" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="n">
-        <v>45604</v>
+        <v>45609</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="F4" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="AMG4" s="0"/>
       <c r="AMH4" s="0"/>
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="n">
-        <v>45563</v>
+        <v>45604</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>38</v>
-      </c>
       <c r="E5" s="11" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AMG5" s="0"/>
       <c r="AMH5" s="0"/>
@@ -1848,13 +1854,13 @@
     </row>
     <row r="6" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="n">
-        <v>45488</v>
+        <v>45563</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>37</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>40</v>
@@ -1863,55 +1869,55 @@
         <v>9</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AMG6" s="0"/>
       <c r="AMH6" s="0"/>
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" s="8" customFormat="true" ht="11.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="n">
+    <row r="7" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="n">
         <v>45488</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AMG7" s="0"/>
       <c r="AMH7" s="0"/>
       <c r="AMI7" s="0"/>
       <c r="AMJ7" s="0"/>
     </row>
-    <row r="8" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="8" customFormat="true" ht="11.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="n">
-        <v>45483</v>
+        <v>45488</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>43</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>44</v>
       </c>
       <c r="E8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="AMG8" s="0"/>
       <c r="AMH8" s="0"/>
@@ -1920,7 +1926,7 @@
     </row>
     <row r="9" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="n">
-        <v>45469</v>
+        <v>45483</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>45</v>
@@ -1932,10 +1938,10 @@
         <v>46</v>
       </c>
       <c r="E9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="AMG9" s="0"/>
       <c r="AMH9" s="0"/>
@@ -1944,22 +1950,22 @@
     </row>
     <row r="10" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="n">
-        <v>45784</v>
+        <v>45469</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="13" t="s">
+      <c r="E10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="AMG10" s="0"/>
       <c r="AMH10" s="0"/>
@@ -1968,7 +1974,7 @@
     </row>
     <row r="11" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="n">
-        <v>45411</v>
+        <v>45784</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>50</v>
@@ -1980,19 +1986,19 @@
         <v>51</v>
       </c>
       <c r="E11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="AMG11" s="0"/>
       <c r="AMH11" s="0"/>
       <c r="AMI11" s="0"/>
       <c r="AMJ11" s="0"/>
     </row>
-    <row r="12" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="n">
-        <v>45394</v>
+        <v>45411</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>52</v>
@@ -2004,10 +2010,10 @@
         <v>53</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>47</v>
+        <v>35</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="AMG12" s="0"/>
       <c r="AMH12" s="0"/>
@@ -2015,23 +2021,23 @@
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="n">
-        <v>45390</v>
+      <c r="A13" s="12" t="n">
+        <v>45394</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>55</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>56</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="14" t="s">
-        <v>57</v>
+      <c r="F13" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="AMG13" s="0"/>
       <c r="AMH13" s="0"/>
@@ -2040,22 +2046,22 @@
     </row>
     <row r="14" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="n">
-        <v>45365</v>
+        <v>45390</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>58</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>60</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>47</v>
+      <c r="F14" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="AMG14" s="0"/>
       <c r="AMH14" s="0"/>
@@ -2064,58 +2070,58 @@
     </row>
     <row r="15" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="n">
-        <v>45363</v>
+        <v>45365</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="13" t="s">
         <v>62</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AMG15" s="0"/>
       <c r="AMH15" s="0"/>
       <c r="AMI15" s="0"/>
       <c r="AMJ15" s="0"/>
     </row>
-    <row r="16" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
+    <row r="16" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9" t="n">
+        <v>45363</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>29</v>
+      <c r="C16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="AMG16" s="0"/>
       <c r="AMH16" s="0"/>
       <c r="AMI16" s="0"/>
       <c r="AMJ16" s="0"/>
     </row>
-    <row r="17" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="n">
-        <v>45238</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="13" t="s">
+    <row r="17" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>33</v>
+      <c r="F17" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="AMG17" s="0"/>
       <c r="AMH17" s="0"/>
@@ -2124,7 +2130,7 @@
     </row>
     <row r="18" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="n">
-        <v>45230</v>
+        <v>45238</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>66</v>
@@ -2132,14 +2138,14 @@
       <c r="C18" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="13" t="s">
         <v>67</v>
       </c>
       <c r="E18" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>33</v>
       </c>
       <c r="AMG18" s="0"/>
       <c r="AMH18" s="0"/>
@@ -2148,7 +2154,7 @@
     </row>
     <row r="19" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="n">
-        <v>45223</v>
+        <v>45230</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>68</v>
@@ -2160,10 +2166,10 @@
         <v>69</v>
       </c>
       <c r="E19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="AMG19" s="0"/>
       <c r="AMH19" s="0"/>
@@ -2172,7 +2178,7 @@
     </row>
     <row r="20" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="n">
-        <v>45236</v>
+        <v>45223</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>70</v>
@@ -2184,10 +2190,10 @@
         <v>71</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>72</v>
+        <v>35</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="AMG20" s="0"/>
       <c r="AMH20" s="0"/>
@@ -2196,22 +2202,22 @@
     </row>
     <row r="21" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="n">
-        <v>45233</v>
+        <v>45236</v>
       </c>
       <c r="B21" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="14" t="s">
-        <v>33</v>
+      <c r="F21" s="15" t="s">
+        <v>74</v>
       </c>
       <c r="AMG21" s="0"/>
       <c r="AMH21" s="0"/>
@@ -2220,7 +2226,7 @@
     </row>
     <row r="22" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="n">
-        <v>45213</v>
+        <v>45233</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>75</v>
@@ -2232,10 +2238,10 @@
         <v>76</v>
       </c>
       <c r="E22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="AMG22" s="0"/>
       <c r="AMH22" s="0"/>
@@ -2244,22 +2250,22 @@
     </row>
     <row r="23" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="n">
-        <v>45199</v>
+        <v>45213</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>77</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>78</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AMG23" s="0"/>
       <c r="AMH23" s="0"/>
@@ -2268,22 +2274,22 @@
     </row>
     <row r="24" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="n">
-        <v>45170</v>
+        <v>45199</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>79</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>80</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AMG24" s="0"/>
       <c r="AMH24" s="0"/>
@@ -2292,7 +2298,7 @@
     </row>
     <row r="25" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="n">
-        <v>45169</v>
+        <v>45170</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>81</v>
@@ -2304,10 +2310,10 @@
         <v>82</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AMG25" s="0"/>
       <c r="AMH25" s="0"/>
@@ -2315,23 +2321,23 @@
       <c r="AMJ25" s="0"/>
     </row>
     <row r="26" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="16" t="n">
+      <c r="A26" s="9" t="n">
         <v>45169</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="18" t="s">
+      <c r="C26" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="11" t="s">
         <v>84</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="AMG26" s="0"/>
       <c r="AMH26" s="0"/>
@@ -2340,7 +2346,7 @@
     </row>
     <row r="27" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="16" t="n">
-        <v>45145</v>
+        <v>45169</v>
       </c>
       <c r="B27" s="17" t="s">
         <v>85</v>
@@ -2349,7 +2355,7 @@
         <v>7</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="E27" s="18" t="s">
         <v>9</v>
@@ -2363,23 +2369,23 @@
       <c r="AMJ27" s="0"/>
     </row>
     <row r="28" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="n">
+      <c r="A28" s="16" t="n">
         <v>45145</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="11" t="s">
+      <c r="C28" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="18" t="s">
         <v>88</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>57</v>
       </c>
       <c r="AMG28" s="0"/>
       <c r="AMH28" s="0"/>
@@ -2403,37 +2409,40 @@
         <v>9</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AMG29" s="0"/>
       <c r="AMH29" s="0"/>
       <c r="AMI29" s="0"/>
       <c r="AMJ29" s="0"/>
     </row>
-    <row r="30" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="n">
-        <v>45112</v>
+        <v>45145</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="F30" s="20" t="s">
-        <v>57</v>
+        <v>92</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="AMG30" s="0"/>
       <c r="AMH30" s="0"/>
       <c r="AMI30" s="0"/>
       <c r="AMJ30" s="0"/>
     </row>
-    <row r="31" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="n">
-        <v>45124</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>92</v>
+        <v>45112</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>7</v>
@@ -2441,11 +2450,8 @@
       <c r="D31" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E31" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>33</v>
+      <c r="F31" s="20" t="s">
+        <v>59</v>
       </c>
       <c r="AMG31" s="0"/>
       <c r="AMH31" s="0"/>
@@ -2454,22 +2460,22 @@
     </row>
     <row r="32" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="n">
-        <v>45119</v>
+        <v>45124</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>94</v>
       </c>
       <c r="C32" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D32" s="11" t="s">
-        <v>96</v>
-      </c>
       <c r="E32" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>33</v>
       </c>
       <c r="AMG32" s="0"/>
       <c r="AMH32" s="0"/>
@@ -2481,19 +2487,19 @@
         <v>45119</v>
       </c>
       <c r="B33" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>97</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>95</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>98</v>
       </c>
       <c r="E33" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>33</v>
       </c>
       <c r="AMG33" s="0"/>
       <c r="AMH33" s="0"/>
@@ -2502,22 +2508,22 @@
     </row>
     <row r="34" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="n">
-        <v>45118</v>
+        <v>45119</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>99</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>100</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AMG34" s="0"/>
       <c r="AMH34" s="0"/>
@@ -2541,7 +2547,7 @@
         <v>9</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AMG35" s="0"/>
       <c r="AMH35" s="0"/>
@@ -2550,7 +2556,7 @@
     </row>
     <row r="36" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="n">
-        <v>45110</v>
+        <v>45118</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>103</v>
@@ -2562,10 +2568,10 @@
         <v>104</v>
       </c>
       <c r="E36" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="AMG36" s="0"/>
       <c r="AMH36" s="0"/>
@@ -2574,7 +2580,7 @@
     </row>
     <row r="37" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="n">
-        <v>45104</v>
+        <v>45110</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>105</v>
@@ -2586,49 +2592,49 @@
         <v>106</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="21" t="s">
-        <v>107</v>
+        <v>35</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="AMG37" s="0"/>
       <c r="AMH37" s="0"/>
       <c r="AMI37" s="0"/>
       <c r="AMJ37" s="0"/>
     </row>
-    <row r="38" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="n">
-        <v>45094</v>
+        <v>45104</v>
       </c>
       <c r="B38" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="11" t="s">
         <v>108</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>110</v>
       </c>
       <c r="E38" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F38" s="20" t="s">
-        <v>57</v>
+      <c r="F38" s="21" t="s">
+        <v>109</v>
       </c>
       <c r="AMG38" s="0"/>
       <c r="AMH38" s="0"/>
       <c r="AMI38" s="0"/>
       <c r="AMJ38" s="0"/>
     </row>
-    <row r="39" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="n">
-        <v>45069</v>
+        <v>45094</v>
       </c>
       <c r="B39" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="11" t="s">
         <v>111</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>13</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>112</v>
@@ -2636,41 +2642,41 @@
       <c r="E39" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F39" s="22" t="s">
-        <v>113</v>
+      <c r="F39" s="20" t="s">
+        <v>59</v>
       </c>
       <c r="AMG39" s="0"/>
       <c r="AMH39" s="0"/>
       <c r="AMI39" s="0"/>
       <c r="AMJ39" s="0"/>
     </row>
-    <row r="40" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="n">
         <v>45069</v>
       </c>
       <c r="B40" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="11" t="s">
         <v>114</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>115</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F40" s="20" t="s">
-        <v>57</v>
+      <c r="F40" s="22" t="s">
+        <v>115</v>
       </c>
       <c r="AMG40" s="0"/>
       <c r="AMH40" s="0"/>
       <c r="AMI40" s="0"/>
       <c r="AMJ40" s="0"/>
     </row>
-    <row r="41" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="n">
-        <v>45064</v>
+        <v>45069</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>116</v>
@@ -2684,17 +2690,17 @@
       <c r="E41" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F41" s="11" t="s">
-        <v>47</v>
+      <c r="F41" s="20" t="s">
+        <v>59</v>
       </c>
       <c r="AMG41" s="0"/>
       <c r="AMH41" s="0"/>
       <c r="AMI41" s="0"/>
       <c r="AMJ41" s="0"/>
     </row>
-    <row r="42" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="n">
-        <v>45049</v>
+        <v>45064</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>118</v>
@@ -2708,8 +2714,8 @@
       <c r="E42" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F42" s="23" t="s">
-        <v>57</v>
+      <c r="F42" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="AMG42" s="0"/>
       <c r="AMH42" s="0"/>
@@ -2723,17 +2729,17 @@
       <c r="B43" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="C43" s="24" t="s">
-        <v>109</v>
+      <c r="C43" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>121</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F43" s="20" t="s">
-        <v>57</v>
+        <v>9</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>59</v>
       </c>
       <c r="AMG43" s="0"/>
       <c r="AMH43" s="0"/>
@@ -2742,31 +2748,31 @@
     </row>
     <row r="44" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="n">
-        <v>45044</v>
+        <v>45049</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C44" s="11" t="s">
-        <v>7</v>
+      <c r="C44" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D44" s="11" t="s">
         <v>123</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AMG44" s="0"/>
       <c r="AMH44" s="0"/>
       <c r="AMI44" s="0"/>
       <c r="AMJ44" s="0"/>
     </row>
-    <row r="45" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="n">
-        <v>45040</v>
+        <v>45044</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>124</v>
@@ -2780,17 +2786,17 @@
       <c r="E45" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F45" s="11" t="s">
-        <v>47</v>
+      <c r="F45" s="20" t="s">
+        <v>59</v>
       </c>
       <c r="AMG45" s="0"/>
       <c r="AMH45" s="0"/>
       <c r="AMI45" s="0"/>
       <c r="AMJ45" s="0"/>
     </row>
-    <row r="46" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="n">
-        <v>45028</v>
+        <v>45040</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>126</v>
@@ -2802,10 +2808,10 @@
         <v>127</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F46" s="20" t="s">
-        <v>57</v>
+        <v>9</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="AMG46" s="0"/>
       <c r="AMH46" s="0"/>
@@ -2814,16 +2820,22 @@
     </row>
     <row r="47" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="n">
-        <v>44996</v>
+        <v>45028</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>128</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>128</v>
+        <v>129</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AMG47" s="0"/>
       <c r="AMH47" s="0"/>
@@ -2832,31 +2844,25 @@
     </row>
     <row r="48" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="n">
-        <v>45007</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>129</v>
+        <v>44996</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="D48" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="E48" s="11" t="s">
-        <v>9</v>
-      </c>
       <c r="F48" s="20" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AMG48" s="0"/>
       <c r="AMH48" s="0"/>
       <c r="AMI48" s="0"/>
       <c r="AMJ48" s="0"/>
     </row>
-    <row r="49" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="n">
-        <v>44993</v>
+        <v>45007</v>
       </c>
       <c r="B49" s="10" t="s">
         <v>131</v>
@@ -2870,8 +2876,8 @@
       <c r="E49" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F49" s="21" t="s">
-        <v>107</v>
+      <c r="F49" s="20" t="s">
+        <v>59</v>
       </c>
       <c r="AMG49" s="0"/>
       <c r="AMH49" s="0"/>
@@ -2895,7 +2901,7 @@
         <v>9</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AMG50" s="0"/>
       <c r="AMH50" s="0"/>
@@ -2904,22 +2910,22 @@
     </row>
     <row r="51" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="n">
-        <v>44991</v>
+        <v>44993</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F51" s="11" t="s">
-        <v>136</v>
+      <c r="F51" s="21" t="s">
+        <v>109</v>
       </c>
       <c r="AMG51" s="0"/>
       <c r="AMH51" s="0"/>
@@ -2928,22 +2934,22 @@
     </row>
     <row r="52" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="n">
-        <v>44981</v>
+        <v>44991</v>
       </c>
       <c r="B52" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="C52" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="11" t="s">
+      <c r="E52" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="11" t="s">
         <v>138</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F52" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="AMG52" s="0"/>
       <c r="AMH52" s="0"/>
@@ -2952,22 +2958,22 @@
     </row>
     <row r="53" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="n">
-        <v>44973</v>
+        <v>44981</v>
       </c>
       <c r="B53" s="10" t="s">
         <v>139</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="D53" s="11" t="s">
         <v>140</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="25" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="AMG53" s="0"/>
       <c r="AMH53" s="0"/>
@@ -2975,47 +2981,47 @@
       <c r="AMJ53" s="0"/>
     </row>
     <row r="54" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="16" t="n">
-        <v>44972</v>
-      </c>
-      <c r="B54" s="17" t="s">
+      <c r="A54" s="9" t="n">
+        <v>44973</v>
+      </c>
+      <c r="B54" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C54" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="E54" s="18" t="s">
+      <c r="C54" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="E54" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F54" s="18" t="s">
-        <v>84</v>
+      <c r="F54" s="25" t="s">
+        <v>32</v>
       </c>
       <c r="AMG54" s="0"/>
       <c r="AMH54" s="0"/>
       <c r="AMI54" s="0"/>
       <c r="AMJ54" s="0"/>
     </row>
-    <row r="55" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="26" t="n">
-        <v>44970</v>
-      </c>
-      <c r="B55" s="27" t="s">
+    <row r="55" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="16" t="n">
+        <v>44972</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C55" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="D55" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="E55" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F55" s="24" t="s">
-        <v>47</v>
+      <c r="E55" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="18" t="s">
+        <v>86</v>
       </c>
       <c r="AMG55" s="0"/>
       <c r="AMH55" s="0"/>
@@ -3024,22 +3030,22 @@
     </row>
     <row r="56" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="26" t="n">
-        <v>44967</v>
+        <v>44970</v>
       </c>
       <c r="B56" s="27" t="s">
         <v>144</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="D56" s="24" t="s">
         <v>145</v>
       </c>
       <c r="E56" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F56" s="14" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="F56" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="AMG56" s="0"/>
       <c r="AMH56" s="0"/>
@@ -3048,7 +3054,7 @@
     </row>
     <row r="57" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="26" t="n">
-        <v>44964</v>
+        <v>44967</v>
       </c>
       <c r="B57" s="27" t="s">
         <v>146</v>
@@ -3060,10 +3066,10 @@
         <v>147</v>
       </c>
       <c r="E57" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F57" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="F57" s="21" t="s">
-        <v>107</v>
       </c>
       <c r="AMG57" s="0"/>
       <c r="AMH57" s="0"/>
@@ -3072,7 +3078,7 @@
     </row>
     <row r="58" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="26" t="n">
-        <v>44952</v>
+        <v>44964</v>
       </c>
       <c r="B58" s="27" t="s">
         <v>148</v>
@@ -3084,10 +3090,10 @@
         <v>149</v>
       </c>
       <c r="E58" s="24" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F58" s="21" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AMG58" s="0"/>
       <c r="AMH58" s="0"/>
@@ -3108,10 +3114,10 @@
         <v>151</v>
       </c>
       <c r="E59" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F59" s="20" t="s">
-        <v>57</v>
+        <v>35</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>109</v>
       </c>
       <c r="AMG59" s="0"/>
       <c r="AMH59" s="0"/>
@@ -3119,23 +3125,23 @@
       <c r="AMJ59" s="0"/>
     </row>
     <row r="60" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="28" t="n">
-        <v>44949</v>
-      </c>
-      <c r="B60" s="29" t="s">
+      <c r="A60" s="26" t="n">
+        <v>44952</v>
+      </c>
+      <c r="B60" s="27" t="s">
         <v>152</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D60" s="24" t="s">
         <v>153</v>
       </c>
       <c r="E60" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F60" s="14" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>59</v>
       </c>
       <c r="AMG60" s="0"/>
       <c r="AMH60" s="0"/>
@@ -3143,23 +3149,23 @@
       <c r="AMJ60" s="0"/>
     </row>
     <row r="61" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="26" t="n">
-        <v>44948</v>
-      </c>
-      <c r="B61" s="27" t="s">
+      <c r="A61" s="28" t="n">
+        <v>44949</v>
+      </c>
+      <c r="B61" s="29" t="s">
         <v>154</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="D61" s="24" t="s">
         <v>155</v>
       </c>
       <c r="E61" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="F61" s="20" t="s">
-        <v>57</v>
       </c>
       <c r="AMG61" s="0"/>
       <c r="AMH61" s="0"/>
@@ -3168,58 +3174,70 @@
     </row>
     <row r="62" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="26" t="n">
-        <v>44946</v>
+        <v>44948</v>
       </c>
       <c r="B62" s="27" t="s">
         <v>156</v>
       </c>
       <c r="C62" s="24" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="D62" s="24" t="s">
         <v>157</v>
       </c>
       <c r="E62" s="24" t="s">
-        <v>158</v>
+        <v>35</v>
       </c>
       <c r="F62" s="20" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AMG62" s="0"/>
       <c r="AMH62" s="0"/>
       <c r="AMI62" s="0"/>
       <c r="AMJ62" s="0"/>
     </row>
-    <row r="63" s="24" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="26" t="n">
-        <v>44929</v>
-      </c>
-      <c r="B63" s="30" t="s">
+        <v>44946</v>
+      </c>
+      <c r="B63" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="C63" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="C63" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D63" s="24" t="s">
+      <c r="E63" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="E63" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="F63" s="14" t="s">
-        <v>33</v>
+      <c r="F63" s="20" t="s">
+        <v>59</v>
       </c>
       <c r="AMG63" s="0"/>
       <c r="AMH63" s="0"/>
       <c r="AMI63" s="0"/>
       <c r="AMJ63" s="0"/>
     </row>
-    <row r="64" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="8" t="s">
+    <row r="64" s="24" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="26" t="n">
+        <v>44929</v>
+      </c>
+      <c r="B64" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="F64" s="8" t="s">
-        <v>29</v>
+      <c r="C64" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="E64" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="AMG64" s="0"/>
       <c r="AMH64" s="0"/>
@@ -3227,71 +3245,59 @@
       <c r="AMJ64" s="0"/>
     </row>
     <row r="65" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="26" t="n">
-        <v>44879</v>
-      </c>
-      <c r="B65" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D65" s="5" t="s">
+      <c r="A65" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E65" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>47</v>
+      <c r="F65" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="AMG65" s="0"/>
       <c r="AMH65" s="0"/>
       <c r="AMI65" s="0"/>
       <c r="AMJ65" s="0"/>
     </row>
-    <row r="66" s="24" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="26" t="n">
-        <v>44858</v>
-      </c>
-      <c r="B66" s="27" t="s">
+        <v>44879</v>
+      </c>
+      <c r="B66" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="C66" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D66" s="24" t="s">
+      <c r="C66" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="E66" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F66" s="24" t="s">
-        <v>47</v>
+      <c r="E66" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="AMG66" s="0"/>
       <c r="AMH66" s="0"/>
       <c r="AMI66" s="0"/>
       <c r="AMJ66" s="0"/>
     </row>
-    <row r="67" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" s="24" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="26" t="n">
-        <v>44855</v>
-      </c>
-      <c r="B67" s="31" t="s">
+        <v>44858</v>
+      </c>
+      <c r="B67" s="27" t="s">
         <v>166</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D67" s="5" t="s">
+      <c r="C67" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="E67" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F67" s="21" t="s">
-        <v>107</v>
+      <c r="E67" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F67" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="AMG67" s="0"/>
       <c r="AMH67" s="0"/>
@@ -3300,7 +3306,7 @@
     </row>
     <row r="68" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="26" t="n">
-        <v>44844</v>
+        <v>44855</v>
       </c>
       <c r="B68" s="31" t="s">
         <v>168</v>
@@ -3312,113 +3318,117 @@
         <v>169</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>170</v>
+        <v>160</v>
+      </c>
+      <c r="F68" s="21" t="s">
+        <v>109</v>
       </c>
       <c r="AMG68" s="0"/>
       <c r="AMH68" s="0"/>
       <c r="AMI68" s="0"/>
       <c r="AMJ68" s="0"/>
     </row>
-    <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="26" t="n">
-        <v>44757</v>
-      </c>
-      <c r="B69" s="32" t="s">
+        <v>44844</v>
+      </c>
+      <c r="B69" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C69" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D69" s="5" t="s">
+      <c r="E69" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F69" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="E69" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F69" s="20" t="s">
-        <v>57</v>
-      </c>
+      <c r="AMG69" s="0"/>
+      <c r="AMH69" s="0"/>
+      <c r="AMI69" s="0"/>
+      <c r="AMJ69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="26" t="n">
-        <v>373466</v>
-      </c>
-      <c r="B70" s="31" t="s">
+        <v>44757</v>
+      </c>
+      <c r="B70" s="32" t="s">
         <v>173</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>174</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>47</v>
+        <v>160</v>
+      </c>
+      <c r="F70" s="20" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="26" t="n">
-        <v>44743</v>
+        <v>373466</v>
+      </c>
+      <c r="B71" s="31" t="s">
+        <v>175</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="F71" s="20" t="s">
-        <v>57</v>
+        <v>176</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="26" t="n">
-        <v>44740</v>
-      </c>
-      <c r="B72" s="33" t="s">
-        <v>176</v>
+        <v>44743</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="E72" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F72" s="14" t="s">
-        <v>33</v>
+      <c r="F72" s="20" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="26" t="n">
-        <v>44739</v>
-      </c>
-      <c r="B73" s="34" t="s">
+        <v>44740</v>
+      </c>
+      <c r="B73" s="33" t="s">
         <v>178</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>179</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>23</v>
+        <v>160</v>
       </c>
       <c r="F73" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="26" t="n">
-        <v>44693</v>
+        <v>44739</v>
       </c>
       <c r="B74" s="34" t="s">
         <v>180</v>
@@ -3430,77 +3440,77 @@
         <v>181</v>
       </c>
       <c r="E74" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F74" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="F74" s="14" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="26" t="n">
-        <v>44695</v>
-      </c>
-      <c r="B75" s="35" t="s">
+        <v>44693</v>
+      </c>
+      <c r="B75" s="34" t="s">
         <v>182</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F75" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F75" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="26" t="n">
+        <v>44695</v>
+      </c>
+      <c r="B76" s="35" t="s">
+        <v>184</v>
+      </c>
+      <c r="C76" s="5" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="28" t="n">
-        <v>44659</v>
-      </c>
-      <c r="B76" s="36" t="s">
-        <v>184</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>185</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F76" s="14" t="s">
-        <v>33</v>
+        <v>160</v>
+      </c>
+      <c r="F76" s="20" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="26" t="n">
-        <v>44712</v>
-      </c>
-      <c r="B77" s="34" t="s">
+      <c r="A77" s="28" t="n">
+        <v>44659</v>
+      </c>
+      <c r="B77" s="36" t="s">
         <v>186</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>187</v>
       </c>
       <c r="E77" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F77" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="26" t="n">
-        <v>44705</v>
-      </c>
-      <c r="B78" s="31" t="s">
+        <v>44712</v>
+      </c>
+      <c r="B78" s="34" t="s">
         <v>188</v>
       </c>
       <c r="C78" s="5" t="s">
@@ -3510,10 +3520,10 @@
         <v>189</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F78" s="20" t="s">
-        <v>57</v>
+        <v>35</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3530,15 +3540,15 @@
         <v>191</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F79" s="20" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="26" t="n">
-        <v>44693</v>
+        <v>44705</v>
       </c>
       <c r="B80" s="31" t="s">
         <v>192</v>
@@ -3550,15 +3560,15 @@
         <v>193</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>47</v>
+        <v>160</v>
+      </c>
+      <c r="F80" s="20" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="26" t="n">
-        <v>44622</v>
+        <v>44693</v>
       </c>
       <c r="B81" s="31" t="s">
         <v>194</v>
@@ -3570,57 +3580,57 @@
         <v>195</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F81" s="20" t="s">
-        <v>57</v>
+        <v>35</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="26" t="n">
-        <v>44614</v>
+        <v>44622</v>
       </c>
       <c r="B82" s="31" t="s">
         <v>196</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>197</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F82" s="14" t="s">
-        <v>33</v>
+        <v>160</v>
+      </c>
+      <c r="F82" s="20" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="26" t="n">
-        <v>44613</v>
+        <v>44614</v>
       </c>
       <c r="B83" s="31" t="s">
         <v>198</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>199</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>47</v>
+        <v>160</v>
+      </c>
+      <c r="F83" s="14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="26" t="n">
-        <v>44608</v>
-      </c>
-      <c r="B84" s="34" t="s">
+        <v>44613</v>
+      </c>
+      <c r="B84" s="31" t="s">
         <v>200</v>
       </c>
       <c r="C84" s="5" t="s">
@@ -3630,60 +3640,60 @@
         <v>201</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F84" s="20" t="s">
-        <v>57</v>
+        <v>160</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="26" t="n">
-        <v>44580</v>
-      </c>
-      <c r="B85" s="31" t="s">
+        <v>44608</v>
+      </c>
+      <c r="B85" s="34" t="s">
         <v>202</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>203</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F85" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="26" t="n">
+        <v>44580</v>
+      </c>
+      <c r="B86" s="31" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="26" t="n">
-        <v>44463</v>
-      </c>
-      <c r="B87" s="31" t="s">
+      <c r="C86" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D86" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C87" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D87" s="5" t="s">
+      <c r="E86" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="5" t="s">
         <v>206</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="26" t="n">
-        <v>44460</v>
+        <v>44463</v>
       </c>
       <c r="B88" s="31" t="s">
         <v>207</v>
@@ -3695,10 +3705,10 @@
         <v>208</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>32</v>
+        <v>160</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>209</v>
+        <v>49</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3706,24 +3716,24 @@
         <v>44460</v>
       </c>
       <c r="B89" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D89" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C89" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D89" s="5" t="s">
+      <c r="E89" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F89" s="5" t="s">
         <v>211</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F89" s="20" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="26" t="n">
-        <v>44372</v>
+        <v>44460</v>
       </c>
       <c r="B90" s="31" t="s">
         <v>212</v>
@@ -3737,73 +3747,73 @@
       <c r="E90" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F90" s="5" t="s">
-        <v>47</v>
+      <c r="F90" s="20" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="26" t="n">
-        <v>44326</v>
+        <v>44372</v>
       </c>
       <c r="B91" s="31" t="s">
         <v>214</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>215</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>158</v>
+        <v>23</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>170</v>
+        <v>49</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="28" t="n">
-        <v>44325</v>
-      </c>
-      <c r="B92" s="37" t="s">
+      <c r="A92" s="26" t="n">
+        <v>44326</v>
+      </c>
+      <c r="B92" s="31" t="s">
         <v>216</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>217</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F92" s="14" t="s">
-        <v>33</v>
+        <v>160</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="26" t="n">
+      <c r="A93" s="28" t="n">
         <v>44325</v>
       </c>
-      <c r="B93" s="31" t="s">
+      <c r="B93" s="37" t="s">
         <v>218</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="D93" s="5" t="s">
         <v>219</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F93" s="5" t="s">
-        <v>47</v>
+        <v>160</v>
+      </c>
+      <c r="F93" s="14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="26" t="n">
-        <v>44321</v>
+        <v>44325</v>
       </c>
       <c r="B94" s="31" t="s">
         <v>220</v>
@@ -3815,15 +3825,15 @@
         <v>221</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F94" s="21" t="s">
-        <v>107</v>
+        <v>23</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="26" t="n">
-        <v>44316</v>
+        <v>44321</v>
       </c>
       <c r="B95" s="31" t="s">
         <v>222</v>
@@ -3835,37 +3845,37 @@
         <v>223</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F95" s="5" t="s">
-        <v>224</v>
+        <v>35</v>
+      </c>
+      <c r="F95" s="21" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="26" t="n">
-        <v>44279</v>
-      </c>
-      <c r="B96" s="5" t="s">
+        <v>44316</v>
+      </c>
+      <c r="B96" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D96" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="C96" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D96" s="5" t="s">
+      <c r="E96" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F96" s="5" t="s">
         <v>226</v>
-      </c>
-      <c r="E96" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F96" s="14" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="26" t="n">
-        <v>44257</v>
-      </c>
-      <c r="B97" s="31" t="s">
+        <v>44279</v>
+      </c>
+      <c r="B97" s="5" t="s">
         <v>227</v>
       </c>
       <c r="C97" s="5" t="s">
@@ -3875,15 +3885,15 @@
         <v>228</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F97" s="5" t="s">
-        <v>47</v>
+        <v>23</v>
+      </c>
+      <c r="F97" s="14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="26" t="n">
-        <v>44243</v>
+        <v>44257</v>
       </c>
       <c r="B98" s="31" t="s">
         <v>229</v>
@@ -3895,57 +3905,57 @@
         <v>230</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="38" t="n">
+      <c r="A99" s="26" t="n">
+        <v>44243</v>
+      </c>
+      <c r="B99" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="38" t="n">
         <v>44231</v>
       </c>
-      <c r="B99" s="39" t="s">
-        <v>231</v>
-      </c>
-      <c r="C99" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D99" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="E99" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="F99" s="40" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="26" t="n">
-        <v>44218</v>
-      </c>
-      <c r="B100" s="31" t="s">
-        <v>232</v>
-      </c>
-      <c r="C100" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D100" s="5" t="s">
+      <c r="B100" s="39" t="s">
         <v>233</v>
       </c>
-      <c r="E100" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F100" s="5" t="s">
-        <v>47</v>
+      <c r="C100" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="E100" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="F100" s="40" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="26" t="n">
-        <v>44216</v>
-      </c>
-      <c r="B101" s="34" t="s">
+        <v>44218</v>
+      </c>
+      <c r="B101" s="31" t="s">
         <v>234</v>
       </c>
       <c r="C101" s="5" t="s">
@@ -3955,17 +3965,17 @@
         <v>235</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F101" s="14" t="s">
-        <v>33</v>
+        <v>160</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="26" t="n">
-        <v>44175</v>
-      </c>
-      <c r="B102" s="31" t="s">
+        <v>44216</v>
+      </c>
+      <c r="B102" s="34" t="s">
         <v>236</v>
       </c>
       <c r="C102" s="5" t="s">
@@ -3975,10 +3985,10 @@
         <v>237</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F102" s="5" t="s">
-        <v>47</v>
+        <v>23</v>
+      </c>
+      <c r="F102" s="14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3995,40 +4005,40 @@
         <v>239</v>
       </c>
       <c r="E103" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="26" t="n">
+        <v>44175</v>
+      </c>
+      <c r="B104" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E104" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F103" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="26" t="n">
-        <v>44162</v>
-      </c>
-      <c r="B105" s="31" t="s">
-        <v>240</v>
-      </c>
-      <c r="C105" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D105" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F105" s="5" t="s">
-        <v>47</v>
+      <c r="F104" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="26" t="n">
-        <v>44148</v>
+        <v>44162</v>
       </c>
       <c r="B106" s="31" t="s">
         <v>242</v>
@@ -4037,158 +4047,158 @@
         <v>7</v>
       </c>
       <c r="D106" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="26" t="n">
+        <v>44148</v>
+      </c>
+      <c r="B107" s="31" t="s">
+        <v>244</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D107" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E106" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F106" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="38" t="n">
+      <c r="E107" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="38" t="n">
         <v>44146</v>
       </c>
-      <c r="B107" s="39" t="s">
-        <v>243</v>
-      </c>
-      <c r="C107" s="40" t="s">
+      <c r="B108" s="39" t="s">
+        <v>245</v>
+      </c>
+      <c r="C108" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D107" s="40" t="s">
-        <v>244</v>
-      </c>
-      <c r="E107" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="F107" s="40" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="26" t="n">
-        <v>44132</v>
-      </c>
-      <c r="B108" s="31" t="s">
-        <v>231</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D108" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="E108" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F108" s="5" t="s">
-        <v>47</v>
+      <c r="D108" s="40" t="s">
+        <v>246</v>
+      </c>
+      <c r="E108" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="F108" s="40" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="26" t="n">
-        <v>44103</v>
+        <v>44132</v>
       </c>
       <c r="B109" s="31" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>247</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="38" t="n">
+      <c r="A110" s="26" t="n">
+        <v>44103</v>
+      </c>
+      <c r="B110" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E110" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="38" t="n">
         <v>44095</v>
       </c>
-      <c r="B110" s="39" t="s">
-        <v>248</v>
-      </c>
-      <c r="C110" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D110" s="40" t="s">
-        <v>249</v>
-      </c>
-      <c r="E110" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F110" s="40" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="26" t="n">
-        <v>44095</v>
-      </c>
-      <c r="B111" s="31" t="s">
+      <c r="B111" s="39" t="s">
         <v>250</v>
       </c>
-      <c r="C111" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D111" s="5" t="s">
+      <c r="C111" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D111" s="40" t="s">
         <v>251</v>
       </c>
-      <c r="E111" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F111" s="20" t="s">
-        <v>57</v>
+      <c r="E111" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="F111" s="40" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="26" t="n">
-        <v>44057</v>
+        <v>44095</v>
       </c>
       <c r="B112" s="31" t="s">
         <v>252</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>253</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F112" s="5" t="s">
-        <v>209</v>
+        <v>35</v>
+      </c>
+      <c r="F112" s="20" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="26" t="n">
-        <v>44028</v>
+        <v>44057</v>
       </c>
       <c r="B113" s="31" t="s">
         <v>254</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>255</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F113" s="20" t="s">
-        <v>57</v>
+        <v>35</v>
+      </c>
+      <c r="F113" s="5" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="26" t="n">
-        <v>44064</v>
+        <v>44028</v>
       </c>
       <c r="B114" s="31" t="s">
         <v>256</v>
@@ -4200,15 +4210,15 @@
         <v>257</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F114" s="5" t="s">
-        <v>47</v>
+        <v>160</v>
+      </c>
+      <c r="F114" s="20" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="26" t="n">
-        <v>44028</v>
+        <v>44064</v>
       </c>
       <c r="B115" s="31" t="s">
         <v>258</v>
@@ -4220,15 +4230,15 @@
         <v>259</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F115" s="20" t="s">
-        <v>57</v>
+        <v>160</v>
+      </c>
+      <c r="F115" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="26" t="n">
-        <v>44016</v>
+        <v>44028</v>
       </c>
       <c r="B116" s="31" t="s">
         <v>260</v>
@@ -4240,15 +4250,15 @@
         <v>261</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F116" s="5" t="s">
-        <v>47</v>
+        <v>160</v>
+      </c>
+      <c r="F116" s="20" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="26" t="n">
-        <v>44010</v>
+        <v>44016</v>
       </c>
       <c r="B117" s="31" t="s">
         <v>262</v>
@@ -4260,35 +4270,35 @@
         <v>263</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="26" t="n">
-        <v>43995</v>
+        <v>44010</v>
       </c>
       <c r="B118" s="31" t="s">
         <v>264</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>265</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F118" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="26" t="n">
-        <v>43948</v>
+        <v>43995</v>
       </c>
       <c r="B119" s="31" t="s">
         <v>266</v>
@@ -4300,15 +4310,15 @@
         <v>267</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F119" s="20" t="s">
-        <v>57</v>
+        <v>35</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="26" t="n">
-        <v>43947</v>
+        <v>43948</v>
       </c>
       <c r="B120" s="31" t="s">
         <v>268</v>
@@ -4320,15 +4330,15 @@
         <v>269</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F120" s="14" t="s">
-        <v>33</v>
+        <v>160</v>
+      </c>
+      <c r="F120" s="20" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="26" t="n">
-        <v>43936</v>
+        <v>43947</v>
       </c>
       <c r="B121" s="31" t="s">
         <v>270</v>
@@ -4340,35 +4350,35 @@
         <v>271</v>
       </c>
       <c r="E121" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F121" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="F121" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="26" t="n">
-        <v>43929</v>
+        <v>43936</v>
       </c>
       <c r="B122" s="31" t="s">
         <v>272</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>273</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>158</v>
+        <v>35</v>
       </c>
       <c r="F122" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="26" t="n">
-        <v>43891</v>
+        <v>43929</v>
       </c>
       <c r="B123" s="31" t="s">
         <v>274</v>
@@ -4380,15 +4390,15 @@
         <v>275</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F123" s="20" t="s">
-        <v>57</v>
+        <v>160</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="26" t="n">
-        <v>43885</v>
+        <v>43891</v>
       </c>
       <c r="B124" s="31" t="s">
         <v>276</v>
@@ -4400,15 +4410,15 @@
         <v>277</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F124" s="5" t="s">
-        <v>47</v>
+        <v>160</v>
+      </c>
+      <c r="F124" s="20" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="26" t="n">
-        <v>43857</v>
+        <v>43885</v>
       </c>
       <c r="B125" s="31" t="s">
         <v>278</v>
@@ -4420,10 +4430,10 @@
         <v>279</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F125" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4440,15 +4450,15 @@
         <v>281</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="26" t="n">
-        <v>43852</v>
+        <v>43857</v>
       </c>
       <c r="B127" s="31" t="s">
         <v>282</v>
@@ -4460,15 +4470,15 @@
         <v>283</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="26" t="n">
-        <v>43584</v>
+        <v>43852</v>
       </c>
       <c r="B128" s="31" t="s">
         <v>284</v>
@@ -4480,10 +4490,10 @@
         <v>285</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>23</v>
+        <v>160</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4503,14 +4513,14 @@
         <v>23</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="26" t="n">
-        <v>43540</v>
-      </c>
-      <c r="B130" s="5" t="s">
+        <v>43584</v>
+      </c>
+      <c r="B130" s="31" t="s">
         <v>288</v>
       </c>
       <c r="C130" s="5" t="s">
@@ -4523,32 +4533,32 @@
         <v>23</v>
       </c>
       <c r="F130" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="26" t="n">
-        <v>43203</v>
-      </c>
-      <c r="B132" s="41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="26" t="n">
+        <v>43540</v>
+      </c>
+      <c r="B131" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="C132" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D132" s="5" t="s">
+      <c r="C131" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D131" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="E132" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F132" s="14" t="s">
-        <v>33</v>
+      <c r="E131" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F131" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4559,61 +4569,61 @@
         <v>292</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D133" s="5" t="s">
         <v>293</v>
       </c>
       <c r="E133" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F133" s="5" t="s">
-        <v>294</v>
+        <v>160</v>
+      </c>
+      <c r="F133" s="14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="26" t="n">
-        <v>42842</v>
+        <v>43203</v>
       </c>
       <c r="B134" s="41" t="s">
+        <v>294</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D134" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="C134" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D134" s="5" t="s">
+      <c r="E134" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F134" s="5" t="s">
         <v>296</v>
-      </c>
-      <c r="E134" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F134" s="14" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="26" t="n">
-        <v>42457</v>
-      </c>
-      <c r="B135" s="5" t="s">
+        <v>42842</v>
+      </c>
+      <c r="B135" s="41" t="s">
         <v>297</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="D135" s="5" t="s">
         <v>298</v>
       </c>
       <c r="E135" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F135" s="5" t="s">
-        <v>47</v>
+        <v>35</v>
+      </c>
+      <c r="F135" s="14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="26" t="n">
-        <v>39028</v>
+        <v>42457</v>
       </c>
       <c r="B136" s="5" t="s">
         <v>299</v>
@@ -4625,21 +4635,41 @@
         <v>300</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F136" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="138" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AMG138" s="0"/>
-      <c r="AMH138" s="0"/>
-      <c r="AMI138" s="0"/>
-      <c r="AMJ138" s="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="26" t="n">
+        <v>39028</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C137" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D137" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="E137" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F137" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="139" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMG139" s="0"/>
+      <c r="AMH139" s="0"/>
+      <c r="AMI139" s="0"/>
+      <c r="AMJ139" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A:F"/>
-  <conditionalFormatting sqref="F87:F1048576 F1:F85">
+  <autoFilter ref="A1:F137"/>
+  <conditionalFormatting sqref="F88:F1048576 F1:F86">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="resolved" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("resolved",F1)))</formula>
     </cfRule>
@@ -4648,132 +4678,133 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="#1768"/>
-    <hyperlink ref="B4" r:id="rId2" display="#1766"/>
-    <hyperlink ref="B5" r:id="rId3" display="#274"/>
-    <hyperlink ref="B6" r:id="rId4" display="#273"/>
-    <hyperlink ref="B7" r:id="rId5" display="#272"/>
-    <hyperlink ref="B8" r:id="rId6" display="#1754"/>
-    <hyperlink ref="B9" r:id="rId7" display="#1752"/>
-    <hyperlink ref="B10" r:id="rId8" display="#1745"/>
-    <hyperlink ref="B11" r:id="rId9" display="#1743"/>
-    <hyperlink ref="B12" r:id="rId10" display="#1258"/>
-    <hyperlink ref="B13" r:id="rId11" display="#271"/>
-    <hyperlink ref="B14" r:id="rId12" display="#2"/>
-    <hyperlink ref="B15" r:id="rId13" display="#1349"/>
-    <hyperlink ref="B17" r:id="rId14" display="#1725"/>
-    <hyperlink ref="B18" r:id="rId15" display="#1724"/>
-    <hyperlink ref="B19" r:id="rId16" display="#1722"/>
-    <hyperlink ref="B20" r:id="rId17" display="#1226"/>
-    <hyperlink ref="B21" r:id="rId18" display="#1225"/>
-    <hyperlink ref="B22" r:id="rId19" display="#1720"/>
-    <hyperlink ref="B23" r:id="rId20" display="#1323"/>
-    <hyperlink ref="B24" r:id="rId21" display="#30"/>
-    <hyperlink ref="B25" r:id="rId22" display="#1712"/>
-    <hyperlink ref="B26" r:id="rId23" display="#1215"/>
-    <hyperlink ref="B27" r:id="rId24" display="#1214"/>
-    <hyperlink ref="B28" r:id="rId25" display="#1213"/>
-    <hyperlink ref="B29" r:id="rId26" display="#1212"/>
-    <hyperlink ref="B31" r:id="rId27" display="#1202"/>
-    <hyperlink ref="B32" r:id="rId28" display="#27"/>
-    <hyperlink ref="B33" r:id="rId29" display="#26"/>
-    <hyperlink ref="B34" r:id="rId30" display="#1201"/>
-    <hyperlink ref="B35" r:id="rId31" display="#1200"/>
-    <hyperlink ref="B36" r:id="rId32" display="#1708"/>
-    <hyperlink ref="B37" r:id="rId33" display="#1185"/>
-    <hyperlink ref="B38" r:id="rId34" display="#11"/>
-    <hyperlink ref="B39" r:id="rId35" display="#1309"/>
-    <hyperlink ref="B40" r:id="rId36" display="#1176"/>
-    <hyperlink ref="B41" r:id="rId37" display="#1171"/>
-    <hyperlink ref="B42" r:id="rId38" display="#1164"/>
-    <hyperlink ref="B43" r:id="rId39" display="#9"/>
-    <hyperlink ref="B44" r:id="rId40" display="#1163"/>
-    <hyperlink ref="B45" r:id="rId41" display="#1161"/>
-    <hyperlink ref="B46" r:id="rId42" display="#1690"/>
-    <hyperlink ref="B48" r:id="rId43" display="#1155"/>
-    <hyperlink ref="B49" r:id="rId44" display="#1150"/>
-    <hyperlink ref="B50" r:id="rId45" display="#1151"/>
-    <hyperlink ref="B51" r:id="rId46" display="#1200"/>
-    <hyperlink ref="B52" r:id="rId47" display="#1681"/>
-    <hyperlink ref="B53" r:id="rId48" display="#51"/>
-    <hyperlink ref="B54" r:id="rId49" display="#1142"/>
-    <hyperlink ref="B55" r:id="rId50" display="#8"/>
-    <hyperlink ref="B56" r:id="rId51" display="#1674"/>
-    <hyperlink ref="B57" r:id="rId52" display="#1672"/>
-    <hyperlink ref="B58" r:id="rId53" display="#1669"/>
-    <hyperlink ref="B59" r:id="rId54" display="#1670"/>
-    <hyperlink ref="B60" r:id="rId55" display="#1184"/>
-    <hyperlink ref="B61" r:id="rId56" display="#49"/>
-    <hyperlink ref="B62" r:id="rId57" display="#1140"/>
-    <hyperlink ref="B63" r:id="rId58" display="#1132"/>
-    <hyperlink ref="B65" r:id="rId59" display="#1125"/>
-    <hyperlink ref="B66" r:id="rId60" display="#1641"/>
-    <hyperlink ref="B67" r:id="rId61" display="#1124"/>
-    <hyperlink ref="B68" r:id="rId62" display="#1122"/>
-    <hyperlink ref="B69" r:id="rId63" display="#43"/>
-    <hyperlink ref="B70" r:id="rId64" display="#1622"/>
-    <hyperlink ref="B72" r:id="rId65" display="#38"/>
-    <hyperlink ref="B73" r:id="rId66" display="#1621"/>
-    <hyperlink ref="B74" r:id="rId67" display="#1616"/>
-    <hyperlink ref="B75" r:id="rId68" display="#37"/>
-    <hyperlink ref="B76" r:id="rId69" display="#36"/>
-    <hyperlink ref="B77" r:id="rId70" display="#1101"/>
-    <hyperlink ref="B78" r:id="rId71" display="#1099"/>
-    <hyperlink ref="B79" r:id="rId72" display="#1098"/>
-    <hyperlink ref="B80" r:id="rId73" display="#1617"/>
-    <hyperlink ref="B81" r:id="rId74" display="#1092"/>
-    <hyperlink ref="B82" r:id="rId75" display="#1128"/>
-    <hyperlink ref="B83" r:id="rId76" display="#1090"/>
-    <hyperlink ref="B84" r:id="rId77" display="#1608"/>
-    <hyperlink ref="B85" r:id="rId78" display="#35"/>
-    <hyperlink ref="B87" r:id="rId79" display="#1070"/>
-    <hyperlink ref="B88" r:id="rId80" display="#1592"/>
-    <hyperlink ref="B89" r:id="rId81" display="#1591"/>
-    <hyperlink ref="B90" r:id="rId82" display="#1578"/>
-    <hyperlink ref="B91" r:id="rId83" display="#41"/>
-    <hyperlink ref="B92" r:id="rId84" display="#42"/>
-    <hyperlink ref="B93" r:id="rId85" display="#1566"/>
-    <hyperlink ref="B94" r:id="rId86" display="#1565"/>
-    <hyperlink ref="B95" r:id="rId87" display="#1046"/>
-    <hyperlink ref="B96" r:id="rId88" display="#1559"/>
-    <hyperlink ref="B97" r:id="rId89" display="#1038"/>
-    <hyperlink ref="B98" r:id="rId90" display="#1037"/>
-    <hyperlink ref="B99" r:id="rId91" display="#1020"/>
-    <hyperlink ref="B100" r:id="rId92" display="#1032"/>
-    <hyperlink ref="B101" r:id="rId93" display="#1546"/>
-    <hyperlink ref="B102" r:id="rId94" display="#1027"/>
-    <hyperlink ref="B103" r:id="rId95" display="#1529"/>
-    <hyperlink ref="B105" r:id="rId96" display="#1527"/>
-    <hyperlink ref="B106" r:id="rId97" display="#558"/>
-    <hyperlink ref="B107" r:id="rId98" display="#1005"/>
-    <hyperlink ref="B108" r:id="rId99" display="#1020"/>
-    <hyperlink ref="B109" r:id="rId100" display="#993"/>
-    <hyperlink ref="B110" r:id="rId101" display="#1520"/>
-    <hyperlink ref="B111" r:id="rId102" display="#1519"/>
-    <hyperlink ref="B112" r:id="rId103" display="#969"/>
-    <hyperlink ref="B113" r:id="rId104" display="#1003"/>
-    <hyperlink ref="B114" r:id="rId105" display="#1015"/>
-    <hyperlink ref="B115" r:id="rId106" display="#1002"/>
-    <hyperlink ref="B116" r:id="rId107" display="#1471"/>
-    <hyperlink ref="B117" r:id="rId108" display="#1497"/>
-    <hyperlink ref="B118" r:id="rId109" display="#947"/>
-    <hyperlink ref="B119" r:id="rId110" display="#933"/>
-    <hyperlink ref="B120" r:id="rId111" display="#932"/>
-    <hyperlink ref="B121" r:id="rId112" display="#931"/>
-    <hyperlink ref="B122" r:id="rId113" display="#987"/>
-    <hyperlink ref="B123" r:id="rId114" display="#988"/>
-    <hyperlink ref="B124" r:id="rId115" display="#982"/>
-    <hyperlink ref="B125" r:id="rId116" display="#979"/>
-    <hyperlink ref="B126" r:id="rId117" display="#977"/>
-    <hyperlink ref="B127" r:id="rId118" display="#975"/>
-    <hyperlink ref="B128" r:id="rId119" display="#1445"/>
-    <hyperlink ref="B129" r:id="rId120" display="#1444"/>
-    <hyperlink ref="B130" r:id="rId121" display="#1427"/>
-    <hyperlink ref="B132" r:id="rId122" display="#23"/>
-    <hyperlink ref="B133" r:id="rId123" display="#22"/>
-    <hyperlink ref="B134" r:id="rId124" display="#18"/>
-    <hyperlink ref="B135" r:id="rId125" display="#1207"/>
-    <hyperlink ref="B136" r:id="rId126" display="#245"/>
+    <hyperlink ref="B3" r:id="rId1" display="#1277"/>
+    <hyperlink ref="B4" r:id="rId2" display="#1768"/>
+    <hyperlink ref="B5" r:id="rId3" display="#1766"/>
+    <hyperlink ref="B6" r:id="rId4" display="#274"/>
+    <hyperlink ref="B7" r:id="rId5" display="#273"/>
+    <hyperlink ref="B8" r:id="rId6" display="#272"/>
+    <hyperlink ref="B9" r:id="rId7" display="#1754"/>
+    <hyperlink ref="B10" r:id="rId8" display="#1752"/>
+    <hyperlink ref="B11" r:id="rId9" display="#1745"/>
+    <hyperlink ref="B12" r:id="rId10" display="#1743"/>
+    <hyperlink ref="B13" r:id="rId11" display="#1258"/>
+    <hyperlink ref="B14" r:id="rId12" display="#271"/>
+    <hyperlink ref="B15" r:id="rId13" display="#2"/>
+    <hyperlink ref="B16" r:id="rId14" display="#1349"/>
+    <hyperlink ref="B18" r:id="rId15" display="#1725"/>
+    <hyperlink ref="B19" r:id="rId16" display="#1724"/>
+    <hyperlink ref="B20" r:id="rId17" display="#1722"/>
+    <hyperlink ref="B21" r:id="rId18" display="#1226"/>
+    <hyperlink ref="B22" r:id="rId19" display="#1225"/>
+    <hyperlink ref="B23" r:id="rId20" display="#1720"/>
+    <hyperlink ref="B24" r:id="rId21" display="#1323"/>
+    <hyperlink ref="B25" r:id="rId22" display="#30"/>
+    <hyperlink ref="B26" r:id="rId23" display="#1712"/>
+    <hyperlink ref="B27" r:id="rId24" display="#1215"/>
+    <hyperlink ref="B28" r:id="rId25" display="#1214"/>
+    <hyperlink ref="B29" r:id="rId26" display="#1213"/>
+    <hyperlink ref="B30" r:id="rId27" display="#1212"/>
+    <hyperlink ref="B32" r:id="rId28" display="#1202"/>
+    <hyperlink ref="B33" r:id="rId29" display="#27"/>
+    <hyperlink ref="B34" r:id="rId30" display="#26"/>
+    <hyperlink ref="B35" r:id="rId31" display="#1201"/>
+    <hyperlink ref="B36" r:id="rId32" display="#1200"/>
+    <hyperlink ref="B37" r:id="rId33" display="#1708"/>
+    <hyperlink ref="B38" r:id="rId34" display="#1185"/>
+    <hyperlink ref="B39" r:id="rId35" display="#11"/>
+    <hyperlink ref="B40" r:id="rId36" display="#1309"/>
+    <hyperlink ref="B41" r:id="rId37" display="#1176"/>
+    <hyperlink ref="B42" r:id="rId38" display="#1171"/>
+    <hyperlink ref="B43" r:id="rId39" display="#1164"/>
+    <hyperlink ref="B44" r:id="rId40" display="#9"/>
+    <hyperlink ref="B45" r:id="rId41" display="#1163"/>
+    <hyperlink ref="B46" r:id="rId42" display="#1161"/>
+    <hyperlink ref="B47" r:id="rId43" display="#1690"/>
+    <hyperlink ref="B49" r:id="rId44" display="#1155"/>
+    <hyperlink ref="B50" r:id="rId45" display="#1150"/>
+    <hyperlink ref="B51" r:id="rId46" display="#1151"/>
+    <hyperlink ref="B52" r:id="rId47" display="#1200"/>
+    <hyperlink ref="B53" r:id="rId48" display="#1681"/>
+    <hyperlink ref="B54" r:id="rId49" display="#51"/>
+    <hyperlink ref="B55" r:id="rId50" display="#1142"/>
+    <hyperlink ref="B56" r:id="rId51" display="#8"/>
+    <hyperlink ref="B57" r:id="rId52" display="#1674"/>
+    <hyperlink ref="B58" r:id="rId53" display="#1672"/>
+    <hyperlink ref="B59" r:id="rId54" display="#1669"/>
+    <hyperlink ref="B60" r:id="rId55" display="#1670"/>
+    <hyperlink ref="B61" r:id="rId56" display="#1184"/>
+    <hyperlink ref="B62" r:id="rId57" display="#49"/>
+    <hyperlink ref="B63" r:id="rId58" display="#1140"/>
+    <hyperlink ref="B64" r:id="rId59" display="#1132"/>
+    <hyperlink ref="B66" r:id="rId60" display="#1125"/>
+    <hyperlink ref="B67" r:id="rId61" display="#1641"/>
+    <hyperlink ref="B68" r:id="rId62" display="#1124"/>
+    <hyperlink ref="B69" r:id="rId63" display="#1122"/>
+    <hyperlink ref="B70" r:id="rId64" display="#43"/>
+    <hyperlink ref="B71" r:id="rId65" display="#1622"/>
+    <hyperlink ref="B73" r:id="rId66" display="#38"/>
+    <hyperlink ref="B74" r:id="rId67" display="#1621"/>
+    <hyperlink ref="B75" r:id="rId68" display="#1616"/>
+    <hyperlink ref="B76" r:id="rId69" display="#37"/>
+    <hyperlink ref="B77" r:id="rId70" display="#36"/>
+    <hyperlink ref="B78" r:id="rId71" display="#1101"/>
+    <hyperlink ref="B79" r:id="rId72" display="#1099"/>
+    <hyperlink ref="B80" r:id="rId73" display="#1098"/>
+    <hyperlink ref="B81" r:id="rId74" display="#1617"/>
+    <hyperlink ref="B82" r:id="rId75" display="#1092"/>
+    <hyperlink ref="B83" r:id="rId76" display="#1128"/>
+    <hyperlink ref="B84" r:id="rId77" display="#1090"/>
+    <hyperlink ref="B85" r:id="rId78" display="#1608"/>
+    <hyperlink ref="B86" r:id="rId79" display="#35"/>
+    <hyperlink ref="B88" r:id="rId80" display="#1070"/>
+    <hyperlink ref="B89" r:id="rId81" display="#1592"/>
+    <hyperlink ref="B90" r:id="rId82" display="#1591"/>
+    <hyperlink ref="B91" r:id="rId83" display="#1578"/>
+    <hyperlink ref="B92" r:id="rId84" display="#41"/>
+    <hyperlink ref="B93" r:id="rId85" display="#42"/>
+    <hyperlink ref="B94" r:id="rId86" display="#1566"/>
+    <hyperlink ref="B95" r:id="rId87" display="#1565"/>
+    <hyperlink ref="B96" r:id="rId88" display="#1046"/>
+    <hyperlink ref="B97" r:id="rId89" display="#1559"/>
+    <hyperlink ref="B98" r:id="rId90" display="#1038"/>
+    <hyperlink ref="B99" r:id="rId91" display="#1037"/>
+    <hyperlink ref="B100" r:id="rId92" display="#1020"/>
+    <hyperlink ref="B101" r:id="rId93" display="#1032"/>
+    <hyperlink ref="B102" r:id="rId94" display="#1546"/>
+    <hyperlink ref="B103" r:id="rId95" display="#1027"/>
+    <hyperlink ref="B104" r:id="rId96" display="#1529"/>
+    <hyperlink ref="B106" r:id="rId97" display="#1527"/>
+    <hyperlink ref="B107" r:id="rId98" display="#558"/>
+    <hyperlink ref="B108" r:id="rId99" display="#1005"/>
+    <hyperlink ref="B109" r:id="rId100" display="#1020"/>
+    <hyperlink ref="B110" r:id="rId101" display="#993"/>
+    <hyperlink ref="B111" r:id="rId102" display="#1520"/>
+    <hyperlink ref="B112" r:id="rId103" display="#1519"/>
+    <hyperlink ref="B113" r:id="rId104" display="#969"/>
+    <hyperlink ref="B114" r:id="rId105" display="#1003"/>
+    <hyperlink ref="B115" r:id="rId106" display="#1015"/>
+    <hyperlink ref="B116" r:id="rId107" display="#1002"/>
+    <hyperlink ref="B117" r:id="rId108" display="#1471"/>
+    <hyperlink ref="B118" r:id="rId109" display="#1497"/>
+    <hyperlink ref="B119" r:id="rId110" display="#947"/>
+    <hyperlink ref="B120" r:id="rId111" display="#933"/>
+    <hyperlink ref="B121" r:id="rId112" display="#932"/>
+    <hyperlink ref="B122" r:id="rId113" display="#931"/>
+    <hyperlink ref="B123" r:id="rId114" display="#987"/>
+    <hyperlink ref="B124" r:id="rId115" display="#988"/>
+    <hyperlink ref="B125" r:id="rId116" display="#982"/>
+    <hyperlink ref="B126" r:id="rId117" display="#979"/>
+    <hyperlink ref="B127" r:id="rId118" display="#977"/>
+    <hyperlink ref="B128" r:id="rId119" display="#975"/>
+    <hyperlink ref="B129" r:id="rId120" display="#1445"/>
+    <hyperlink ref="B130" r:id="rId121" display="#1444"/>
+    <hyperlink ref="B131" r:id="rId122" display="#1427"/>
+    <hyperlink ref="B133" r:id="rId123" display="#23"/>
+    <hyperlink ref="B134" r:id="rId124" display="#22"/>
+    <hyperlink ref="B135" r:id="rId125" display="#18"/>
+    <hyperlink ref="B136" r:id="rId126" display="#1207"/>
+    <hyperlink ref="B137" r:id="rId127" display="#245"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
@@ -4782,7 +4813,7 @@
     <oddHeader>&amp;C&amp;"Sans,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Sans,Regular"Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId127"/>
+  <drawing r:id="rId128"/>
 </worksheet>
 </file>
 
@@ -4815,10 +4846,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -4827,10 +4858,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated ticket list (mostly, updated okapi tickes from bitbucket to gitlab)
</commit_message>
<xml_diff>
--- a/docs/tools/tickets/OmegaT_issues_nopw.xlsx
+++ b/docs/tools/tickets/OmegaT_issues_nopw.xlsx
@@ -13,8 +13,8 @@
     <sheet name="ETS" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A:$F</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A$1:$F$140</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A$1:$F$141</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A:$F</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="true" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="314">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -419,6 +419,12 @@
   </si>
   <si>
     <t xml:space="preserve">Project not loaded if it contains DTD internal entities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#1695</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate JSON format stastics file when save</t>
   </si>
   <si>
     <t xml:space="preserve">#1161</t>
@@ -1185,7 +1191,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1201,7 +1207,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9EEF2"/>
-        <bgColor rgb="FFDDE8CB"/>
+        <bgColor rgb="FFEEEEEE"/>
       </patternFill>
     </fill>
     <fill>
@@ -1225,7 +1231,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF5CE"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFEEEEEE"/>
       </patternFill>
     </fill>
     <fill>
@@ -1244,6 +1250,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFDBB6"/>
         <bgColor rgb="FFFFD7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFD9EEF2"/>
       </patternFill>
     </fill>
   </fills>
@@ -1340,10 +1352,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1393,6 +1401,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1539,11 +1551,11 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFDDE8CB"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FFFFD7D7"/>
-      <rgbColor rgb="FFAFD095"/>
-      <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFDBB6"/>
       <rgbColor rgb="FF3366FF"/>
@@ -1745,12 +1757,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ142"/>
+  <dimension ref="A1:AMJ143"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
@@ -1855,7 +1867,7 @@
       <c r="E5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="5" t="s">
         <v>36</v>
       </c>
       <c r="AMG5" s="0"/>
@@ -1879,7 +1891,7 @@
       <c r="E6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="5" t="s">
         <v>36</v>
       </c>
       <c r="AMG6" s="0"/>
@@ -1903,7 +1915,7 @@
       <c r="E7" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="5" t="s">
         <v>36</v>
       </c>
       <c r="AMG7" s="0"/>
@@ -1927,7 +1939,7 @@
       <c r="E8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="5" t="s">
         <v>44</v>
       </c>
       <c r="AMG8" s="0"/>
@@ -1951,7 +1963,7 @@
       <c r="E9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="5" t="s">
         <v>36</v>
       </c>
       <c r="AMG9" s="0"/>
@@ -1975,7 +1987,7 @@
       <c r="E10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="5" t="s">
         <v>36</v>
       </c>
       <c r="AMG10" s="0"/>
@@ -1984,7 +1996,7 @@
       <c r="AMJ10" s="0"/>
     </row>
     <row r="11" s="8" customFormat="true" ht="11.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="n">
+      <c r="A11" s="13" t="n">
         <v>45488</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -1993,13 +2005,13 @@
       <c r="C11" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>51</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="5" t="s">
         <v>36</v>
       </c>
       <c r="AMG11" s="0"/>
@@ -2008,7 +2020,7 @@
       <c r="AMJ11" s="0"/>
     </row>
     <row r="12" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14" t="n">
+      <c r="A12" s="13" t="n">
         <v>45483</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -2017,13 +2029,13 @@
       <c r="C12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>53</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="5" t="s">
         <v>36</v>
       </c>
       <c r="AMG12" s="0"/>
@@ -2032,7 +2044,7 @@
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="n">
+      <c r="A13" s="13" t="n">
         <v>45469</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -2041,13 +2053,13 @@
       <c r="C13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>55</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="5" t="s">
         <v>44</v>
       </c>
       <c r="AMG13" s="0"/>
@@ -2056,7 +2068,7 @@
       <c r="AMJ13" s="0"/>
     </row>
     <row r="14" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="n">
+      <c r="A14" s="13" t="n">
         <v>45784</v>
       </c>
       <c r="B14" s="10" t="s">
@@ -2065,13 +2077,13 @@
       <c r="C14" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>57</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="5" t="s">
         <v>36</v>
       </c>
       <c r="AMG14" s="0"/>
@@ -2080,7 +2092,7 @@
       <c r="AMJ14" s="0"/>
     </row>
     <row r="15" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="n">
+      <c r="A15" s="13" t="n">
         <v>45411</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -2089,13 +2101,13 @@
       <c r="C15" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="14" t="s">
         <v>59</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="5" t="s">
         <v>36</v>
       </c>
       <c r="AMG15" s="0"/>
@@ -2104,7 +2116,7 @@
       <c r="AMJ15" s="0"/>
     </row>
     <row r="16" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="n">
+      <c r="A16" s="13" t="n">
         <v>45394</v>
       </c>
       <c r="B16" s="10" t="s">
@@ -2113,7 +2125,7 @@
       <c r="C16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>61</v>
       </c>
       <c r="E16" s="11" t="s">
@@ -2143,7 +2155,7 @@
       <c r="E17" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="15" t="s">
         <v>32</v>
       </c>
       <c r="AMG17" s="0"/>
@@ -2161,7 +2173,7 @@
       <c r="C18" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>67</v>
       </c>
       <c r="E18" s="11" t="s">
@@ -2203,7 +2215,7 @@
       <c r="A20" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="16" t="s">
         <v>29</v>
       </c>
       <c r="AMG20" s="0"/>
@@ -2221,13 +2233,13 @@
       <c r="C21" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="14" t="s">
         <v>72</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="15" t="s">
         <v>36</v>
       </c>
       <c r="AMG21" s="0"/>
@@ -2251,7 +2263,7 @@
       <c r="E22" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="15" t="s">
         <v>36</v>
       </c>
       <c r="AMG22" s="0"/>
@@ -2299,7 +2311,7 @@
       <c r="E24" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="17" t="s">
         <v>79</v>
       </c>
       <c r="AMG24" s="0"/>
@@ -2323,7 +2335,7 @@
       <c r="E25" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="F25" s="15" t="s">
         <v>36</v>
       </c>
       <c r="AMG25" s="0"/>
@@ -2428,22 +2440,22 @@
       <c r="AMJ29" s="0"/>
     </row>
     <row r="30" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="19" t="n">
+      <c r="A30" s="18" t="n">
         <v>45169</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="21" t="s">
+      <c r="C30" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F30" s="20" t="s">
         <v>91</v>
       </c>
       <c r="AMG30" s="0"/>
@@ -2452,22 +2464,22 @@
       <c r="AMJ30" s="0"/>
     </row>
     <row r="31" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="19" t="n">
+      <c r="A31" s="18" t="n">
         <v>45145</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="21" t="s">
+      <c r="C31" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="21" t="s">
+      <c r="F31" s="20" t="s">
         <v>93</v>
       </c>
       <c r="AMG31" s="0"/>
@@ -2491,7 +2503,7 @@
       <c r="E32" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F32" s="22" t="s">
+      <c r="F32" s="21" t="s">
         <v>32</v>
       </c>
       <c r="AMG32" s="0"/>
@@ -2515,7 +2527,7 @@
       <c r="E33" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F33" s="22" t="s">
+      <c r="F33" s="21" t="s">
         <v>32</v>
       </c>
       <c r="AMG33" s="0"/>
@@ -2557,7 +2569,7 @@
       <c r="E35" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F35" s="16" t="s">
+      <c r="F35" s="15" t="s">
         <v>36</v>
       </c>
       <c r="AMG35" s="0"/>
@@ -2581,7 +2593,7 @@
       <c r="E36" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F36" s="16" t="s">
+      <c r="F36" s="15" t="s">
         <v>36</v>
       </c>
       <c r="AMG36" s="0"/>
@@ -2605,7 +2617,7 @@
       <c r="E37" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F37" s="16" t="s">
+      <c r="F37" s="15" t="s">
         <v>36</v>
       </c>
       <c r="AMG37" s="0"/>
@@ -2629,7 +2641,7 @@
       <c r="E38" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F38" s="16" t="s">
+      <c r="F38" s="15" t="s">
         <v>36</v>
       </c>
       <c r="AMG38" s="0"/>
@@ -2653,7 +2665,7 @@
       <c r="E39" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F39" s="16" t="s">
+      <c r="F39" s="15" t="s">
         <v>36</v>
       </c>
       <c r="AMG39" s="0"/>
@@ -2701,7 +2713,7 @@
       <c r="E41" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F41" s="23" t="s">
+      <c r="F41" s="22" t="s">
         <v>114</v>
       </c>
       <c r="AMG41" s="0"/>
@@ -2749,7 +2761,7 @@
       <c r="E43" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="24" t="s">
+      <c r="F43" s="23" t="s">
         <v>120</v>
       </c>
       <c r="AMG43" s="0"/>
@@ -2821,7 +2833,7 @@
       <c r="E46" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F46" s="25" t="s">
+      <c r="F46" s="24" t="s">
         <v>32</v>
       </c>
       <c r="AMG46" s="0"/>
@@ -2836,7 +2848,7 @@
       <c r="B47" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C47" s="26" t="s">
+      <c r="C47" s="25" t="s">
         <v>116</v>
       </c>
       <c r="D47" s="11" t="s">
@@ -2877,9 +2889,9 @@
       <c r="AMI48" s="0"/>
       <c r="AMJ48" s="0"/>
     </row>
-    <row r="49" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="n">
-        <v>45040</v>
+        <v>45041</v>
       </c>
       <c r="B49" s="10" t="s">
         <v>131</v>
@@ -2891,19 +2903,19 @@
         <v>132</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" s="11" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="AMG49" s="0"/>
       <c r="AMH49" s="0"/>
       <c r="AMI49" s="0"/>
       <c r="AMJ49" s="0"/>
     </row>
-    <row r="50" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="n">
-        <v>45028</v>
+        <v>45040</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>133</v>
@@ -2915,10 +2927,10 @@
         <v>134</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F50" s="12" t="s">
-        <v>32</v>
+        <v>9</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="AMG50" s="0"/>
       <c r="AMH50" s="0"/>
@@ -2927,13 +2939,19 @@
     </row>
     <row r="51" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="n">
-        <v>44996</v>
+        <v>45028</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>135</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="F51" s="12" t="s">
         <v>32</v>
@@ -2945,19 +2963,14 @@
     </row>
     <row r="52" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="n">
-        <v>45007</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>136</v>
-      </c>
+        <v>44996</v>
+      </c>
+      <c r="B52" s="26"/>
       <c r="C52" s="11" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="D52" s="11" t="s">
         <v>137</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>9</v>
       </c>
       <c r="F52" s="12" t="s">
         <v>32</v>
@@ -2967,9 +2980,9 @@
       <c r="AMI52" s="0"/>
       <c r="AMJ52" s="0"/>
     </row>
-    <row r="53" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="n">
-        <v>44993</v>
+        <v>45007</v>
       </c>
       <c r="B53" s="10" t="s">
         <v>138</v>
@@ -2983,8 +2996,8 @@
       <c r="E53" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F53" s="23" t="s">
-        <v>114</v>
+      <c r="F53" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="AMG53" s="0"/>
       <c r="AMH53" s="0"/>
@@ -3007,7 +3020,7 @@
       <c r="E54" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F54" s="23" t="s">
+      <c r="F54" s="22" t="s">
         <v>114</v>
       </c>
       <c r="AMG54" s="0"/>
@@ -3017,22 +3030,22 @@
     </row>
     <row r="55" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="n">
-        <v>44991</v>
+        <v>44993</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E55" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F55" s="11" t="s">
-        <v>143</v>
+      <c r="F55" s="22" t="s">
+        <v>114</v>
       </c>
       <c r="AMG55" s="0"/>
       <c r="AMH55" s="0"/>
@@ -3041,22 +3054,22 @@
     </row>
     <row r="56" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="n">
-        <v>44981</v>
+        <v>44991</v>
       </c>
       <c r="B56" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="C56" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D56" s="11" t="s">
+      <c r="E56" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="11" t="s">
         <v>145</v>
-      </c>
-      <c r="E56" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F56" s="11" t="s">
-        <v>44</v>
       </c>
       <c r="AMG56" s="0"/>
       <c r="AMH56" s="0"/>
@@ -3065,22 +3078,22 @@
     </row>
     <row r="57" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="9" t="n">
-        <v>44973</v>
+        <v>44981</v>
       </c>
       <c r="B57" s="10" t="s">
         <v>146</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="D57" s="11" t="s">
         <v>147</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57" s="27" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="AMG57" s="0"/>
       <c r="AMH57" s="0"/>
@@ -3088,47 +3101,47 @@
       <c r="AMJ57" s="0"/>
     </row>
     <row r="58" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="19" t="n">
-        <v>44972</v>
-      </c>
-      <c r="B58" s="20" t="s">
+      <c r="A58" s="9" t="n">
+        <v>44973</v>
+      </c>
+      <c r="B58" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C58" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D58" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="E58" s="21" t="s">
+      <c r="C58" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="E58" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F58" s="21" t="s">
-        <v>91</v>
+      <c r="F58" s="27" t="s">
+        <v>36</v>
       </c>
       <c r="AMG58" s="0"/>
       <c r="AMH58" s="0"/>
       <c r="AMI58" s="0"/>
       <c r="AMJ58" s="0"/>
     </row>
-    <row r="59" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="28" t="n">
-        <v>44970</v>
-      </c>
-      <c r="B59" s="29" t="s">
+    <row r="59" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="18" t="n">
+        <v>44972</v>
+      </c>
+      <c r="B59" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="C59" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="D59" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="E59" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="F59" s="26" t="s">
-        <v>44</v>
+      <c r="E59" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="AMG59" s="0"/>
       <c r="AMH59" s="0"/>
@@ -3137,22 +3150,22 @@
     </row>
     <row r="60" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="28" t="n">
-        <v>44967</v>
+        <v>44970</v>
       </c>
       <c r="B60" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="C60" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D60" s="26" t="s">
+      <c r="C60" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="D60" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="E60" s="26" t="s">
+      <c r="E60" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="F60" s="16" t="s">
-        <v>36</v>
+      <c r="F60" s="25" t="s">
+        <v>44</v>
       </c>
       <c r="AMG60" s="0"/>
       <c r="AMH60" s="0"/>
@@ -3161,22 +3174,22 @@
     </row>
     <row r="61" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="28" t="n">
-        <v>44964</v>
+        <v>44967</v>
       </c>
       <c r="B61" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="C61" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D61" s="26" t="s">
+      <c r="C61" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="E61" s="26" t="s">
+      <c r="E61" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="F61" s="23" t="s">
-        <v>114</v>
+      <c r="F61" s="15" t="s">
+        <v>36</v>
       </c>
       <c r="AMG61" s="0"/>
       <c r="AMH61" s="0"/>
@@ -3185,21 +3198,21 @@
     </row>
     <row r="62" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="28" t="n">
-        <v>44952</v>
+        <v>44964</v>
       </c>
       <c r="B62" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="C62" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D62" s="26" t="s">
+      <c r="C62" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="E62" s="26" t="s">
+      <c r="E62" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="F62" s="23" t="s">
+      <c r="F62" s="22" t="s">
         <v>114</v>
       </c>
       <c r="AMG62" s="0"/>
@@ -3214,17 +3227,17 @@
       <c r="B63" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="C63" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D63" s="26" t="s">
+      <c r="C63" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="E63" s="26" t="s">
+      <c r="E63" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="F63" s="12" t="s">
-        <v>32</v>
+      <c r="F63" s="22" t="s">
+        <v>114</v>
       </c>
       <c r="AMG63" s="0"/>
       <c r="AMH63" s="0"/>
@@ -3232,23 +3245,23 @@
       <c r="AMJ63" s="0"/>
     </row>
     <row r="64" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="30" t="n">
-        <v>44949</v>
-      </c>
-      <c r="B64" s="31" t="s">
+      <c r="A64" s="28" t="n">
+        <v>44952</v>
+      </c>
+      <c r="B64" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="C64" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D64" s="26" t="s">
+      <c r="C64" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="E64" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F64" s="16" t="s">
-        <v>36</v>
+      <c r="E64" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="AMG64" s="0"/>
       <c r="AMH64" s="0"/>
@@ -3256,23 +3269,23 @@
       <c r="AMJ64" s="0"/>
     </row>
     <row r="65" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="28" t="n">
-        <v>44948</v>
-      </c>
-      <c r="B65" s="29" t="s">
+      <c r="A65" s="30" t="n">
+        <v>44949</v>
+      </c>
+      <c r="B65" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="C65" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="D65" s="26" t="s">
+      <c r="C65" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="E65" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="F65" s="12" t="s">
-        <v>32</v>
+      <c r="E65" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>36</v>
       </c>
       <c r="AMG65" s="0"/>
       <c r="AMH65" s="0"/>
@@ -3281,19 +3294,19 @@
     </row>
     <row r="66" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="28" t="n">
-        <v>44946</v>
+        <v>44948</v>
       </c>
       <c r="B66" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="C66" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D66" s="26" t="s">
+      <c r="C66" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D66" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="E66" s="26" t="s">
-        <v>165</v>
+      <c r="E66" s="25" t="s">
+        <v>39</v>
       </c>
       <c r="F66" s="12" t="s">
         <v>32</v>
@@ -3303,36 +3316,48 @@
       <c r="AMI66" s="0"/>
       <c r="AMJ66" s="0"/>
     </row>
-    <row r="67" s="26" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="28" t="n">
-        <v>44929</v>
-      </c>
-      <c r="B67" s="32" t="s">
+        <v>44946</v>
+      </c>
+      <c r="B67" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="C67" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="C67" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D67" s="26" t="s">
+      <c r="E67" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="E67" s="26" t="s">
-        <v>165</v>
-      </c>
-      <c r="F67" s="16" t="s">
-        <v>36</v>
+      <c r="F67" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="AMG67" s="0"/>
       <c r="AMH67" s="0"/>
       <c r="AMI67" s="0"/>
       <c r="AMJ67" s="0"/>
     </row>
-    <row r="68" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="8" t="s">
+    <row r="68" s="25" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="28" t="n">
+        <v>44929</v>
+      </c>
+      <c r="B68" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="F68" s="8" t="s">
-        <v>29</v>
+      <c r="C68" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="E68" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="F68" s="15" t="s">
+        <v>36</v>
       </c>
       <c r="AMG68" s="0"/>
       <c r="AMH68" s="0"/>
@@ -3340,46 +3365,34 @@
       <c r="AMJ68" s="0"/>
     </row>
     <row r="69" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="28" t="n">
-        <v>44879</v>
-      </c>
-      <c r="B69" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D69" s="5" t="s">
+      <c r="A69" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="E69" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>44</v>
+      <c r="F69" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="AMG69" s="0"/>
       <c r="AMH69" s="0"/>
       <c r="AMI69" s="0"/>
       <c r="AMJ69" s="0"/>
     </row>
-    <row r="70" s="26" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="28" t="n">
-        <v>44858</v>
-      </c>
-      <c r="B70" s="29" t="s">
+        <v>44879</v>
+      </c>
+      <c r="B70" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="C70" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D70" s="26" t="s">
+      <c r="C70" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="E70" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="F70" s="26" t="s">
+      <c r="E70" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F70" s="5" t="s">
         <v>44</v>
       </c>
       <c r="AMG70" s="0"/>
@@ -3387,24 +3400,24 @@
       <c r="AMI70" s="0"/>
       <c r="AMJ70" s="0"/>
     </row>
-    <row r="71" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" s="25" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="28" t="n">
-        <v>44855</v>
-      </c>
-      <c r="B71" s="33" t="s">
+        <v>44858</v>
+      </c>
+      <c r="B71" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="C71" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D71" s="5" t="s">
+      <c r="C71" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E71" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F71" s="23" t="s">
-        <v>114</v>
+      <c r="E71" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F71" s="25" t="s">
+        <v>44</v>
       </c>
       <c r="AMG71" s="0"/>
       <c r="AMH71" s="0"/>
@@ -3413,7 +3426,7 @@
     </row>
     <row r="72" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="28" t="n">
-        <v>44844</v>
+        <v>44855</v>
       </c>
       <c r="B72" s="33" t="s">
         <v>175</v>
@@ -3425,113 +3438,117 @@
         <v>176</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>177</v>
+        <v>167</v>
+      </c>
+      <c r="F72" s="22" t="s">
+        <v>114</v>
       </c>
       <c r="AMG72" s="0"/>
       <c r="AMH72" s="0"/>
       <c r="AMI72" s="0"/>
       <c r="AMJ72" s="0"/>
     </row>
-    <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="28" t="n">
-        <v>44757</v>
-      </c>
-      <c r="B73" s="34" t="s">
+        <v>44844</v>
+      </c>
+      <c r="B73" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="C73" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D73" s="5" t="s">
+      <c r="E73" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F73" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="E73" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F73" s="12" t="s">
-        <v>32</v>
-      </c>
+      <c r="AMG73" s="0"/>
+      <c r="AMH73" s="0"/>
+      <c r="AMI73" s="0"/>
+      <c r="AMJ73" s="0"/>
     </row>
     <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="28" t="n">
-        <v>373466</v>
-      </c>
-      <c r="B74" s="33" t="s">
+        <v>44757</v>
+      </c>
+      <c r="B74" s="34" t="s">
         <v>180</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>181</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>44</v>
+        <v>167</v>
+      </c>
+      <c r="F74" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="28" t="n">
-        <v>44743</v>
+        <v>373466</v>
+      </c>
+      <c r="B75" s="33" t="s">
+        <v>182</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="F75" s="12" t="s">
-        <v>32</v>
+        <v>183</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="28" t="n">
-        <v>44740</v>
-      </c>
-      <c r="B76" s="35" t="s">
-        <v>183</v>
+        <v>44743</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="E76" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F76" s="16" t="s">
-        <v>36</v>
+      <c r="F76" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="28" t="n">
-        <v>44739</v>
-      </c>
-      <c r="B77" s="36" t="s">
+        <v>44740</v>
+      </c>
+      <c r="B77" s="35" t="s">
         <v>185</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>186</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F77" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="F77" s="15" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="28" t="n">
-        <v>44693</v>
+        <v>44739</v>
       </c>
       <c r="B78" s="36" t="s">
         <v>187</v>
@@ -3543,77 +3560,77 @@
         <v>188</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F78" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F78" s="15" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="28" t="n">
-        <v>44695</v>
-      </c>
-      <c r="B79" s="37" t="s">
+        <v>44693</v>
+      </c>
+      <c r="B79" s="36" t="s">
         <v>189</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>190</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F79" s="12" t="s">
-        <v>32</v>
+        <v>39</v>
+      </c>
+      <c r="F79" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="30" t="n">
-        <v>44659</v>
-      </c>
-      <c r="B80" s="38" t="s">
+      <c r="A80" s="28" t="n">
+        <v>44695</v>
+      </c>
+      <c r="B80" s="37" t="s">
         <v>191</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>192</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F80" s="16" t="s">
-        <v>36</v>
+        <v>167</v>
+      </c>
+      <c r="F80" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="28" t="n">
-        <v>44712</v>
-      </c>
-      <c r="B81" s="36" t="s">
+      <c r="A81" s="30" t="n">
+        <v>44659</v>
+      </c>
+      <c r="B81" s="38" t="s">
         <v>193</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>194</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>120</v>
+        <v>167</v>
+      </c>
+      <c r="F81" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="28" t="n">
-        <v>44705</v>
-      </c>
-      <c r="B82" s="33" t="s">
+        <v>44712</v>
+      </c>
+      <c r="B82" s="36" t="s">
         <v>195</v>
       </c>
       <c r="C82" s="5" t="s">
@@ -3623,10 +3640,10 @@
         <v>196</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F82" s="12" t="s">
-        <v>32</v>
+        <v>39</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3643,7 +3660,7 @@
         <v>198</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F83" s="12" t="s">
         <v>32</v>
@@ -3651,7 +3668,7 @@
     </row>
     <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="28" t="n">
-        <v>44693</v>
+        <v>44705</v>
       </c>
       <c r="B84" s="33" t="s">
         <v>199</v>
@@ -3663,15 +3680,15 @@
         <v>200</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>44</v>
+        <v>167</v>
+      </c>
+      <c r="F84" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="28" t="n">
-        <v>44622</v>
+        <v>44693</v>
       </c>
       <c r="B85" s="33" t="s">
         <v>201</v>
@@ -3683,57 +3700,57 @@
         <v>202</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F85" s="12" t="s">
-        <v>32</v>
+        <v>39</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="28" t="n">
-        <v>44614</v>
+        <v>44622</v>
       </c>
       <c r="B86" s="33" t="s">
         <v>203</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>204</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F86" s="16" t="s">
-        <v>36</v>
+        <v>167</v>
+      </c>
+      <c r="F86" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="28" t="n">
-        <v>44613</v>
+        <v>44614</v>
       </c>
       <c r="B87" s="33" t="s">
         <v>205</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>206</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>44</v>
+        <v>167</v>
+      </c>
+      <c r="F87" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="28" t="n">
-        <v>44608</v>
-      </c>
-      <c r="B88" s="36" t="s">
+        <v>44613</v>
+      </c>
+      <c r="B88" s="33" t="s">
         <v>207</v>
       </c>
       <c r="C88" s="5" t="s">
@@ -3743,60 +3760,60 @@
         <v>208</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F88" s="12" t="s">
-        <v>32</v>
+        <v>167</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="28" t="n">
-        <v>44580</v>
-      </c>
-      <c r="B89" s="33" t="s">
+        <v>44608</v>
+      </c>
+      <c r="B89" s="36" t="s">
         <v>209</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>210</v>
       </c>
       <c r="E89" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F89" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="28" t="n">
+        <v>44580</v>
+      </c>
+      <c r="B90" s="33" t="s">
+        <v>211</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E90" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F89" s="5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="28" t="n">
-        <v>44463</v>
-      </c>
-      <c r="B91" s="33" t="s">
-        <v>212</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D91" s="5" t="s">
+      <c r="F90" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="5" t="s">
         <v>213</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="28" t="n">
-        <v>44460</v>
+        <v>44463</v>
       </c>
       <c r="B92" s="33" t="s">
         <v>214</v>
@@ -3808,10 +3825,10 @@
         <v>215</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>39</v>
+        <v>167</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>216</v>
+        <v>44</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3819,24 +3836,24 @@
         <v>44460</v>
       </c>
       <c r="B93" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D93" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C93" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D93" s="5" t="s">
+      <c r="E93" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F93" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F93" s="12" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="28" t="n">
-        <v>44372</v>
+        <v>44460</v>
       </c>
       <c r="B94" s="33" t="s">
         <v>219</v>
@@ -3850,35 +3867,35 @@
       <c r="E94" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F94" s="5" t="s">
-        <v>44</v>
+      <c r="F94" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="28" t="n">
-        <v>44326</v>
+        <v>44372</v>
       </c>
       <c r="B95" s="33" t="s">
         <v>221</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>222</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>165</v>
+        <v>23</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>177</v>
+        <v>44</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="30" t="n">
-        <v>44325</v>
-      </c>
-      <c r="B96" s="39" t="s">
+      <c r="A96" s="28" t="n">
+        <v>44326</v>
+      </c>
+      <c r="B96" s="33" t="s">
         <v>223</v>
       </c>
       <c r="C96" s="5" t="s">
@@ -3888,35 +3905,35 @@
         <v>224</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F96" s="16" t="s">
-        <v>36</v>
+        <v>167</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="28" t="n">
+      <c r="A97" s="30" t="n">
         <v>44325</v>
       </c>
-      <c r="B97" s="33" t="s">
+      <c r="B97" s="39" t="s">
         <v>225</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="D97" s="5" t="s">
         <v>226</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F97" s="5" t="s">
-        <v>44</v>
+        <v>167</v>
+      </c>
+      <c r="F97" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="28" t="n">
-        <v>44321</v>
+        <v>44325</v>
       </c>
       <c r="B98" s="33" t="s">
         <v>227</v>
@@ -3928,15 +3945,15 @@
         <v>228</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F98" s="23" t="s">
-        <v>114</v>
+        <v>23</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="28" t="n">
-        <v>44316</v>
+        <v>44321</v>
       </c>
       <c r="B99" s="33" t="s">
         <v>229</v>
@@ -3948,37 +3965,37 @@
         <v>230</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F99" s="5" t="s">
-        <v>231</v>
+        <v>39</v>
+      </c>
+      <c r="F99" s="22" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="28" t="n">
-        <v>44279</v>
-      </c>
-      <c r="B100" s="5" t="s">
+        <v>44316</v>
+      </c>
+      <c r="B100" s="33" t="s">
+        <v>231</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="C100" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D100" s="5" t="s">
+      <c r="E100" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F100" s="5" t="s">
         <v>233</v>
-      </c>
-      <c r="E100" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F100" s="16" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="28" t="n">
-        <v>44257</v>
-      </c>
-      <c r="B101" s="33" t="s">
+        <v>44279</v>
+      </c>
+      <c r="B101" s="5" t="s">
         <v>234</v>
       </c>
       <c r="C101" s="5" t="s">
@@ -3988,15 +4005,15 @@
         <v>235</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F101" s="5" t="s">
-        <v>44</v>
+        <v>23</v>
+      </c>
+      <c r="F101" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="28" t="n">
-        <v>44243</v>
+        <v>44257</v>
       </c>
       <c r="B102" s="33" t="s">
         <v>236</v>
@@ -4008,57 +4025,57 @@
         <v>237</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F102" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="40" t="n">
+      <c r="A103" s="28" t="n">
+        <v>44243</v>
+      </c>
+      <c r="B103" s="33" t="s">
+        <v>238</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="40" t="n">
         <v>44231</v>
       </c>
-      <c r="B103" s="41" t="s">
-        <v>238</v>
-      </c>
-      <c r="C103" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="D103" s="42" t="s">
-        <v>184</v>
-      </c>
-      <c r="E103" s="42" t="s">
-        <v>165</v>
-      </c>
-      <c r="F103" s="42" t="s">
+      <c r="B104" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="C104" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D104" s="42" t="s">
+        <v>186</v>
+      </c>
+      <c r="E104" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="F104" s="42" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="28" t="n">
-        <v>44218</v>
-      </c>
-      <c r="B104" s="33" t="s">
-        <v>239</v>
-      </c>
-      <c r="C104" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D104" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="E104" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F104" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="28" t="n">
-        <v>44216</v>
-      </c>
-      <c r="B105" s="36" t="s">
+        <v>44218</v>
+      </c>
+      <c r="B105" s="33" t="s">
         <v>241</v>
       </c>
       <c r="C105" s="5" t="s">
@@ -4068,17 +4085,17 @@
         <v>242</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F105" s="16" t="s">
-        <v>36</v>
+        <v>167</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="28" t="n">
-        <v>44175</v>
-      </c>
-      <c r="B106" s="33" t="s">
+        <v>44216</v>
+      </c>
+      <c r="B106" s="36" t="s">
         <v>243</v>
       </c>
       <c r="C106" s="5" t="s">
@@ -4088,10 +4105,10 @@
         <v>244</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F106" s="5" t="s">
-        <v>44</v>
+        <v>23</v>
+      </c>
+      <c r="F106" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4108,40 +4125,40 @@
         <v>246</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>23</v>
+        <v>167</v>
       </c>
       <c r="F107" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="28" t="n">
-        <v>44162</v>
-      </c>
-      <c r="B109" s="33" t="s">
+    <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="28" t="n">
+        <v>44175</v>
+      </c>
+      <c r="B108" s="33" t="s">
         <v>247</v>
       </c>
-      <c r="C109" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D109" s="5" t="s">
+      <c r="C108" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D108" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="E109" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F109" s="5" t="s">
+      <c r="E108" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F108" s="5" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="5" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="28" t="n">
-        <v>44148</v>
+        <v>44162</v>
       </c>
       <c r="B110" s="33" t="s">
         <v>249</v>
@@ -4150,124 +4167,124 @@
         <v>7</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>8</v>
+        <v>250</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>165</v>
+        <v>39</v>
       </c>
       <c r="F110" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="40" t="n">
+      <c r="A111" s="28" t="n">
+        <v>44148</v>
+      </c>
+      <c r="B111" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E111" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="40" t="n">
         <v>44146</v>
       </c>
-      <c r="B111" s="41" t="s">
-        <v>250</v>
-      </c>
-      <c r="C111" s="42" t="s">
+      <c r="B112" s="41" t="s">
+        <v>252</v>
+      </c>
+      <c r="C112" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D111" s="42" t="s">
-        <v>251</v>
-      </c>
-      <c r="E111" s="42" t="s">
-        <v>165</v>
-      </c>
-      <c r="F111" s="42" t="s">
+      <c r="D112" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="E112" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="F112" s="42" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="28" t="n">
-        <v>44132</v>
-      </c>
-      <c r="B112" s="33" t="s">
-        <v>238</v>
-      </c>
-      <c r="C112" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D112" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="E112" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F112" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="28" t="n">
-        <v>44103</v>
+        <v>44132</v>
       </c>
       <c r="B113" s="33" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>254</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F113" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="40" t="n">
+      <c r="A114" s="28" t="n">
+        <v>44103</v>
+      </c>
+      <c r="B114" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="40" t="n">
         <v>44095</v>
       </c>
-      <c r="B114" s="41" t="s">
-        <v>255</v>
-      </c>
-      <c r="C114" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="D114" s="42" t="s">
-        <v>256</v>
-      </c>
-      <c r="E114" s="42" t="s">
+      <c r="B115" s="41" t="s">
+        <v>257</v>
+      </c>
+      <c r="C115" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D115" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="E115" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="F114" s="42" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="28" t="n">
-        <v>44095</v>
-      </c>
-      <c r="B115" s="33" t="s">
-        <v>257</v>
-      </c>
-      <c r="C115" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D115" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="E115" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F115" s="12" t="s">
-        <v>32</v>
+      <c r="F115" s="42" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="28" t="n">
-        <v>44057</v>
+        <v>44095</v>
       </c>
       <c r="B116" s="33" t="s">
         <v>259</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>260</v>
@@ -4275,33 +4292,33 @@
       <c r="E116" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F116" s="5" t="s">
-        <v>216</v>
+      <c r="F116" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="28" t="n">
-        <v>44028</v>
+        <v>44057</v>
       </c>
       <c r="B117" s="33" t="s">
         <v>261</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>262</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F117" s="12" t="s">
-        <v>32</v>
+        <v>39</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="28" t="n">
-        <v>44064</v>
+        <v>44028</v>
       </c>
       <c r="B118" s="33" t="s">
         <v>263</v>
@@ -4313,15 +4330,15 @@
         <v>264</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F118" s="5" t="s">
-        <v>44</v>
+        <v>167</v>
+      </c>
+      <c r="F118" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="28" t="n">
-        <v>44028</v>
+        <v>44064</v>
       </c>
       <c r="B119" s="33" t="s">
         <v>265</v>
@@ -4333,15 +4350,15 @@
         <v>266</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F119" s="12" t="s">
-        <v>32</v>
+        <v>167</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="28" t="n">
-        <v>44016</v>
+        <v>44028</v>
       </c>
       <c r="B120" s="33" t="s">
         <v>267</v>
@@ -4353,15 +4370,15 @@
         <v>268</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F120" s="5" t="s">
-        <v>44</v>
+        <v>167</v>
+      </c>
+      <c r="F120" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="28" t="n">
-        <v>44010</v>
+        <v>44016</v>
       </c>
       <c r="B121" s="33" t="s">
         <v>269</v>
@@ -4373,7 +4390,7 @@
         <v>270</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="F121" s="5" t="s">
         <v>44</v>
@@ -4381,19 +4398,19 @@
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="28" t="n">
-        <v>43995</v>
+        <v>44010</v>
       </c>
       <c r="B122" s="33" t="s">
         <v>271</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>272</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F122" s="5" t="s">
         <v>44</v>
@@ -4401,7 +4418,7 @@
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="28" t="n">
-        <v>43948</v>
+        <v>43995</v>
       </c>
       <c r="B123" s="33" t="s">
         <v>273</v>
@@ -4413,15 +4430,15 @@
         <v>274</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F123" s="12" t="s">
-        <v>32</v>
+        <v>39</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="28" t="n">
-        <v>43947</v>
+        <v>43948</v>
       </c>
       <c r="B124" s="33" t="s">
         <v>275</v>
@@ -4433,15 +4450,15 @@
         <v>276</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F124" s="16" t="s">
-        <v>36</v>
+        <v>167</v>
+      </c>
+      <c r="F124" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="28" t="n">
-        <v>43936</v>
+        <v>43947</v>
       </c>
       <c r="B125" s="33" t="s">
         <v>277</v>
@@ -4453,27 +4470,27 @@
         <v>278</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F125" s="5" t="s">
-        <v>44</v>
+        <v>167</v>
+      </c>
+      <c r="F125" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="28" t="n">
-        <v>43929</v>
+        <v>43936</v>
       </c>
       <c r="B126" s="33" t="s">
         <v>279</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D126" s="5" t="s">
         <v>280</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>165</v>
+        <v>39</v>
       </c>
       <c r="F126" s="5" t="s">
         <v>44</v>
@@ -4481,7 +4498,7 @@
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="28" t="n">
-        <v>43891</v>
+        <v>43929</v>
       </c>
       <c r="B127" s="33" t="s">
         <v>281</v>
@@ -4493,15 +4510,15 @@
         <v>282</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F127" s="12" t="s">
-        <v>32</v>
+        <v>167</v>
+      </c>
+      <c r="F127" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="28" t="n">
-        <v>43885</v>
+        <v>43891</v>
       </c>
       <c r="B128" s="33" t="s">
         <v>283</v>
@@ -4513,15 +4530,15 @@
         <v>284</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F128" s="5" t="s">
-        <v>44</v>
+        <v>167</v>
+      </c>
+      <c r="F128" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="28" t="n">
-        <v>43857</v>
+        <v>43885</v>
       </c>
       <c r="B129" s="33" t="s">
         <v>285</v>
@@ -4533,7 +4550,7 @@
         <v>286</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F129" s="5" t="s">
         <v>44</v>
@@ -4553,7 +4570,7 @@
         <v>288</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F130" s="5" t="s">
         <v>44</v>
@@ -4561,7 +4578,7 @@
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="28" t="n">
-        <v>43852</v>
+        <v>43857</v>
       </c>
       <c r="B131" s="33" t="s">
         <v>289</v>
@@ -4573,7 +4590,7 @@
         <v>290</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F131" s="5" t="s">
         <v>44</v>
@@ -4581,7 +4598,7 @@
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="28" t="n">
-        <v>43584</v>
+        <v>43852</v>
       </c>
       <c r="B132" s="33" t="s">
         <v>291</v>
@@ -4593,7 +4610,7 @@
         <v>292</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>23</v>
+        <v>167</v>
       </c>
       <c r="F132" s="5" t="s">
         <v>44</v>
@@ -4621,9 +4638,9 @@
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="28" t="n">
-        <v>43540</v>
-      </c>
-      <c r="B134" s="5" t="s">
+        <v>43584</v>
+      </c>
+      <c r="B134" s="33" t="s">
         <v>295</v>
       </c>
       <c r="C134" s="5" t="s">
@@ -4639,29 +4656,29 @@
         <v>44</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="28" t="n">
-        <v>43203</v>
-      </c>
-      <c r="B136" s="43" t="s">
+    <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="28" t="n">
+        <v>43540</v>
+      </c>
+      <c r="B135" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="C136" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D136" s="5" t="s">
+      <c r="C135" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D135" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="E136" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F136" s="16" t="s">
-        <v>36</v>
+      <c r="E135" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F135" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="5" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4678,55 +4695,55 @@
         <v>300</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F137" s="5" t="s">
-        <v>301</v>
+        <v>167</v>
+      </c>
+      <c r="F137" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="28" t="n">
-        <v>42842</v>
+        <v>43203</v>
       </c>
       <c r="B138" s="43" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C138" s="5" t="s">
         <v>63</v>
       </c>
       <c r="D138" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="E138" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F138" s="5" t="s">
         <v>303</v>
-      </c>
-      <c r="E138" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F138" s="16" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="28" t="n">
-        <v>42457</v>
-      </c>
-      <c r="B139" s="5" t="s">
+        <v>42842</v>
+      </c>
+      <c r="B139" s="43" t="s">
         <v>304</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="D139" s="5" t="s">
         <v>305</v>
       </c>
       <c r="E139" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F139" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="F139" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="28" t="n">
-        <v>39028</v>
+        <v>42457</v>
       </c>
       <c r="B140" s="5" t="s">
         <v>306</v>
@@ -4738,21 +4755,41 @@
         <v>307</v>
       </c>
       <c r="E140" s="5" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F140" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="142" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AMG142" s="0"/>
-      <c r="AMH142" s="0"/>
-      <c r="AMI142" s="0"/>
-      <c r="AMJ142" s="0"/>
+    <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="28" t="n">
+        <v>39028</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="C141" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D141" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="E141" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F141" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="143" s="25" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMG143" s="0"/>
+      <c r="AMH143" s="0"/>
+      <c r="AMI143" s="0"/>
+      <c r="AMJ143" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A:F"/>
-  <conditionalFormatting sqref="F91:F1048576 F1:F89">
+  <autoFilter ref="A1:F141"/>
+  <conditionalFormatting sqref="F92:F1048576 F1:F90">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="resolved" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("resolved",F1)))</formula>
     </cfRule>
@@ -4804,92 +4841,93 @@
     <hyperlink ref="B46" r:id="rId41" display="#1164"/>
     <hyperlink ref="B47" r:id="rId42" display="#9"/>
     <hyperlink ref="B48" r:id="rId43" display="#1163"/>
-    <hyperlink ref="B49" r:id="rId44" display="#1161"/>
-    <hyperlink ref="B50" r:id="rId45" display="#1690"/>
-    <hyperlink ref="B52" r:id="rId46" display="#1155"/>
-    <hyperlink ref="B53" r:id="rId47" display="#1150"/>
-    <hyperlink ref="B54" r:id="rId48" display="#1151"/>
-    <hyperlink ref="B55" r:id="rId49" display="#1200"/>
-    <hyperlink ref="B56" r:id="rId50" display="#1681"/>
-    <hyperlink ref="B57" r:id="rId51" display="#51"/>
-    <hyperlink ref="B58" r:id="rId52" display="#1142"/>
-    <hyperlink ref="B59" r:id="rId53" display="#8"/>
-    <hyperlink ref="B60" r:id="rId54" display="#1674"/>
-    <hyperlink ref="B61" r:id="rId55" display="#1672"/>
-    <hyperlink ref="B62" r:id="rId56" display="#1669"/>
-    <hyperlink ref="B63" r:id="rId57" display="#1670"/>
-    <hyperlink ref="B64" r:id="rId58" display="#1184"/>
-    <hyperlink ref="B65" r:id="rId59" display="#49"/>
-    <hyperlink ref="B66" r:id="rId60" display="#1140"/>
-    <hyperlink ref="B67" r:id="rId61" display="#1132"/>
-    <hyperlink ref="B69" r:id="rId62" display="#1125"/>
-    <hyperlink ref="B70" r:id="rId63" display="#1641"/>
-    <hyperlink ref="B71" r:id="rId64" display="#1124"/>
-    <hyperlink ref="B72" r:id="rId65" display="#1122"/>
-    <hyperlink ref="B73" r:id="rId66" display="#43"/>
-    <hyperlink ref="B74" r:id="rId67" display="#1622"/>
-    <hyperlink ref="B76" r:id="rId68" display="#38"/>
-    <hyperlink ref="B77" r:id="rId69" display="#1621"/>
-    <hyperlink ref="B78" r:id="rId70" display="#1616"/>
-    <hyperlink ref="B79" r:id="rId71" display="#37"/>
-    <hyperlink ref="B80" r:id="rId72" display="#36"/>
-    <hyperlink ref="B81" r:id="rId73" display="#1101"/>
-    <hyperlink ref="B82" r:id="rId74" display="#1099"/>
-    <hyperlink ref="B83" r:id="rId75" display="#1098"/>
-    <hyperlink ref="B84" r:id="rId76" display="#1617"/>
-    <hyperlink ref="B85" r:id="rId77" display="#1092"/>
-    <hyperlink ref="B86" r:id="rId78" display="#1128"/>
-    <hyperlink ref="B87" r:id="rId79" display="#1090"/>
-    <hyperlink ref="B88" r:id="rId80" display="#1608"/>
-    <hyperlink ref="B89" r:id="rId81" display="#35"/>
-    <hyperlink ref="B91" r:id="rId82" display="#1070"/>
-    <hyperlink ref="B92" r:id="rId83" display="#1592"/>
-    <hyperlink ref="B93" r:id="rId84" display="#1591"/>
-    <hyperlink ref="B94" r:id="rId85" display="#1578"/>
-    <hyperlink ref="B95" r:id="rId86" display="#41"/>
-    <hyperlink ref="B96" r:id="rId87" display="#42"/>
-    <hyperlink ref="B97" r:id="rId88" display="#1566"/>
-    <hyperlink ref="B98" r:id="rId89" display="#1565"/>
-    <hyperlink ref="B99" r:id="rId90" display="#1046"/>
-    <hyperlink ref="B100" r:id="rId91" display="#1559"/>
-    <hyperlink ref="B101" r:id="rId92" display="#1038"/>
-    <hyperlink ref="B102" r:id="rId93" display="#1037"/>
-    <hyperlink ref="B103" r:id="rId94" display="#1020"/>
-    <hyperlink ref="B104" r:id="rId95" display="#1032"/>
-    <hyperlink ref="B105" r:id="rId96" display="#1546"/>
-    <hyperlink ref="B106" r:id="rId97" display="#1027"/>
-    <hyperlink ref="B107" r:id="rId98" display="#1529"/>
-    <hyperlink ref="B109" r:id="rId99" display="#1527"/>
-    <hyperlink ref="B110" r:id="rId100" display="#558"/>
-    <hyperlink ref="B111" r:id="rId101" display="#1005"/>
-    <hyperlink ref="B112" r:id="rId102" display="#1020"/>
-    <hyperlink ref="B113" r:id="rId103" display="#993"/>
-    <hyperlink ref="B114" r:id="rId104" display="#1520"/>
-    <hyperlink ref="B115" r:id="rId105" display="#1519"/>
-    <hyperlink ref="B116" r:id="rId106" display="#969"/>
-    <hyperlink ref="B117" r:id="rId107" display="#1003"/>
-    <hyperlink ref="B118" r:id="rId108" display="#1015"/>
-    <hyperlink ref="B119" r:id="rId109" display="#1002"/>
-    <hyperlink ref="B120" r:id="rId110" display="#1471"/>
-    <hyperlink ref="B121" r:id="rId111" display="#1497"/>
-    <hyperlink ref="B122" r:id="rId112" display="#947"/>
-    <hyperlink ref="B123" r:id="rId113" display="#933"/>
-    <hyperlink ref="B124" r:id="rId114" display="#932"/>
-    <hyperlink ref="B125" r:id="rId115" display="#931"/>
-    <hyperlink ref="B126" r:id="rId116" display="#987"/>
-    <hyperlink ref="B127" r:id="rId117" display="#988"/>
-    <hyperlink ref="B128" r:id="rId118" display="#982"/>
-    <hyperlink ref="B129" r:id="rId119" display="#979"/>
-    <hyperlink ref="B130" r:id="rId120" display="#977"/>
-    <hyperlink ref="B131" r:id="rId121" display="#975"/>
-    <hyperlink ref="B132" r:id="rId122" display="#1445"/>
-    <hyperlink ref="B133" r:id="rId123" display="#1444"/>
-    <hyperlink ref="B134" r:id="rId124" display="#1427"/>
-    <hyperlink ref="B136" r:id="rId125" display="#23"/>
-    <hyperlink ref="B137" r:id="rId126" display="#22"/>
-    <hyperlink ref="B138" r:id="rId127" display="#18"/>
-    <hyperlink ref="B139" r:id="rId128" display="#1207"/>
-    <hyperlink ref="B140" r:id="rId129" display="#245"/>
+    <hyperlink ref="B49" r:id="rId44" display="#1695"/>
+    <hyperlink ref="B50" r:id="rId45" display="#1161"/>
+    <hyperlink ref="B51" r:id="rId46" display="#1690"/>
+    <hyperlink ref="B53" r:id="rId47" display="#1155"/>
+    <hyperlink ref="B54" r:id="rId48" display="#1150"/>
+    <hyperlink ref="B55" r:id="rId49" display="#1151"/>
+    <hyperlink ref="B56" r:id="rId50" display="#1200"/>
+    <hyperlink ref="B57" r:id="rId51" display="#1681"/>
+    <hyperlink ref="B58" r:id="rId52" display="#51"/>
+    <hyperlink ref="B59" r:id="rId53" display="#1142"/>
+    <hyperlink ref="B60" r:id="rId54" display="#8"/>
+    <hyperlink ref="B61" r:id="rId55" display="#1674"/>
+    <hyperlink ref="B62" r:id="rId56" display="#1672"/>
+    <hyperlink ref="B63" r:id="rId57" display="#1669"/>
+    <hyperlink ref="B64" r:id="rId58" display="#1670"/>
+    <hyperlink ref="B65" r:id="rId59" display="#1184"/>
+    <hyperlink ref="B66" r:id="rId60" display="#49"/>
+    <hyperlink ref="B67" r:id="rId61" display="#1140"/>
+    <hyperlink ref="B68" r:id="rId62" display="#1132"/>
+    <hyperlink ref="B70" r:id="rId63" display="#1125"/>
+    <hyperlink ref="B71" r:id="rId64" display="#1641"/>
+    <hyperlink ref="B72" r:id="rId65" display="#1124"/>
+    <hyperlink ref="B73" r:id="rId66" display="#1122"/>
+    <hyperlink ref="B74" r:id="rId67" display="#43"/>
+    <hyperlink ref="B75" r:id="rId68" display="#1622"/>
+    <hyperlink ref="B77" r:id="rId69" display="#38"/>
+    <hyperlink ref="B78" r:id="rId70" display="#1621"/>
+    <hyperlink ref="B79" r:id="rId71" display="#1616"/>
+    <hyperlink ref="B80" r:id="rId72" display="#37"/>
+    <hyperlink ref="B81" r:id="rId73" display="#36"/>
+    <hyperlink ref="B82" r:id="rId74" display="#1101"/>
+    <hyperlink ref="B83" r:id="rId75" display="#1099"/>
+    <hyperlink ref="B84" r:id="rId76" display="#1098"/>
+    <hyperlink ref="B85" r:id="rId77" display="#1617"/>
+    <hyperlink ref="B86" r:id="rId78" display="#1092"/>
+    <hyperlink ref="B87" r:id="rId79" display="#1128"/>
+    <hyperlink ref="B88" r:id="rId80" display="#1090"/>
+    <hyperlink ref="B89" r:id="rId81" display="#1608"/>
+    <hyperlink ref="B90" r:id="rId82" display="#35"/>
+    <hyperlink ref="B92" r:id="rId83" display="#1070"/>
+    <hyperlink ref="B93" r:id="rId84" display="#1592"/>
+    <hyperlink ref="B94" r:id="rId85" display="#1591"/>
+    <hyperlink ref="B95" r:id="rId86" display="#1578"/>
+    <hyperlink ref="B96" r:id="rId87" display="#41"/>
+    <hyperlink ref="B97" r:id="rId88" display="#42"/>
+    <hyperlink ref="B98" r:id="rId89" display="#1566"/>
+    <hyperlink ref="B99" r:id="rId90" display="#1565"/>
+    <hyperlink ref="B100" r:id="rId91" display="#1046"/>
+    <hyperlink ref="B101" r:id="rId92" display="#1559"/>
+    <hyperlink ref="B102" r:id="rId93" display="#1038"/>
+    <hyperlink ref="B103" r:id="rId94" display="#1037"/>
+    <hyperlink ref="B104" r:id="rId95" display="#1020"/>
+    <hyperlink ref="B105" r:id="rId96" display="#1032"/>
+    <hyperlink ref="B106" r:id="rId97" display="#1546"/>
+    <hyperlink ref="B107" r:id="rId98" display="#1027"/>
+    <hyperlink ref="B108" r:id="rId99" display="#1529"/>
+    <hyperlink ref="B110" r:id="rId100" display="#1527"/>
+    <hyperlink ref="B111" r:id="rId101" display="#558"/>
+    <hyperlink ref="B112" r:id="rId102" display="#1005"/>
+    <hyperlink ref="B113" r:id="rId103" display="#1020"/>
+    <hyperlink ref="B114" r:id="rId104" display="#993"/>
+    <hyperlink ref="B115" r:id="rId105" display="#1520"/>
+    <hyperlink ref="B116" r:id="rId106" display="#1519"/>
+    <hyperlink ref="B117" r:id="rId107" display="#969"/>
+    <hyperlink ref="B118" r:id="rId108" display="#1003"/>
+    <hyperlink ref="B119" r:id="rId109" display="#1015"/>
+    <hyperlink ref="B120" r:id="rId110" display="#1002"/>
+    <hyperlink ref="B121" r:id="rId111" display="#1471"/>
+    <hyperlink ref="B122" r:id="rId112" display="#1497"/>
+    <hyperlink ref="B123" r:id="rId113" display="#947"/>
+    <hyperlink ref="B124" r:id="rId114" display="#933"/>
+    <hyperlink ref="B125" r:id="rId115" display="#932"/>
+    <hyperlink ref="B126" r:id="rId116" display="#931"/>
+    <hyperlink ref="B127" r:id="rId117" display="#987"/>
+    <hyperlink ref="B128" r:id="rId118" display="#988"/>
+    <hyperlink ref="B129" r:id="rId119" display="#982"/>
+    <hyperlink ref="B130" r:id="rId120" display="#979"/>
+    <hyperlink ref="B131" r:id="rId121" display="#977"/>
+    <hyperlink ref="B132" r:id="rId122" display="#975"/>
+    <hyperlink ref="B133" r:id="rId123" display="#1445"/>
+    <hyperlink ref="B134" r:id="rId124" display="#1444"/>
+    <hyperlink ref="B135" r:id="rId125" display="#1427"/>
+    <hyperlink ref="B137" r:id="rId126" display="#23"/>
+    <hyperlink ref="B138" r:id="rId127" display="#22"/>
+    <hyperlink ref="B139" r:id="rId128" display="#18"/>
+    <hyperlink ref="B140" r:id="rId129" display="#1207"/>
+    <hyperlink ref="B141" r:id="rId130" display="#245"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
@@ -4898,7 +4936,7 @@
     <oddHeader>&amp;C&amp;"Sans,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Sans,Regular"Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId130"/>
+  <drawing r:id="rId131"/>
 </worksheet>
 </file>
 
@@ -4931,10 +4969,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -4943,10 +4981,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated info in ticket 1323 > 51 > 276
</commit_message>
<xml_diff>
--- a/docs/tools/tickets/OmegaT_issues_nopw.xlsx
+++ b/docs/tools/tickets/OmegaT_issues_nopw.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="322">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t xml:space="preserve">#1323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Migrated</t>
   </si>
   <si>
     <t xml:space="preserve">#30</t>
@@ -1866,15 +1869,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ149"/>
+  <dimension ref="A1:AMN149"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
@@ -1914,8 +1917,12 @@
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
+      <c r="AMK1" s="0"/>
+      <c r="AML1" s="0"/>
+      <c r="AMM1" s="0"/>
+      <c r="AMN1" s="0"/>
     </row>
-    <row r="2" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="8" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
         <v>28</v>
       </c>
@@ -1926,6 +1933,10 @@
       <c r="AMH2" s="0"/>
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
+      <c r="AMK2" s="0"/>
+      <c r="AML2" s="0"/>
+      <c r="AMM2" s="0"/>
+      <c r="AMN2" s="0"/>
     </row>
     <row r="3" s="8" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9"/>
@@ -1938,8 +1949,12 @@
       <c r="AMH3" s="0"/>
       <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
+      <c r="AMK3" s="0"/>
+      <c r="AML3" s="0"/>
+      <c r="AMM3" s="0"/>
+      <c r="AMN3" s="0"/>
     </row>
-    <row r="4" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="8" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="n">
         <v>45849</v>
       </c>
@@ -1962,8 +1977,12 @@
       <c r="AMH4" s="0"/>
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
+      <c r="AMK4" s="0"/>
+      <c r="AML4" s="0"/>
+      <c r="AMM4" s="0"/>
+      <c r="AMN4" s="0"/>
     </row>
-    <row r="5" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="8" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="n">
         <v>45849</v>
       </c>
@@ -1986,6 +2005,10 @@
       <c r="AMH5" s="0"/>
       <c r="AMI5" s="0"/>
       <c r="AMJ5" s="0"/>
+      <c r="AMK5" s="0"/>
+      <c r="AML5" s="0"/>
+      <c r="AMM5" s="0"/>
+      <c r="AMN5" s="0"/>
     </row>
     <row r="6" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="n">
@@ -2010,8 +2033,12 @@
       <c r="AMH6" s="0"/>
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
+      <c r="AMK6" s="0"/>
+      <c r="AML6" s="0"/>
+      <c r="AMM6" s="0"/>
+      <c r="AMN6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="n">
         <v>45814</v>
       </c>
@@ -3045,7 +3072,7 @@
       <c r="AME7" s="8"/>
       <c r="AMF7" s="8"/>
     </row>
-    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="n">
         <v>45677</v>
       </c>
@@ -4079,7 +4106,7 @@
       <c r="AME8" s="8"/>
       <c r="AMF8" s="8"/>
     </row>
-    <row r="9" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="8" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
         <v>44</v>
       </c>
@@ -4090,8 +4117,12 @@
       <c r="AMH9" s="0"/>
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
+      <c r="AMK9" s="0"/>
+      <c r="AML9" s="0"/>
+      <c r="AMM9" s="0"/>
+      <c r="AMN9" s="0"/>
     </row>
-    <row r="10" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="8" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="n">
         <v>45629</v>
       </c>
@@ -4114,8 +4145,12 @@
       <c r="AMH10" s="0"/>
       <c r="AMI10" s="0"/>
       <c r="AMJ10" s="0"/>
+      <c r="AMK10" s="0"/>
+      <c r="AML10" s="0"/>
+      <c r="AMM10" s="0"/>
+      <c r="AMN10" s="0"/>
     </row>
-    <row r="11" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="8" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="n">
         <v>45609</v>
       </c>
@@ -4138,8 +4173,12 @@
       <c r="AMH11" s="0"/>
       <c r="AMI11" s="0"/>
       <c r="AMJ11" s="0"/>
+      <c r="AMK11" s="0"/>
+      <c r="AML11" s="0"/>
+      <c r="AMM11" s="0"/>
+      <c r="AMN11" s="0"/>
     </row>
-    <row r="12" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="8" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="n">
         <v>45604</v>
       </c>
@@ -4162,8 +4201,12 @@
       <c r="AMH12" s="0"/>
       <c r="AMI12" s="0"/>
       <c r="AMJ12" s="0"/>
+      <c r="AMK12" s="0"/>
+      <c r="AML12" s="0"/>
+      <c r="AMM12" s="0"/>
+      <c r="AMN12" s="0"/>
     </row>
-    <row r="13" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" s="8" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="n">
         <v>45568</v>
       </c>
@@ -4186,8 +4229,12 @@
       <c r="AMH13" s="0"/>
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
+      <c r="AMK13" s="0"/>
+      <c r="AML13" s="0"/>
+      <c r="AMM13" s="0"/>
+      <c r="AMN13" s="0"/>
     </row>
-    <row r="14" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="8" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="n">
         <v>45563</v>
       </c>
@@ -5224,8 +5271,12 @@
       <c r="AMH14" s="0"/>
       <c r="AMI14" s="0"/>
       <c r="AMJ14" s="0"/>
+      <c r="AMK14" s="0"/>
+      <c r="AML14" s="0"/>
+      <c r="AMM14" s="0"/>
+      <c r="AMN14" s="0"/>
     </row>
-    <row r="15" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="11" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="n">
         <v>45488</v>
       </c>
@@ -5248,8 +5299,12 @@
       <c r="AMH15" s="0"/>
       <c r="AMI15" s="0"/>
       <c r="AMJ15" s="0"/>
+      <c r="AMK15" s="0"/>
+      <c r="AML15" s="0"/>
+      <c r="AMM15" s="0"/>
+      <c r="AMN15" s="0"/>
     </row>
-    <row r="16" s="11" customFormat="true" ht="11.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" s="11" customFormat="true" ht="11.15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="n">
         <v>45488</v>
       </c>
@@ -6286,8 +6341,12 @@
       <c r="AMH16" s="0"/>
       <c r="AMI16" s="0"/>
       <c r="AMJ16" s="0"/>
+      <c r="AMK16" s="0"/>
+      <c r="AML16" s="0"/>
+      <c r="AMM16" s="0"/>
+      <c r="AMN16" s="0"/>
     </row>
-    <row r="17" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="8" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="n">
         <v>45483</v>
       </c>
@@ -6310,8 +6369,12 @@
       <c r="AMH17" s="0"/>
       <c r="AMI17" s="0"/>
       <c r="AMJ17" s="0"/>
+      <c r="AMK17" s="0"/>
+      <c r="AML17" s="0"/>
+      <c r="AMM17" s="0"/>
+      <c r="AMN17" s="0"/>
     </row>
-    <row r="18" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" s="8" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="n">
         <v>45469</v>
       </c>
@@ -6334,8 +6397,12 @@
       <c r="AMH18" s="0"/>
       <c r="AMI18" s="0"/>
       <c r="AMJ18" s="0"/>
+      <c r="AMK18" s="0"/>
+      <c r="AML18" s="0"/>
+      <c r="AMM18" s="0"/>
+      <c r="AMN18" s="0"/>
     </row>
-    <row r="19" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" s="8" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="n">
         <v>45784</v>
       </c>
@@ -6358,8 +6425,12 @@
       <c r="AMH19" s="0"/>
       <c r="AMI19" s="0"/>
       <c r="AMJ19" s="0"/>
+      <c r="AMK19" s="0"/>
+      <c r="AML19" s="0"/>
+      <c r="AMM19" s="0"/>
+      <c r="AMN19" s="0"/>
     </row>
-    <row r="20" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" s="8" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13" t="n">
         <v>45411</v>
       </c>
@@ -6382,8 +6453,12 @@
       <c r="AMH20" s="0"/>
       <c r="AMI20" s="0"/>
       <c r="AMJ20" s="0"/>
+      <c r="AMK20" s="0"/>
+      <c r="AML20" s="0"/>
+      <c r="AMM20" s="0"/>
+      <c r="AMN20" s="0"/>
     </row>
-    <row r="21" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="8" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="n">
         <v>45394</v>
       </c>
@@ -7420,8 +7495,12 @@
       <c r="AMH21" s="0"/>
       <c r="AMI21" s="0"/>
       <c r="AMJ21" s="0"/>
+      <c r="AMK21" s="0"/>
+      <c r="AML21" s="0"/>
+      <c r="AMM21" s="0"/>
+      <c r="AMN21" s="0"/>
     </row>
-    <row r="22" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="n">
         <v>45390</v>
       </c>
@@ -7444,8 +7523,12 @@
       <c r="AMH22" s="0"/>
       <c r="AMI22" s="0"/>
       <c r="AMJ22" s="0"/>
+      <c r="AMK22" s="0"/>
+      <c r="AML22" s="0"/>
+      <c r="AMM22" s="0"/>
+      <c r="AMN22" s="0"/>
     </row>
-    <row r="23" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="n">
         <v>45365</v>
       </c>
@@ -7468,8 +7551,12 @@
       <c r="AMH23" s="0"/>
       <c r="AMI23" s="0"/>
       <c r="AMJ23" s="0"/>
+      <c r="AMK23" s="0"/>
+      <c r="AML23" s="0"/>
+      <c r="AMM23" s="0"/>
+      <c r="AMN23" s="0"/>
     </row>
-    <row r="24" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="n">
         <v>45363</v>
       </c>
@@ -7492,8 +7579,12 @@
       <c r="AMH24" s="0"/>
       <c r="AMI24" s="0"/>
       <c r="AMJ24" s="0"/>
+      <c r="AMK24" s="0"/>
+      <c r="AML24" s="0"/>
+      <c r="AMM24" s="0"/>
+      <c r="AMN24" s="0"/>
     </row>
-    <row r="25" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" s="11" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
         <v>78</v>
       </c>
@@ -8522,8 +8613,12 @@
       <c r="AMH25" s="0"/>
       <c r="AMI25" s="0"/>
       <c r="AMJ25" s="0"/>
+      <c r="AMK25" s="0"/>
+      <c r="AML25" s="0"/>
+      <c r="AMM25" s="0"/>
+      <c r="AMN25" s="0"/>
     </row>
-    <row r="26" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" s="8" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="n">
         <v>45238</v>
       </c>
@@ -9560,8 +9655,12 @@
       <c r="AMH26" s="0"/>
       <c r="AMI26" s="0"/>
       <c r="AMJ26" s="0"/>
+      <c r="AMK26" s="0"/>
+      <c r="AML26" s="0"/>
+      <c r="AMM26" s="0"/>
+      <c r="AMN26" s="0"/>
     </row>
-    <row r="27" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="n">
         <v>45230</v>
       </c>
@@ -9584,8 +9683,12 @@
       <c r="AMH27" s="0"/>
       <c r="AMI27" s="0"/>
       <c r="AMJ27" s="0"/>
+      <c r="AMK27" s="0"/>
+      <c r="AML27" s="0"/>
+      <c r="AMM27" s="0"/>
+      <c r="AMN27" s="0"/>
     </row>
-    <row r="28" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="n">
         <v>45223</v>
       </c>
@@ -9608,8 +9711,12 @@
       <c r="AMH28" s="0"/>
       <c r="AMI28" s="0"/>
       <c r="AMJ28" s="0"/>
+      <c r="AMK28" s="0"/>
+      <c r="AML28" s="0"/>
+      <c r="AMM28" s="0"/>
+      <c r="AMN28" s="0"/>
     </row>
-    <row r="29" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="n">
         <v>45236</v>
       </c>
@@ -9632,8 +9739,12 @@
       <c r="AMH29" s="0"/>
       <c r="AMI29" s="0"/>
       <c r="AMJ29" s="0"/>
+      <c r="AMK29" s="0"/>
+      <c r="AML29" s="0"/>
+      <c r="AMM29" s="0"/>
+      <c r="AMN29" s="0"/>
     </row>
-    <row r="30" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="n">
         <v>45233</v>
       </c>
@@ -9656,8 +9767,12 @@
       <c r="AMH30" s="0"/>
       <c r="AMI30" s="0"/>
       <c r="AMJ30" s="0"/>
+      <c r="AMK30" s="0"/>
+      <c r="AML30" s="0"/>
+      <c r="AMM30" s="0"/>
+      <c r="AMN30" s="0"/>
     </row>
-    <row r="31" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="n">
         <v>45213</v>
       </c>
@@ -9680,43 +9795,51 @@
       <c r="AMH31" s="0"/>
       <c r="AMI31" s="0"/>
       <c r="AMJ31" s="0"/>
+      <c r="AMK31" s="0"/>
+      <c r="AML31" s="0"/>
+      <c r="AMM31" s="0"/>
+      <c r="AMN31" s="0"/>
     </row>
-    <row r="32" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="n">
+    <row r="32" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="18" t="n">
         <v>45199</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F32" s="11" t="s">
-        <v>34</v>
+      <c r="F32" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="AMG32" s="0"/>
       <c r="AMH32" s="0"/>
       <c r="AMI32" s="0"/>
       <c r="AMJ32" s="0"/>
+      <c r="AMK32" s="0"/>
+      <c r="AML32" s="0"/>
+      <c r="AMM32" s="0"/>
+      <c r="AMN32" s="0"/>
     </row>
-    <row r="33" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="n">
         <v>45170</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>33</v>
@@ -9728,19 +9851,23 @@
       <c r="AMH33" s="0"/>
       <c r="AMI33" s="0"/>
       <c r="AMJ33" s="0"/>
+      <c r="AMK33" s="0"/>
+      <c r="AML33" s="0"/>
+      <c r="AMM33" s="0"/>
+      <c r="AMN33" s="0"/>
     </row>
-    <row r="34" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="n">
         <v>45169</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E34" s="11" t="s">
         <v>33</v>
@@ -9752,13 +9879,17 @@
       <c r="AMH34" s="0"/>
       <c r="AMI34" s="0"/>
       <c r="AMJ34" s="0"/>
+      <c r="AMK34" s="0"/>
+      <c r="AML34" s="0"/>
+      <c r="AMM34" s="0"/>
+      <c r="AMN34" s="0"/>
     </row>
     <row r="35" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="18" t="n">
         <v>45169</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C35" s="20" t="s">
         <v>7</v>
@@ -9770,19 +9901,23 @@
         <v>9</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AMG35" s="0"/>
       <c r="AMH35" s="0"/>
       <c r="AMI35" s="0"/>
       <c r="AMJ35" s="0"/>
+      <c r="AMK35" s="0"/>
+      <c r="AML35" s="0"/>
+      <c r="AMM35" s="0"/>
+      <c r="AMN35" s="0"/>
     </row>
-    <row r="36" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="18" t="n">
         <v>45145</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C36" s="20" t="s">
         <v>7</v>
@@ -9794,25 +9929,29 @@
         <v>9</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AMG36" s="0"/>
       <c r="AMH36" s="0"/>
       <c r="AMI36" s="0"/>
       <c r="AMJ36" s="0"/>
+      <c r="AMK36" s="0"/>
+      <c r="AML36" s="0"/>
+      <c r="AMM36" s="0"/>
+      <c r="AMN36" s="0"/>
     </row>
-    <row r="37" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="n">
         <v>45145</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>9</v>
@@ -9824,19 +9963,23 @@
       <c r="AMH37" s="0"/>
       <c r="AMI37" s="0"/>
       <c r="AMJ37" s="0"/>
+      <c r="AMK37" s="0"/>
+      <c r="AML37" s="0"/>
+      <c r="AMM37" s="0"/>
+      <c r="AMN37" s="0"/>
     </row>
-    <row r="38" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="n">
         <v>45145</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C38" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E38" s="11" t="s">
         <v>9</v>
@@ -9848,8 +9991,12 @@
       <c r="AMH38" s="0"/>
       <c r="AMI38" s="0"/>
       <c r="AMJ38" s="0"/>
+      <c r="AMK38" s="0"/>
+      <c r="AML38" s="0"/>
+      <c r="AMM38" s="0"/>
+      <c r="AMN38" s="0"/>
     </row>
-    <row r="39" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="n">
         <v>45112</v>
       </c>
@@ -9857,7 +10004,7 @@
         <v>7</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F39" s="12" t="s">
         <v>43</v>
@@ -9866,19 +10013,23 @@
       <c r="AMH39" s="0"/>
       <c r="AMI39" s="0"/>
       <c r="AMJ39" s="0"/>
+      <c r="AMK39" s="0"/>
+      <c r="AML39" s="0"/>
+      <c r="AMM39" s="0"/>
+      <c r="AMN39" s="0"/>
     </row>
-    <row r="40" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="n">
         <v>45124</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>9</v>
@@ -9890,19 +10041,23 @@
       <c r="AMH40" s="0"/>
       <c r="AMI40" s="0"/>
       <c r="AMJ40" s="0"/>
+      <c r="AMK40" s="0"/>
+      <c r="AML40" s="0"/>
+      <c r="AMM40" s="0"/>
+      <c r="AMN40" s="0"/>
     </row>
-    <row r="41" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="n">
         <v>45119</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>33</v>
@@ -9914,19 +10069,23 @@
       <c r="AMH41" s="0"/>
       <c r="AMI41" s="0"/>
       <c r="AMJ41" s="0"/>
+      <c r="AMK41" s="0"/>
+      <c r="AML41" s="0"/>
+      <c r="AMM41" s="0"/>
+      <c r="AMN41" s="0"/>
     </row>
-    <row r="42" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="n">
         <v>45119</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E42" s="11" t="s">
         <v>33</v>
@@ -9938,19 +10097,23 @@
       <c r="AMH42" s="0"/>
       <c r="AMI42" s="0"/>
       <c r="AMJ42" s="0"/>
+      <c r="AMK42" s="0"/>
+      <c r="AML42" s="0"/>
+      <c r="AMM42" s="0"/>
+      <c r="AMN42" s="0"/>
     </row>
-    <row r="43" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="n">
         <v>45118</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>9</v>
@@ -9962,19 +10125,23 @@
       <c r="AMH43" s="0"/>
       <c r="AMI43" s="0"/>
       <c r="AMJ43" s="0"/>
+      <c r="AMK43" s="0"/>
+      <c r="AML43" s="0"/>
+      <c r="AMM43" s="0"/>
+      <c r="AMN43" s="0"/>
     </row>
-    <row r="44" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="n">
         <v>45118</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>9</v>
@@ -9986,19 +10153,23 @@
       <c r="AMH44" s="0"/>
       <c r="AMI44" s="0"/>
       <c r="AMJ44" s="0"/>
+      <c r="AMK44" s="0"/>
+      <c r="AML44" s="0"/>
+      <c r="AMM44" s="0"/>
+      <c r="AMN44" s="0"/>
     </row>
-    <row r="45" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="n">
         <v>45110</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E45" s="11" t="s">
         <v>33</v>
@@ -10010,43 +10181,51 @@
       <c r="AMH45" s="0"/>
       <c r="AMI45" s="0"/>
       <c r="AMJ45" s="0"/>
+      <c r="AMK45" s="0"/>
+      <c r="AML45" s="0"/>
+      <c r="AMM45" s="0"/>
+      <c r="AMN45" s="0"/>
     </row>
-    <row r="46" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="n">
         <v>45104</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E46" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F46" s="22" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AMG46" s="0"/>
       <c r="AMH46" s="0"/>
       <c r="AMI46" s="0"/>
       <c r="AMJ46" s="0"/>
+      <c r="AMK46" s="0"/>
+      <c r="AML46" s="0"/>
+      <c r="AMM46" s="0"/>
+      <c r="AMN46" s="0"/>
     </row>
-    <row r="47" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="n">
         <v>45094</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E47" s="11" t="s">
         <v>9</v>
@@ -10058,43 +10237,51 @@
       <c r="AMH47" s="0"/>
       <c r="AMI47" s="0"/>
       <c r="AMJ47" s="0"/>
+      <c r="AMK47" s="0"/>
+      <c r="AML47" s="0"/>
+      <c r="AMM47" s="0"/>
+      <c r="AMN47" s="0"/>
     </row>
-    <row r="48" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="n">
         <v>45069</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C48" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F48" s="23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AMG48" s="0"/>
       <c r="AMH48" s="0"/>
       <c r="AMI48" s="0"/>
       <c r="AMJ48" s="0"/>
+      <c r="AMK48" s="0"/>
+      <c r="AML48" s="0"/>
+      <c r="AMM48" s="0"/>
+      <c r="AMN48" s="0"/>
     </row>
-    <row r="49" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="n">
         <v>45069</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E49" s="11" t="s">
         <v>9</v>
@@ -10106,19 +10293,23 @@
       <c r="AMH49" s="0"/>
       <c r="AMI49" s="0"/>
       <c r="AMJ49" s="0"/>
+      <c r="AMK49" s="0"/>
+      <c r="AML49" s="0"/>
+      <c r="AMM49" s="0"/>
+      <c r="AMN49" s="0"/>
     </row>
-    <row r="50" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="n">
         <v>45064</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E50" s="11" t="s">
         <v>9</v>
@@ -10130,19 +10321,23 @@
       <c r="AMH50" s="0"/>
       <c r="AMI50" s="0"/>
       <c r="AMJ50" s="0"/>
+      <c r="AMK50" s="0"/>
+      <c r="AML50" s="0"/>
+      <c r="AMM50" s="0"/>
+      <c r="AMN50" s="0"/>
     </row>
-    <row r="51" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="n">
         <v>45049</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>9</v>
@@ -10154,19 +10349,23 @@
       <c r="AMH51" s="0"/>
       <c r="AMI51" s="0"/>
       <c r="AMJ51" s="0"/>
+      <c r="AMK51" s="0"/>
+      <c r="AML51" s="0"/>
+      <c r="AMM51" s="0"/>
+      <c r="AMN51" s="0"/>
     </row>
-    <row r="52" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="n">
         <v>45049</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E52" s="11" t="s">
         <v>33</v>
@@ -10178,19 +10377,23 @@
       <c r="AMH52" s="0"/>
       <c r="AMI52" s="0"/>
       <c r="AMJ52" s="0"/>
+      <c r="AMK52" s="0"/>
+      <c r="AML52" s="0"/>
+      <c r="AMM52" s="0"/>
+      <c r="AMN52" s="0"/>
     </row>
-    <row r="53" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="n">
         <v>45044</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C53" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E53" s="11" t="s">
         <v>9</v>
@@ -10202,19 +10405,23 @@
       <c r="AMH53" s="0"/>
       <c r="AMI53" s="0"/>
       <c r="AMJ53" s="0"/>
+      <c r="AMK53" s="0"/>
+      <c r="AML53" s="0"/>
+      <c r="AMM53" s="0"/>
+      <c r="AMN53" s="0"/>
     </row>
-    <row r="54" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" s="11" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="n">
         <v>45041</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C54" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E54" s="11" t="s">
         <v>33</v>
@@ -10226,19 +10433,23 @@
       <c r="AMH54" s="0"/>
       <c r="AMI54" s="0"/>
       <c r="AMJ54" s="0"/>
+      <c r="AMK54" s="0"/>
+      <c r="AML54" s="0"/>
+      <c r="AMM54" s="0"/>
+      <c r="AMN54" s="0"/>
     </row>
-    <row r="55" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="n">
         <v>45040</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C55" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E55" s="11" t="s">
         <v>9</v>
@@ -10250,19 +10461,23 @@
       <c r="AMH55" s="0"/>
       <c r="AMI55" s="0"/>
       <c r="AMJ55" s="0"/>
+      <c r="AMK55" s="0"/>
+      <c r="AML55" s="0"/>
+      <c r="AMM55" s="0"/>
+      <c r="AMN55" s="0"/>
     </row>
-    <row r="56" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="n">
         <v>45028</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C56" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E56" s="11" t="s">
         <v>33</v>
@@ -10274,8 +10489,12 @@
       <c r="AMH56" s="0"/>
       <c r="AMI56" s="0"/>
       <c r="AMJ56" s="0"/>
+      <c r="AMK56" s="0"/>
+      <c r="AML56" s="0"/>
+      <c r="AMM56" s="0"/>
+      <c r="AMN56" s="0"/>
     </row>
-    <row r="57" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="9" t="n">
         <v>44996</v>
       </c>
@@ -10284,7 +10503,7 @@
         <v>31</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F57" s="12" t="s">
         <v>43</v>
@@ -10293,19 +10512,23 @@
       <c r="AMH57" s="0"/>
       <c r="AMI57" s="0"/>
       <c r="AMJ57" s="0"/>
+      <c r="AMK57" s="0"/>
+      <c r="AML57" s="0"/>
+      <c r="AMM57" s="0"/>
+      <c r="AMN57" s="0"/>
     </row>
-    <row r="58" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="9" t="n">
         <v>45007</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C58" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E58" s="11" t="s">
         <v>9</v>
@@ -10317,91 +10540,107 @@
       <c r="AMH58" s="0"/>
       <c r="AMI58" s="0"/>
       <c r="AMJ58" s="0"/>
+      <c r="AMK58" s="0"/>
+      <c r="AML58" s="0"/>
+      <c r="AMM58" s="0"/>
+      <c r="AMN58" s="0"/>
     </row>
-    <row r="59" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="9" t="n">
         <v>44993</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C59" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E59" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F59" s="22" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AMG59" s="0"/>
       <c r="AMH59" s="0"/>
       <c r="AMI59" s="0"/>
       <c r="AMJ59" s="0"/>
+      <c r="AMK59" s="0"/>
+      <c r="AML59" s="0"/>
+      <c r="AMM59" s="0"/>
+      <c r="AMN59" s="0"/>
     </row>
-    <row r="60" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="9" t="n">
         <v>44993</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C60" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E60" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F60" s="22" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AMG60" s="0"/>
       <c r="AMH60" s="0"/>
       <c r="AMI60" s="0"/>
       <c r="AMJ60" s="0"/>
+      <c r="AMK60" s="0"/>
+      <c r="AML60" s="0"/>
+      <c r="AMM60" s="0"/>
+      <c r="AMN60" s="0"/>
     </row>
-    <row r="61" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="n">
         <v>44991</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C61" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E61" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F61" s="11" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AMG61" s="0"/>
       <c r="AMH61" s="0"/>
       <c r="AMI61" s="0"/>
       <c r="AMJ61" s="0"/>
+      <c r="AMK61" s="0"/>
+      <c r="AML61" s="0"/>
+      <c r="AMM61" s="0"/>
+      <c r="AMN61" s="0"/>
     </row>
-    <row r="62" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="n">
         <v>44981</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C62" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>33</v>
@@ -10413,19 +10652,23 @@
       <c r="AMH62" s="0"/>
       <c r="AMI62" s="0"/>
       <c r="AMJ62" s="0"/>
+      <c r="AMK62" s="0"/>
+      <c r="AML62" s="0"/>
+      <c r="AMM62" s="0"/>
+      <c r="AMN62" s="0"/>
     </row>
-    <row r="63" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="n">
         <v>44973</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C63" s="11" t="s">
         <v>31</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E63" s="11" t="s">
         <v>9</v>
@@ -10437,43 +10680,51 @@
       <c r="AMH63" s="0"/>
       <c r="AMI63" s="0"/>
       <c r="AMJ63" s="0"/>
+      <c r="AMK63" s="0"/>
+      <c r="AML63" s="0"/>
+      <c r="AMM63" s="0"/>
+      <c r="AMN63" s="0"/>
     </row>
-    <row r="64" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="18" t="n">
         <v>44972</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C64" s="20" t="s">
         <v>7</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E64" s="20" t="s">
         <v>9</v>
       </c>
       <c r="F64" s="20" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AMG64" s="0"/>
       <c r="AMH64" s="0"/>
       <c r="AMI64" s="0"/>
       <c r="AMJ64" s="0"/>
+      <c r="AMK64" s="0"/>
+      <c r="AML64" s="0"/>
+      <c r="AMM64" s="0"/>
+      <c r="AMN64" s="0"/>
     </row>
-    <row r="65" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="28" t="n">
         <v>44970</v>
       </c>
       <c r="B65" s="29" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C65" s="25" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D65" s="25" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E65" s="25" t="s">
         <v>33</v>
@@ -10485,19 +10736,23 @@
       <c r="AMH65" s="0"/>
       <c r="AMI65" s="0"/>
       <c r="AMJ65" s="0"/>
+      <c r="AMK65" s="0"/>
+      <c r="AML65" s="0"/>
+      <c r="AMM65" s="0"/>
+      <c r="AMN65" s="0"/>
     </row>
-    <row r="66" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="28" t="n">
         <v>44967</v>
       </c>
       <c r="B66" s="29" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C66" s="25" t="s">
         <v>7</v>
       </c>
       <c r="D66" s="25" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E66" s="25" t="s">
         <v>33</v>
@@ -10509,91 +10764,107 @@
       <c r="AMH66" s="0"/>
       <c r="AMI66" s="0"/>
       <c r="AMJ66" s="0"/>
+      <c r="AMK66" s="0"/>
+      <c r="AML66" s="0"/>
+      <c r="AMM66" s="0"/>
+      <c r="AMN66" s="0"/>
     </row>
-    <row r="67" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="28" t="n">
         <v>44964</v>
       </c>
       <c r="B67" s="29" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C67" s="25" t="s">
         <v>7</v>
       </c>
       <c r="D67" s="25" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E67" s="25" t="s">
         <v>33</v>
       </c>
       <c r="F67" s="22" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AMG67" s="0"/>
       <c r="AMH67" s="0"/>
       <c r="AMI67" s="0"/>
       <c r="AMJ67" s="0"/>
+      <c r="AMK67" s="0"/>
+      <c r="AML67" s="0"/>
+      <c r="AMM67" s="0"/>
+      <c r="AMN67" s="0"/>
     </row>
-    <row r="68" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="28" t="n">
         <v>44952</v>
       </c>
       <c r="B68" s="29" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C68" s="25" t="s">
         <v>7</v>
       </c>
       <c r="D68" s="25" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E68" s="25" t="s">
         <v>33</v>
       </c>
       <c r="F68" s="22" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AMG68" s="0"/>
       <c r="AMH68" s="0"/>
       <c r="AMI68" s="0"/>
       <c r="AMJ68" s="0"/>
+      <c r="AMK68" s="0"/>
+      <c r="AML68" s="0"/>
+      <c r="AMM68" s="0"/>
+      <c r="AMN68" s="0"/>
     </row>
-    <row r="69" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" s="11" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="28" t="n">
         <v>44952</v>
       </c>
       <c r="B69" s="29" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C69" s="25" t="s">
         <v>7</v>
       </c>
       <c r="D69" s="25" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E69" s="25" t="s">
         <v>33</v>
       </c>
       <c r="F69" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AMG69" s="0"/>
       <c r="AMH69" s="0"/>
       <c r="AMI69" s="0"/>
       <c r="AMJ69" s="0"/>
+      <c r="AMK69" s="0"/>
+      <c r="AML69" s="0"/>
+      <c r="AMM69" s="0"/>
+      <c r="AMN69" s="0"/>
     </row>
-    <row r="70" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" s="11" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="30" t="n">
         <v>44949</v>
       </c>
       <c r="B70" s="31" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C70" s="25" t="s">
         <v>13</v>
       </c>
       <c r="D70" s="25" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E70" s="25" t="s">
         <v>9</v>
@@ -10605,19 +10876,23 @@
       <c r="AMH70" s="0"/>
       <c r="AMI70" s="0"/>
       <c r="AMJ70" s="0"/>
+      <c r="AMK70" s="0"/>
+      <c r="AML70" s="0"/>
+      <c r="AMM70" s="0"/>
+      <c r="AMN70" s="0"/>
     </row>
-    <row r="71" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" s="11" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="28" t="n">
         <v>44948</v>
       </c>
       <c r="B71" s="29" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C71" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D71" s="25" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E71" s="25" t="s">
         <v>33</v>
@@ -10629,22 +10904,26 @@
       <c r="AMH71" s="0"/>
       <c r="AMI71" s="0"/>
       <c r="AMJ71" s="0"/>
+      <c r="AMK71" s="0"/>
+      <c r="AML71" s="0"/>
+      <c r="AMM71" s="0"/>
+      <c r="AMN71" s="0"/>
     </row>
-    <row r="72" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" s="11" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="28" t="n">
         <v>44946</v>
       </c>
       <c r="B72" s="29" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C72" s="25" t="s">
         <v>7</v>
       </c>
       <c r="D72" s="25" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E72" s="25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F72" s="12" t="s">
         <v>43</v>
@@ -10653,22 +10932,26 @@
       <c r="AMH72" s="0"/>
       <c r="AMI72" s="0"/>
       <c r="AMJ72" s="0"/>
+      <c r="AMK72" s="0"/>
+      <c r="AML72" s="0"/>
+      <c r="AMM72" s="0"/>
+      <c r="AMN72" s="0"/>
     </row>
-    <row r="73" s="11" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" s="11" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="28" t="n">
         <v>44929</v>
       </c>
       <c r="B73" s="32" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C73" s="25" t="s">
         <v>7</v>
       </c>
       <c r="D73" s="25" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E73" s="25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F73" s="15" t="s">
         <v>47</v>
@@ -11691,10 +11974,14 @@
       <c r="AMH73" s="0"/>
       <c r="AMI73" s="0"/>
       <c r="AMJ73" s="0"/>
+      <c r="AMK73" s="0"/>
+      <c r="AML73" s="0"/>
+      <c r="AMM73" s="0"/>
+      <c r="AMN73" s="0"/>
     </row>
-    <row r="74" s="25" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" s="25" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
@@ -12721,22 +13008,26 @@
       <c r="AMH74" s="0"/>
       <c r="AMI74" s="0"/>
       <c r="AMJ74" s="0"/>
+      <c r="AMK74" s="0"/>
+      <c r="AML74" s="0"/>
+      <c r="AMM74" s="0"/>
+      <c r="AMN74" s="0"/>
     </row>
-    <row r="75" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" s="8" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="28" t="n">
         <v>44879</v>
       </c>
       <c r="B75" s="33" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>34</v>
@@ -12745,19 +13036,23 @@
       <c r="AMH75" s="0"/>
       <c r="AMI75" s="0"/>
       <c r="AMJ75" s="0"/>
+      <c r="AMK75" s="0"/>
+      <c r="AML75" s="0"/>
+      <c r="AMM75" s="0"/>
+      <c r="AMN75" s="0"/>
     </row>
-    <row r="76" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" s="8" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="28" t="n">
         <v>44858</v>
       </c>
       <c r="B76" s="29" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C76" s="25" t="s">
         <v>7</v>
       </c>
       <c r="D76" s="25" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E76" s="25" t="s">
         <v>33</v>
@@ -13783,25 +14078,29 @@
       <c r="AMH76" s="0"/>
       <c r="AMI76" s="0"/>
       <c r="AMJ76" s="0"/>
+      <c r="AMK76" s="0"/>
+      <c r="AML76" s="0"/>
+      <c r="AMM76" s="0"/>
+      <c r="AMN76" s="0"/>
     </row>
-    <row r="77" s="25" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" s="25" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="28" t="n">
         <v>44855</v>
       </c>
       <c r="B77" s="33" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F77" s="22" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G77" s="8"/>
       <c r="H77" s="8"/>
@@ -14821,46 +15120,54 @@
       <c r="AMH77" s="0"/>
       <c r="AMI77" s="0"/>
       <c r="AMJ77" s="0"/>
+      <c r="AMK77" s="0"/>
+      <c r="AML77" s="0"/>
+      <c r="AMM77" s="0"/>
+      <c r="AMN77" s="0"/>
     </row>
-    <row r="78" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" s="8" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="28" t="n">
         <v>44844</v>
       </c>
       <c r="B78" s="33" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AMG78" s="0"/>
       <c r="AMH78" s="0"/>
       <c r="AMI78" s="0"/>
       <c r="AMJ78" s="0"/>
+      <c r="AMK78" s="0"/>
+      <c r="AML78" s="0"/>
+      <c r="AMM78" s="0"/>
+      <c r="AMN78" s="0"/>
     </row>
-    <row r="79" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" s="8" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="28" t="n">
         <v>44757</v>
       </c>
       <c r="B79" s="34" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F79" s="12" t="s">
         <v>43</v>
@@ -15883,19 +16190,23 @@
       <c r="AMH79" s="0"/>
       <c r="AMI79" s="0"/>
       <c r="AMJ79" s="0"/>
+      <c r="AMK79" s="0"/>
+      <c r="AML79" s="0"/>
+      <c r="AMM79" s="0"/>
+      <c r="AMN79" s="0"/>
     </row>
-    <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="28" t="n">
         <v>373466</v>
       </c>
       <c r="B80" s="33" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E80" s="5" t="s">
         <v>23</v>
@@ -15904,7 +16215,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="28" t="n">
         <v>44743</v>
       </c>
@@ -15912,44 +16223,44 @@
         <v>7</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F81" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="28" t="n">
         <v>44740</v>
       </c>
       <c r="B82" s="35" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F82" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="28" t="n">
         <v>44739</v>
       </c>
       <c r="B83" s="36" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>23</v>
@@ -15958,18 +16269,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="28" t="n">
         <v>44693</v>
       </c>
       <c r="B84" s="36" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E84" s="5" t="s">
         <v>33</v>
@@ -15978,118 +16289,118 @@
         <v>47</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="28" t="n">
         <v>44695</v>
       </c>
       <c r="B85" s="37" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F85" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="30" t="n">
         <v>44659</v>
       </c>
       <c r="B86" s="38" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F86" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="28" t="n">
         <v>44712</v>
       </c>
       <c r="B87" s="36" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E87" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="28" t="n">
         <v>44705</v>
       </c>
       <c r="B88" s="33" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F88" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="28" t="n">
         <v>44705</v>
       </c>
       <c r="B89" s="33" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F89" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="28" t="n">
         <v>44693</v>
       </c>
       <c r="B90" s="33" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E90" s="5" t="s">
         <v>33</v>
@@ -16098,78 +16409,78 @@
         <v>34</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="28" t="n">
         <v>44622</v>
       </c>
       <c r="B91" s="33" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F91" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="28" t="n">
         <v>44614</v>
       </c>
       <c r="B92" s="33" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C92" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F92" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="28" t="n">
         <v>44613</v>
       </c>
       <c r="B93" s="33" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C93" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F93" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="28" t="n">
         <v>44608</v>
       </c>
       <c r="B94" s="36" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E94" s="5" t="s">
         <v>23</v>
@@ -16178,83 +16489,83 @@
         <v>43</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="28" t="n">
         <v>44580</v>
       </c>
       <c r="B95" s="33" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E95" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="28" t="n">
         <v>44463</v>
       </c>
       <c r="B97" s="33" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F97" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="28" t="n">
         <v>44460</v>
       </c>
       <c r="B98" s="33" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E98" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="28" t="n">
         <v>44460</v>
       </c>
       <c r="B99" s="33" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>23</v>
@@ -16263,18 +16574,18 @@
         <v>43</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="28" t="n">
         <v>44372</v>
       </c>
       <c r="B100" s="33" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E100" s="5" t="s">
         <v>23</v>
@@ -16283,58 +16594,58 @@
         <v>34</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="28" t="n">
         <v>44326</v>
       </c>
       <c r="B101" s="33" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="30" t="n">
         <v>44325</v>
       </c>
       <c r="B102" s="39" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F102" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="28" t="n">
         <v>44325</v>
       </c>
       <c r="B103" s="33" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E103" s="5" t="s">
         <v>23</v>
@@ -16343,58 +16654,58 @@
         <v>34</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="28" t="n">
         <v>44321</v>
       </c>
       <c r="B104" s="33" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E104" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F104" s="22" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="28" t="n">
         <v>44316</v>
       </c>
       <c r="B105" s="33" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="28" t="n">
         <v>44279</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E106" s="5" t="s">
         <v>23</v>
@@ -16403,98 +16714,98 @@
         <v>47</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="28" t="n">
         <v>44257</v>
       </c>
       <c r="B107" s="33" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C107" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F107" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="28" t="n">
         <v>44243</v>
       </c>
       <c r="B108" s="33" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C108" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F108" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="40" t="n">
         <v>44231</v>
       </c>
       <c r="B109" s="41" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C109" s="42" t="s">
         <v>7</v>
       </c>
       <c r="D109" s="42" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E109" s="42" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F109" s="42" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="28" t="n">
         <v>44218</v>
       </c>
       <c r="B110" s="33" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C110" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F110" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="28" t="n">
         <v>44216</v>
       </c>
       <c r="B111" s="36" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C111" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E111" s="5" t="s">
         <v>23</v>
@@ -16503,38 +16814,38 @@
         <v>47</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="28" t="n">
         <v>44175</v>
       </c>
       <c r="B112" s="33" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C112" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F112" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="28" t="n">
         <v>44175</v>
       </c>
       <c r="B113" s="33" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C113" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E113" s="5" t="s">
         <v>23</v>
@@ -16543,23 +16854,23 @@
         <v>34</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="28" t="n">
         <v>44162</v>
       </c>
       <c r="B115" s="33" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C115" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E115" s="5" t="s">
         <v>33</v>
@@ -16568,12 +16879,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="28" t="n">
         <v>44148</v>
       </c>
       <c r="B116" s="33" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C116" s="5" t="s">
         <v>7</v>
@@ -16582,104 +16893,104 @@
         <v>8</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F116" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="40" t="n">
         <v>44146</v>
       </c>
       <c r="B117" s="41" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C117" s="42" t="s">
         <v>13</v>
       </c>
       <c r="D117" s="42" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E117" s="42" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F117" s="42" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="28" t="n">
         <v>44132</v>
       </c>
       <c r="B118" s="33" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C118" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F118" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="28" t="n">
         <v>44103</v>
       </c>
       <c r="B119" s="33" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C119" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F119" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="40" t="n">
         <v>44095</v>
       </c>
       <c r="B120" s="41" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C120" s="42" t="s">
         <v>7</v>
       </c>
       <c r="D120" s="42" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E120" s="42" t="s">
         <v>33</v>
       </c>
       <c r="F120" s="42" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="28" t="n">
         <v>44095</v>
       </c>
       <c r="B121" s="33" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C121" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E121" s="5" t="s">
         <v>33</v>
@@ -16688,98 +16999,98 @@
         <v>43</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="28" t="n">
         <v>44057</v>
       </c>
       <c r="B122" s="33" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C122" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E122" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F122" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="28" t="n">
         <v>44028</v>
       </c>
       <c r="B123" s="33" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C123" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F123" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="28" t="n">
         <v>44064</v>
       </c>
       <c r="B124" s="33" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C124" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F124" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="28" t="n">
         <v>44028</v>
       </c>
       <c r="B125" s="33" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C125" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F125" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="28" t="n">
         <v>44016</v>
       </c>
       <c r="B126" s="33" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C126" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E126" s="5" t="s">
         <v>33</v>
@@ -16788,18 +17099,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="28" t="n">
         <v>44010</v>
       </c>
       <c r="B127" s="33" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C127" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E127" s="5" t="s">
         <v>23</v>
@@ -16808,18 +17119,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="28" t="n">
         <v>43995</v>
       </c>
       <c r="B128" s="33" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C128" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E128" s="5" t="s">
         <v>33</v>
@@ -16828,58 +17139,58 @@
         <v>34</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="28" t="n">
         <v>43948</v>
       </c>
       <c r="B129" s="33" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C129" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F129" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="28" t="n">
         <v>43947</v>
       </c>
       <c r="B130" s="33" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C130" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F130" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="28" t="n">
         <v>43936</v>
       </c>
       <c r="B131" s="33" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C131" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E131" s="5" t="s">
         <v>33</v>
@@ -16888,138 +17199,138 @@
         <v>34</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="28" t="n">
         <v>43929</v>
       </c>
       <c r="B132" s="33" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C132" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F132" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="28" t="n">
         <v>43891</v>
       </c>
       <c r="B133" s="33" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C133" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E133" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F133" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="28" t="n">
         <v>43885</v>
       </c>
       <c r="B134" s="33" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C134" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E134" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F134" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="28" t="n">
         <v>43857</v>
       </c>
       <c r="B135" s="33" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C135" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E135" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F135" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="28" t="n">
         <v>43857</v>
       </c>
       <c r="B136" s="33" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C136" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F136" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="28" t="n">
         <v>43852</v>
       </c>
       <c r="B137" s="33" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C137" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F137" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="28" t="n">
         <v>43584</v>
       </c>
       <c r="B138" s="33" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C138" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E138" s="5" t="s">
         <v>23</v>
@@ -17028,18 +17339,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="28" t="n">
         <v>43584</v>
       </c>
       <c r="B139" s="33" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C139" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E139" s="5" t="s">
         <v>23</v>
@@ -17048,18 +17359,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="28" t="n">
         <v>43540</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C140" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E140" s="5" t="s">
         <v>23</v>
@@ -17068,63 +17379,63 @@
         <v>34</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="28" t="n">
         <v>43203</v>
       </c>
       <c r="B142" s="43" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C142" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E142" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F142" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="28" t="n">
         <v>43203</v>
       </c>
       <c r="B143" s="43" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C143" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E143" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F143" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="28" t="n">
         <v>42842</v>
       </c>
       <c r="B144" s="43" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C144" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E144" s="5" t="s">
         <v>33</v>
@@ -17133,18 +17444,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="28" t="n">
         <v>42457</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C145" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E145" s="5" t="s">
         <v>23</v>
@@ -17153,18 +17464,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="28" t="n">
         <v>39028</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C146" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E146" s="5" t="s">
         <v>33</v>
@@ -19220,9 +19531,19 @@
       <c r="AMH149" s="0"/>
       <c r="AMI149" s="0"/>
       <c r="AMJ149" s="0"/>
+      <c r="AMK149" s="0"/>
+      <c r="AML149" s="0"/>
+      <c r="AMM149" s="0"/>
+      <c r="AMN149" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F146"/>
+  <autoFilter ref="A1:F146">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Protected entries in XLIFF show translation as source text"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="F97:F1048576 F1:F95">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="resolved" dxfId="13">
       <formula>NOT(ISERROR(SEARCH("resolved",F1)))</formula>
@@ -19407,10 +19728,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -19419,10 +19740,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>